<commit_message>
Complete Ch 05 Understanding CALCULATE and CALCULATETABLE
</commit_message>
<xml_diff>
--- a/Definitive Guide to DAX/DAX Functions Covered.xlsx
+++ b/Definitive Guide to DAX/DAX Functions Covered.xlsx
@@ -8,27 +8,35 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github.com\open-word\DAX\Definitive Guide to DAX\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF221FCD-B915-4E83-8C35-DEFF085579B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F3608B2-30F1-44A9-AE4E-12E22CC363B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="1680" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-26670" yWindow="3225" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
-  <si>
-    <t>Ch 05</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="27">
   <si>
     <t>CALCULATE</t>
   </si>
@@ -39,38 +47,95 @@
     <t>KEEPFILTERS</t>
   </si>
   <si>
-    <t>Calculate modifier</t>
-  </si>
-  <si>
     <t>Using basic table functions</t>
   </si>
   <si>
     <t>Understanding evaluation contexts</t>
   </si>
   <si>
-    <t>Ch 03</t>
-  </si>
-  <si>
-    <t>Ch 04</t>
-  </si>
-  <si>
     <t>Understanding CALCULATE and CALCULATETABLE</t>
   </si>
   <si>
-    <t>Ch 01</t>
-  </si>
-  <si>
-    <t>Ch 02</t>
+    <t>USERELATIONSHIP</t>
+  </si>
+  <si>
+    <t>Function</t>
+  </si>
+  <si>
+    <t>Chapter</t>
+  </si>
+  <si>
+    <t>Section</t>
+  </si>
+  <si>
+    <t>Subsection</t>
+  </si>
+  <si>
+    <t>Key</t>
+  </si>
+  <si>
+    <t>Understanding USERELATIONSHIP</t>
+  </si>
+  <si>
+    <t>Understanding CROSSFILTER</t>
+  </si>
+  <si>
+    <t>CROSSFILTER</t>
+  </si>
+  <si>
+    <t>Understanding KEEPFILTERS</t>
+  </si>
+  <si>
+    <t>Understanding ALL in CALCULATE</t>
+  </si>
+  <si>
+    <t>Filter argument modifier</t>
+  </si>
+  <si>
+    <t>REMOVEFILTER when used as a top-level ALL call, F 05 39</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Note</t>
+  </si>
+  <si>
+    <t>ALLSELECTED</t>
+  </si>
+  <si>
+    <t>Introducing ALL and ALLSELECTED</t>
+  </si>
+  <si>
+    <t>CALCULATE modifiers</t>
+  </si>
+  <si>
+    <t>CALCULATE rules</t>
+  </si>
+  <si>
+    <t>CALCULATE modifier, table function</t>
+  </si>
+  <si>
+    <t>CALCULATE modifier</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="00"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -96,8 +161,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -378,72 +444,295 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="E2:N8"/>
+  <dimension ref="B1:K14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="44.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="44.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="33.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="31.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="51.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="5:14" x14ac:dyDescent="0.25">
-      <c r="E2" t="s">
+    <row r="1" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="5:14" x14ac:dyDescent="0.25">
-      <c r="E3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="5:14" x14ac:dyDescent="0.25">
-      <c r="E4" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="F4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="5:14" x14ac:dyDescent="0.25">
-      <c r="E5" t="s">
-        <v>8</v>
-      </c>
-      <c r="F5" t="s">
+      <c r="J1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C3" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C4" s="1">
+        <v>3</v>
+      </c>
+      <c r="D4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C5" s="1">
+        <v>4</v>
+      </c>
+      <c r="D5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C6" s="1">
+        <v>5</v>
+      </c>
+      <c r="D6" t="s">
+        <v>5</v>
+      </c>
+      <c r="I6" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C7" s="1">
+        <v>5</v>
+      </c>
+      <c r="D7" t="s">
+        <v>5</v>
+      </c>
+      <c r="I7" t="s">
+        <v>1</v>
+      </c>
+      <c r="J7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C8" s="1">
+        <v>5</v>
+      </c>
+      <c r="D8" t="s">
+        <v>5</v>
+      </c>
+      <c r="I8" t="s">
+        <v>2</v>
+      </c>
+      <c r="J8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B9" t="str">
+        <f>_xlfn.CONCAT(TEXT(C9,"00"),TEXT(E9,"00"),TEXT(G9,"00"))</f>
+        <v>050401</v>
+      </c>
+      <c r="C9" s="1">
+        <v>5</v>
+      </c>
+      <c r="D9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" s="1">
+        <v>4</v>
+      </c>
+      <c r="F9" t="s">
+        <v>23</v>
+      </c>
+      <c r="G9" s="1">
+        <v>1</v>
+      </c>
+      <c r="H9" t="s">
+        <v>12</v>
+      </c>
+      <c r="I9" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="5:14" x14ac:dyDescent="0.25">
-      <c r="E6" t="s">
+      <c r="J9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B10" t="str">
+        <f>_xlfn.CONCAT(TEXT(C10,"00"),TEXT(E10,"00"),TEXT(G10,"00"))</f>
+        <v>050402</v>
+      </c>
+      <c r="C10" s="1">
+        <v>5</v>
+      </c>
+      <c r="D10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" s="1">
+        <v>4</v>
+      </c>
+      <c r="F10" t="s">
+        <v>23</v>
+      </c>
+      <c r="G10" s="1">
+        <v>2</v>
+      </c>
+      <c r="H10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I10" t="s">
+        <v>14</v>
+      </c>
+      <c r="J10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B11" t="str">
+        <f t="shared" ref="B11:B12" si="0">_xlfn.CONCAT(TEXT(C11,"00"),TEXT(E11,"00"),TEXT(G11,"00"))</f>
+        <v>050403</v>
+      </c>
+      <c r="C11" s="1">
+        <v>5</v>
+      </c>
+      <c r="D11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11" s="1">
+        <v>4</v>
+      </c>
+      <c r="F11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G11" s="1">
+        <v>3</v>
+      </c>
+      <c r="H11" t="s">
+        <v>15</v>
+      </c>
+      <c r="I11" t="s">
+        <v>2</v>
+      </c>
+      <c r="J11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B12" t="str">
+        <f t="shared" si="0"/>
+        <v>050404</v>
+      </c>
+      <c r="C12" s="1">
+        <v>5</v>
+      </c>
+      <c r="D12" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12" s="1">
+        <v>4</v>
+      </c>
+      <c r="F12" t="s">
+        <v>23</v>
+      </c>
+      <c r="G12" s="1">
+        <v>4</v>
+      </c>
+      <c r="H12" t="s">
+        <v>16</v>
+      </c>
+      <c r="I12" t="s">
+        <v>1</v>
+      </c>
+      <c r="J12" t="s">
+        <v>25</v>
+      </c>
+      <c r="K12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B13" t="str">
+        <f t="shared" ref="B13:B14" si="1">_xlfn.CONCAT(TEXT(C13,"00"),TEXT(E13,"00"),TEXT(G13,"00"))</f>
+        <v>050405</v>
+      </c>
+      <c r="C13" s="1">
+        <v>5</v>
+      </c>
+      <c r="D13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E13" s="1">
+        <v>4</v>
+      </c>
+      <c r="F13" t="s">
+        <v>23</v>
+      </c>
+      <c r="G13" s="1">
+        <v>5</v>
+      </c>
+      <c r="H13" t="s">
+        <v>22</v>
+      </c>
+      <c r="I13" t="s">
+        <v>21</v>
+      </c>
+      <c r="J13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B14" t="str">
+        <f t="shared" si="1"/>
+        <v>050501</v>
+      </c>
+      <c r="C14" s="1">
+        <v>5</v>
+      </c>
+      <c r="D14" t="s">
+        <v>5</v>
+      </c>
+      <c r="E14" s="1">
+        <v>5</v>
+      </c>
+      <c r="F14" t="s">
+        <v>24</v>
+      </c>
+      <c r="G14" s="1">
+        <v>1</v>
+      </c>
+      <c r="H14" t="s">
+        <v>24</v>
+      </c>
+      <c r="I14" t="s">
         <v>0</v>
       </c>
-      <c r="F6" t="s">
-        <v>9</v>
-      </c>
-      <c r="L6" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="5:14" x14ac:dyDescent="0.25">
-      <c r="L7" t="s">
-        <v>2</v>
-      </c>
-      <c r="N7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="5:14" x14ac:dyDescent="0.25">
-      <c r="L8" t="s">
-        <v>3</v>
-      </c>
-      <c r="N8" t="s">
-        <v>4</v>
-      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update DAX Functions Covered.xlsx
</commit_message>
<xml_diff>
--- a/Definitive Guide to DAX/DAX Functions Covered.xlsx
+++ b/Definitive Guide to DAX/DAX Functions Covered.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github.com\open-word\DAX\Definitive Guide to DAX\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F3608B2-30F1-44A9-AE4E-12E22CC363B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA6C29F6-D4F2-4EF7-95FB-68A53FDC561F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26670" yWindow="3225" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="18240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -149,7 +149,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -157,13 +157,105 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -447,7 +539,7 @@
   <dimension ref="B1:K14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -513,223 +605,248 @@
       </c>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C6" s="1">
-        <v>5</v>
-      </c>
-      <c r="D6" t="s">
-        <v>5</v>
-      </c>
-      <c r="I6" t="s">
+      <c r="B6" s="2"/>
+      <c r="C6" s="3">
+        <v>5</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4" t="s">
         <v>0</v>
       </c>
+      <c r="J6" s="4"/>
+      <c r="K6" s="5"/>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C7" s="1">
-        <v>5</v>
-      </c>
-      <c r="D7" t="s">
-        <v>5</v>
-      </c>
-      <c r="I7" t="s">
+      <c r="B7" s="6"/>
+      <c r="C7" s="7">
+        <v>5</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="J7" t="s">
+      <c r="J7" s="8" t="s">
         <v>25</v>
       </c>
+      <c r="K7" s="9"/>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C8" s="1">
-        <v>5</v>
-      </c>
-      <c r="D8" t="s">
-        <v>5</v>
-      </c>
-      <c r="I8" t="s">
+      <c r="B8" s="6"/>
+      <c r="C8" s="7">
+        <v>5</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="J8" t="s">
+      <c r="J8" s="8" t="s">
         <v>26</v>
       </c>
+      <c r="K8" s="9"/>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B9" t="str">
+      <c r="B9" s="6" t="str">
         <f>_xlfn.CONCAT(TEXT(C9,"00"),TEXT(E9,"00"),TEXT(G9,"00"))</f>
         <v>050401</v>
       </c>
-      <c r="C9" s="1">
-        <v>5</v>
-      </c>
-      <c r="D9" t="s">
-        <v>5</v>
-      </c>
-      <c r="E9" s="1">
+      <c r="C9" s="7">
+        <v>5</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" s="7">
         <v>4</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="G9" s="1">
+      <c r="G9" s="7">
         <v>1</v>
       </c>
-      <c r="H9" t="s">
+      <c r="H9" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="I9" t="s">
+      <c r="I9" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="J9" t="s">
+      <c r="J9" s="8" t="s">
         <v>26</v>
       </c>
+      <c r="K9" s="9"/>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B10" t="str">
+      <c r="B10" s="6" t="str">
         <f>_xlfn.CONCAT(TEXT(C10,"00"),TEXT(E10,"00"),TEXT(G10,"00"))</f>
         <v>050402</v>
       </c>
-      <c r="C10" s="1">
-        <v>5</v>
-      </c>
-      <c r="D10" t="s">
-        <v>5</v>
-      </c>
-      <c r="E10" s="1">
+      <c r="C10" s="7">
+        <v>5</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" s="7">
         <v>4</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="G10" s="1">
+      <c r="G10" s="7">
         <v>2</v>
       </c>
-      <c r="H10" t="s">
+      <c r="H10" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="I10" t="s">
+      <c r="I10" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="J10" t="s">
+      <c r="J10" s="8" t="s">
         <v>26</v>
       </c>
+      <c r="K10" s="9"/>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B11" t="str">
+      <c r="B11" s="6" t="str">
         <f t="shared" ref="B11:B12" si="0">_xlfn.CONCAT(TEXT(C11,"00"),TEXT(E11,"00"),TEXT(G11,"00"))</f>
         <v>050403</v>
       </c>
-      <c r="C11" s="1">
-        <v>5</v>
-      </c>
-      <c r="D11" t="s">
-        <v>5</v>
-      </c>
-      <c r="E11" s="1">
+      <c r="C11" s="7">
+        <v>5</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11" s="7">
         <v>4</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="G11" s="1">
+      <c r="G11" s="7">
         <v>3</v>
       </c>
-      <c r="H11" t="s">
+      <c r="H11" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="I11" t="s">
+      <c r="I11" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="J11" t="s">
+      <c r="J11" s="8" t="s">
         <v>17</v>
       </c>
+      <c r="K11" s="9"/>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B12" t="str">
+      <c r="B12" s="6" t="str">
         <f t="shared" si="0"/>
         <v>050404</v>
       </c>
-      <c r="C12" s="1">
-        <v>5</v>
-      </c>
-      <c r="D12" t="s">
-        <v>5</v>
-      </c>
-      <c r="E12" s="1">
+      <c r="C12" s="7">
+        <v>5</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12" s="7">
         <v>4</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F12" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="G12" s="1">
+      <c r="G12" s="7">
         <v>4</v>
       </c>
-      <c r="H12" t="s">
+      <c r="H12" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="I12" t="s">
+      <c r="I12" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="J12" t="s">
+      <c r="J12" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="K12" t="s">
+      <c r="K12" s="9" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B13" t="str">
+      <c r="B13" s="6" t="str">
         <f t="shared" ref="B13:B14" si="1">_xlfn.CONCAT(TEXT(C13,"00"),TEXT(E13,"00"),TEXT(G13,"00"))</f>
         <v>050405</v>
       </c>
-      <c r="C13" s="1">
-        <v>5</v>
-      </c>
-      <c r="D13" t="s">
-        <v>5</v>
-      </c>
-      <c r="E13" s="1">
+      <c r="C13" s="7">
+        <v>5</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E13" s="7">
         <v>4</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F13" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="G13" s="1">
-        <v>5</v>
-      </c>
-      <c r="H13" t="s">
+      <c r="G13" s="7">
+        <v>5</v>
+      </c>
+      <c r="H13" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="I13" t="s">
+      <c r="I13" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="J13" t="s">
+      <c r="J13" s="8" t="s">
         <v>25</v>
       </c>
+      <c r="K13" s="9"/>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B14" t="str">
+      <c r="B14" s="10" t="str">
         <f t="shared" si="1"/>
         <v>050501</v>
       </c>
-      <c r="C14" s="1">
-        <v>5</v>
-      </c>
-      <c r="D14" t="s">
-        <v>5</v>
-      </c>
-      <c r="E14" s="1">
-        <v>5</v>
-      </c>
-      <c r="F14" t="s">
+      <c r="C14" s="11">
+        <v>5</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="E14" s="11">
+        <v>5</v>
+      </c>
+      <c r="F14" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="G14" s="1">
+      <c r="G14" s="11">
         <v>1</v>
       </c>
-      <c r="H14" t="s">
+      <c r="H14" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="I14" t="s">
+      <c r="I14" s="12" t="s">
         <v>0</v>
       </c>
+      <c r="J14" s="12"/>
+      <c r="K14" s="13"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
Complete Ch 07 Working with iterators and with CALCULATE
</commit_message>
<xml_diff>
--- a/Definitive Guide to DAX/DAX Functions Covered.xlsx
+++ b/Definitive Guide to DAX/DAX Functions Covered.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github.com\open-word\DAX\Definitive Guide to DAX\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA6C29F6-D4F2-4EF7-95FB-68A53FDC561F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25958EE1-4490-4481-8D85-BECECA92569C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="18240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="1680" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="44">
   <si>
     <t>CALCULATE</t>
   </si>
@@ -117,6 +117,57 @@
   </si>
   <si>
     <t>CALCULATE modifier</t>
+  </si>
+  <si>
+    <t>Using iterators</t>
+  </si>
+  <si>
+    <t>Working with iterators and with CALCULATE</t>
+  </si>
+  <si>
+    <t>Understanding iterator cardinality</t>
+  </si>
+  <si>
+    <t>Leveraging context transition in iterators</t>
+  </si>
+  <si>
+    <t>Using CONCATENATEX</t>
+  </si>
+  <si>
+    <t>ADDCOLUMNS, SUMMARIZECOLUMNS</t>
+  </si>
+  <si>
+    <t>CONCATENATEX</t>
+  </si>
+  <si>
+    <t>Solving common scenarios with iterators</t>
+  </si>
+  <si>
+    <t>Computing averages and moving averages</t>
+  </si>
+  <si>
+    <t>Using RANKX</t>
+  </si>
+  <si>
+    <t>AVERAGEX</t>
+  </si>
+  <si>
+    <t>SUMX, RELATED, RELATEDTABLE</t>
+  </si>
+  <si>
+    <t>Iterators returning tables</t>
+  </si>
+  <si>
+    <t>MAXX, AVERAGEX</t>
+  </si>
+  <si>
+    <t>RANKX, HASONEVALUE, ALLSELECTED</t>
+  </si>
+  <si>
+    <t>Changing calculation granularity</t>
+  </si>
+  <si>
+    <t>SUMX, VALUES</t>
   </si>
 </sst>
 </file>
@@ -241,7 +292,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -249,13 +300,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -536,21 +591,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:K14"/>
+  <dimension ref="B1:K21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="44.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="37.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="33.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="37.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="35.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="31.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="51.7109375" bestFit="1" customWidth="1"/>
   </cols>
@@ -624,229 +677,424 @@
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B7" s="6"/>
-      <c r="C7" s="7">
-        <v>5</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
-      <c r="I7" s="8" t="s">
+      <c r="C7" s="1">
+        <v>5</v>
+      </c>
+      <c r="D7" t="s">
+        <v>5</v>
+      </c>
+      <c r="I7" t="s">
         <v>1</v>
       </c>
-      <c r="J7" s="8" t="s">
+      <c r="J7" t="s">
         <v>25</v>
       </c>
-      <c r="K7" s="9"/>
+      <c r="K7" s="7"/>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B8" s="6"/>
-      <c r="C8" s="7">
-        <v>5</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="8" t="s">
+      <c r="C8" s="1">
+        <v>5</v>
+      </c>
+      <c r="D8" t="s">
+        <v>5</v>
+      </c>
+      <c r="I8" t="s">
         <v>2</v>
       </c>
-      <c r="J8" s="8" t="s">
+      <c r="J8" t="s">
         <v>26</v>
       </c>
-      <c r="K8" s="9"/>
+      <c r="K8" s="7"/>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B9" s="6" t="str">
         <f>_xlfn.CONCAT(TEXT(C9,"00"),TEXT(E9,"00"),TEXT(G9,"00"))</f>
         <v>050401</v>
       </c>
-      <c r="C9" s="7">
-        <v>5</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="E9" s="7">
+      <c r="C9" s="1">
+        <v>5</v>
+      </c>
+      <c r="D9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" s="1">
         <v>4</v>
       </c>
-      <c r="F9" s="8" t="s">
+      <c r="F9" t="s">
         <v>23</v>
       </c>
-      <c r="G9" s="7">
+      <c r="G9" s="1">
         <v>1</v>
       </c>
-      <c r="H9" s="8" t="s">
+      <c r="H9" t="s">
         <v>12</v>
       </c>
-      <c r="I9" s="8" t="s">
+      <c r="I9" t="s">
         <v>6</v>
       </c>
-      <c r="J9" s="8" t="s">
+      <c r="J9" t="s">
         <v>26</v>
       </c>
-      <c r="K9" s="9"/>
+      <c r="K9" s="7"/>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B10" s="6" t="str">
         <f>_xlfn.CONCAT(TEXT(C10,"00"),TEXT(E10,"00"),TEXT(G10,"00"))</f>
         <v>050402</v>
       </c>
-      <c r="C10" s="7">
-        <v>5</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="E10" s="7">
+      <c r="C10" s="1">
+        <v>5</v>
+      </c>
+      <c r="D10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" s="1">
         <v>4</v>
       </c>
-      <c r="F10" s="8" t="s">
+      <c r="F10" t="s">
         <v>23</v>
       </c>
-      <c r="G10" s="7">
+      <c r="G10" s="1">
         <v>2</v>
       </c>
-      <c r="H10" s="8" t="s">
+      <c r="H10" t="s">
         <v>13</v>
       </c>
-      <c r="I10" s="8" t="s">
+      <c r="I10" t="s">
         <v>14</v>
       </c>
-      <c r="J10" s="8" t="s">
+      <c r="J10" t="s">
         <v>26</v>
       </c>
-      <c r="K10" s="9"/>
+      <c r="K10" s="7"/>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B11" s="6" t="str">
         <f t="shared" ref="B11:B12" si="0">_xlfn.CONCAT(TEXT(C11,"00"),TEXT(E11,"00"),TEXT(G11,"00"))</f>
         <v>050403</v>
       </c>
-      <c r="C11" s="7">
-        <v>5</v>
-      </c>
-      <c r="D11" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="E11" s="7">
+      <c r="C11" s="1">
+        <v>5</v>
+      </c>
+      <c r="D11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11" s="1">
         <v>4</v>
       </c>
-      <c r="F11" s="8" t="s">
+      <c r="F11" t="s">
         <v>23</v>
       </c>
-      <c r="G11" s="7">
+      <c r="G11" s="1">
         <v>3</v>
       </c>
-      <c r="H11" s="8" t="s">
+      <c r="H11" t="s">
         <v>15</v>
       </c>
-      <c r="I11" s="8" t="s">
+      <c r="I11" t="s">
         <v>2</v>
       </c>
-      <c r="J11" s="8" t="s">
+      <c r="J11" t="s">
         <v>17</v>
       </c>
-      <c r="K11" s="9"/>
+      <c r="K11" s="7"/>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B12" s="6" t="str">
         <f t="shared" si="0"/>
         <v>050404</v>
       </c>
-      <c r="C12" s="7">
-        <v>5</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="E12" s="7">
+      <c r="C12" s="1">
+        <v>5</v>
+      </c>
+      <c r="D12" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12" s="1">
         <v>4</v>
       </c>
-      <c r="F12" s="8" t="s">
+      <c r="F12" t="s">
         <v>23</v>
       </c>
-      <c r="G12" s="7">
+      <c r="G12" s="1">
         <v>4</v>
       </c>
-      <c r="H12" s="8" t="s">
+      <c r="H12" t="s">
         <v>16</v>
       </c>
-      <c r="I12" s="8" t="s">
+      <c r="I12" t="s">
         <v>1</v>
       </c>
-      <c r="J12" s="8" t="s">
+      <c r="J12" t="s">
         <v>25</v>
       </c>
-      <c r="K12" s="9" t="s">
+      <c r="K12" s="7" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B13" s="6" t="str">
-        <f t="shared" ref="B13:B14" si="1">_xlfn.CONCAT(TEXT(C13,"00"),TEXT(E13,"00"),TEXT(G13,"00"))</f>
+        <f t="shared" ref="B13:B20" si="1">_xlfn.CONCAT(TEXT(C13,"00"),TEXT(E13,"00"),TEXT(G13,"00"))</f>
         <v>050405</v>
       </c>
-      <c r="C13" s="7">
-        <v>5</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="E13" s="7">
+      <c r="C13" s="1">
+        <v>5</v>
+      </c>
+      <c r="D13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E13" s="1">
         <v>4</v>
       </c>
-      <c r="F13" s="8" t="s">
+      <c r="F13" t="s">
         <v>23</v>
       </c>
-      <c r="G13" s="7">
-        <v>5</v>
-      </c>
-      <c r="H13" s="8" t="s">
+      <c r="G13" s="1">
+        <v>5</v>
+      </c>
+      <c r="H13" t="s">
         <v>22</v>
       </c>
-      <c r="I13" s="8" t="s">
+      <c r="I13" t="s">
         <v>21</v>
       </c>
-      <c r="J13" s="8" t="s">
+      <c r="J13" t="s">
         <v>25</v>
       </c>
-      <c r="K13" s="9"/>
+      <c r="K13" s="7"/>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B14" s="10" t="str">
+      <c r="B14" s="8" t="str">
         <f t="shared" si="1"/>
         <v>050501</v>
       </c>
-      <c r="C14" s="11">
-        <v>5</v>
-      </c>
-      <c r="D14" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="E14" s="11">
-        <v>5</v>
-      </c>
-      <c r="F14" s="12" t="s">
+      <c r="C14" s="9">
+        <v>5</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E14" s="9">
+        <v>5</v>
+      </c>
+      <c r="F14" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="G14" s="11">
+      <c r="G14" s="9">
         <v>1</v>
       </c>
-      <c r="H14" s="12" t="s">
+      <c r="H14" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="I14" s="12" t="s">
+      <c r="I14" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="J14" s="12"/>
-      <c r="K14" s="13"/>
+      <c r="J14" s="10"/>
+      <c r="K14" s="11"/>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B15" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>070101</v>
+      </c>
+      <c r="C15" s="3">
+        <v>7</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E15" s="3">
+        <v>1</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G15" s="3">
+        <v>1</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="I15" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="J15" s="4"/>
+      <c r="K15" s="5"/>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B16" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>070102</v>
+      </c>
+      <c r="C16" s="14">
+        <v>7</v>
+      </c>
+      <c r="D16" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="E16" s="14">
+        <v>1</v>
+      </c>
+      <c r="F16" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="G16" s="14">
+        <v>2</v>
+      </c>
+      <c r="H16" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="I16" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="J16" s="15"/>
+      <c r="K16" s="7"/>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B17" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>070103</v>
+      </c>
+      <c r="C17" s="14">
+        <v>7</v>
+      </c>
+      <c r="D17" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="E17" s="14">
+        <v>1</v>
+      </c>
+      <c r="F17" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="G17" s="14">
+        <v>3</v>
+      </c>
+      <c r="H17" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="I17" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="J17" s="15"/>
+      <c r="K17" s="7"/>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B18" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>070104</v>
+      </c>
+      <c r="C18" s="14">
+        <v>7</v>
+      </c>
+      <c r="D18" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="E18" s="14">
+        <v>1</v>
+      </c>
+      <c r="F18" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="G18" s="14">
+        <v>4</v>
+      </c>
+      <c r="H18" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="I18" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="J18" s="15"/>
+      <c r="K18" s="7"/>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B19" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>070201</v>
+      </c>
+      <c r="C19" s="14">
+        <v>7</v>
+      </c>
+      <c r="D19" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="E19" s="14">
+        <v>2</v>
+      </c>
+      <c r="F19" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="G19" s="14">
+        <v>1</v>
+      </c>
+      <c r="H19" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="I19" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="J19" s="15"/>
+      <c r="K19" s="7"/>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B20" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>070202</v>
+      </c>
+      <c r="C20" s="14">
+        <v>7</v>
+      </c>
+      <c r="D20" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="E20" s="14">
+        <v>2</v>
+      </c>
+      <c r="F20" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="G20" s="14">
+        <v>2</v>
+      </c>
+      <c r="H20" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="I20" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="J20" s="15"/>
+      <c r="K20" s="7"/>
+    </row>
+    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B21" s="8" t="str">
+        <f t="shared" ref="B21" si="2">_xlfn.CONCAT(TEXT(C21,"00"),TEXT(E21,"00"),TEXT(G21,"00"))</f>
+        <v>070203</v>
+      </c>
+      <c r="C21" s="9">
+        <v>7</v>
+      </c>
+      <c r="D21" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="E21" s="9">
+        <v>2</v>
+      </c>
+      <c r="F21" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="G21" s="16">
+        <v>3</v>
+      </c>
+      <c r="H21" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="I21" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="J21" s="10"/>
+      <c r="K21" s="11"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
Complete Ch 08 03, Ch 08 04
</commit_message>
<xml_diff>
--- a/Definitive Guide to DAX/DAX Functions Covered.xlsx
+++ b/Definitive Guide to DAX/DAX Functions Covered.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github.com\open-word\DAX\Definitive Guide to DAX\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25958EE1-4490-4481-8D85-BECECA92569C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FA58050-DE88-4BB4-A0B8-D675600DD63F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="1680" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="18240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="67">
   <si>
     <t>CALCULATE</t>
   </si>
@@ -168,6 +168,75 @@
   </si>
   <si>
     <t>SUMX, VALUES</t>
+  </si>
+  <si>
+    <t>Time intelligence calculations</t>
+  </si>
+  <si>
+    <t>Introducing basic time intelligence functions</t>
+  </si>
+  <si>
+    <t>Computing a moving annual total</t>
+  </si>
+  <si>
+    <t>DATES IN PERIOD, DATEBETWEEN</t>
+  </si>
+  <si>
+    <t>Using the right call order for nested time intelligence functions</t>
+  </si>
+  <si>
+    <t>NEXTDAY, SAMEPERIODLASTYEAR</t>
+  </si>
+  <si>
+    <t>Introducing time intelligence</t>
+  </si>
+  <si>
+    <t>Building a date table</t>
+  </si>
+  <si>
+    <t>Understanding basic time intelligence calculations</t>
+  </si>
+  <si>
+    <t>Using CALENDAR and CALENDARAUTO</t>
+  </si>
+  <si>
+    <t>Working with multiple dates</t>
+  </si>
+  <si>
+    <t>Handling multiple relationships to the date table</t>
+  </si>
+  <si>
+    <t>Using Mark as Date Table</t>
+  </si>
+  <si>
+    <t>Handling multiple date tables</t>
+  </si>
+  <si>
+    <t>CALENDAR, CALENDARAUTO</t>
+  </si>
+  <si>
+    <t>CALCULATE, FILTER</t>
+  </si>
+  <si>
+    <t>Using YTD, QTD, MTD</t>
+  </si>
+  <si>
+    <t>Computing time periods from prior periods</t>
+  </si>
+  <si>
+    <t>Mixing time intelligence functions</t>
+  </si>
+  <si>
+    <t>Computing a difference over previous periods</t>
+  </si>
+  <si>
+    <t>DATESYTD, DATESQTD, DATESMTD, TOTALYTD, TOTALQTD, TOTALMTD</t>
+  </si>
+  <si>
+    <t>SAMEPERIODLASTYEAR, DATEADD, PARALLELPERIOD, PREVIOUSYEAR, PREVIOUSQUARTER, PREVIOUSMONTH</t>
+  </si>
+  <si>
+    <t>SAMEPERIODLASTYEAR, DATESYTD</t>
   </si>
 </sst>
 </file>
@@ -292,7 +361,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -305,12 +374,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -591,19 +655,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:K21"/>
+  <dimension ref="B1:K36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I40" sqref="I40"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="44.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="37.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="46.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="37.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="35.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="58" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="63.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="31.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="51.7109375" bestFit="1" customWidth="1"/>
   </cols>
@@ -916,7 +982,7 @@
       <c r="H15" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="I15" s="13" t="s">
+      <c r="I15" s="4" t="s">
         <v>38</v>
       </c>
       <c r="J15" s="4"/>
@@ -927,28 +993,27 @@
         <f t="shared" si="1"/>
         <v>070102</v>
       </c>
-      <c r="C16" s="14">
+      <c r="C16" s="1">
         <v>7</v>
       </c>
-      <c r="D16" s="15" t="s">
+      <c r="D16" t="s">
         <v>28</v>
       </c>
-      <c r="E16" s="14">
-        <v>1</v>
-      </c>
-      <c r="F16" s="15" t="s">
+      <c r="E16" s="1">
+        <v>1</v>
+      </c>
+      <c r="F16" t="s">
         <v>27</v>
       </c>
-      <c r="G16" s="14">
+      <c r="G16" s="1">
         <v>2</v>
       </c>
-      <c r="H16" s="15" t="s">
+      <c r="H16" t="s">
         <v>30</v>
       </c>
-      <c r="I16" s="12" t="s">
+      <c r="I16" t="s">
         <v>40</v>
       </c>
-      <c r="J16" s="15"/>
       <c r="K16" s="7"/>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.25">
@@ -956,28 +1021,27 @@
         <f t="shared" si="1"/>
         <v>070103</v>
       </c>
-      <c r="C17" s="14">
+      <c r="C17" s="1">
         <v>7</v>
       </c>
-      <c r="D17" s="15" t="s">
+      <c r="D17" t="s">
         <v>28</v>
       </c>
-      <c r="E17" s="14">
-        <v>1</v>
-      </c>
-      <c r="F17" s="15" t="s">
+      <c r="E17" s="1">
+        <v>1</v>
+      </c>
+      <c r="F17" t="s">
         <v>27</v>
       </c>
-      <c r="G17" s="14">
+      <c r="G17" s="1">
         <v>3</v>
       </c>
-      <c r="H17" s="15" t="s">
+      <c r="H17" t="s">
         <v>31</v>
       </c>
-      <c r="I17" s="15" t="s">
+      <c r="I17" t="s">
         <v>33</v>
       </c>
-      <c r="J17" s="15"/>
       <c r="K17" s="7"/>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.25">
@@ -985,28 +1049,27 @@
         <f t="shared" si="1"/>
         <v>070104</v>
       </c>
-      <c r="C18" s="14">
+      <c r="C18" s="1">
         <v>7</v>
       </c>
-      <c r="D18" s="15" t="s">
+      <c r="D18" t="s">
         <v>28</v>
       </c>
-      <c r="E18" s="14">
-        <v>1</v>
-      </c>
-      <c r="F18" s="15" t="s">
+      <c r="E18" s="1">
+        <v>1</v>
+      </c>
+      <c r="F18" t="s">
         <v>27</v>
       </c>
-      <c r="G18" s="14">
-        <v>4</v>
-      </c>
-      <c r="H18" s="15" t="s">
+      <c r="G18" s="1">
+        <v>4</v>
+      </c>
+      <c r="H18" t="s">
         <v>39</v>
       </c>
-      <c r="I18" s="15" t="s">
+      <c r="I18" t="s">
         <v>32</v>
       </c>
-      <c r="J18" s="15"/>
       <c r="K18" s="7"/>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.25">
@@ -1014,28 +1077,27 @@
         <f t="shared" si="1"/>
         <v>070201</v>
       </c>
-      <c r="C19" s="14">
+      <c r="C19" s="1">
         <v>7</v>
       </c>
-      <c r="D19" s="15" t="s">
+      <c r="D19" t="s">
         <v>28</v>
       </c>
-      <c r="E19" s="14">
+      <c r="E19" s="1">
         <v>2</v>
       </c>
-      <c r="F19" s="15" t="s">
+      <c r="F19" t="s">
         <v>34</v>
       </c>
-      <c r="G19" s="14">
-        <v>1</v>
-      </c>
-      <c r="H19" s="15" t="s">
+      <c r="G19" s="1">
+        <v>1</v>
+      </c>
+      <c r="H19" t="s">
         <v>35</v>
       </c>
-      <c r="I19" s="15" t="s">
+      <c r="I19" t="s">
         <v>37</v>
       </c>
-      <c r="J19" s="15"/>
       <c r="K19" s="7"/>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.25">
@@ -1043,28 +1105,27 @@
         <f t="shared" si="1"/>
         <v>070202</v>
       </c>
-      <c r="C20" s="14">
+      <c r="C20" s="1">
         <v>7</v>
       </c>
-      <c r="D20" s="15" t="s">
+      <c r="D20" t="s">
         <v>28</v>
       </c>
-      <c r="E20" s="14">
+      <c r="E20" s="1">
         <v>2</v>
       </c>
-      <c r="F20" s="15" t="s">
+      <c r="F20" t="s">
         <v>34</v>
       </c>
-      <c r="G20" s="14">
+      <c r="G20" s="1">
         <v>2</v>
       </c>
-      <c r="H20" s="15" t="s">
+      <c r="H20" t="s">
         <v>36</v>
       </c>
-      <c r="I20" s="15" t="s">
+      <c r="I20" t="s">
         <v>41</v>
       </c>
-      <c r="J20" s="15"/>
       <c r="K20" s="7"/>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.25">
@@ -1084,17 +1145,380 @@
       <c r="F21" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="G21" s="16">
+      <c r="G21" s="9">
         <v>3</v>
       </c>
-      <c r="H21" s="17" t="s">
+      <c r="H21" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="I21" s="17" t="s">
+      <c r="I21" s="10" t="s">
         <v>43</v>
       </c>
       <c r="J21" s="10"/>
       <c r="K21" s="11"/>
+    </row>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B23" s="6" t="str">
+        <f t="shared" ref="B23:B34" si="3">_xlfn.CONCAT(TEXT(C23,"00"),TEXT(E23,"00"),TEXT(G23,"00"))</f>
+        <v>080101</v>
+      </c>
+      <c r="C23" s="1">
+        <v>8</v>
+      </c>
+      <c r="D23" t="s">
+        <v>44</v>
+      </c>
+      <c r="E23" s="12">
+        <v>1</v>
+      </c>
+      <c r="F23" t="s">
+        <v>50</v>
+      </c>
+      <c r="G23" s="12">
+        <v>1</v>
+      </c>
+      <c r="H23" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B24" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>080102</v>
+      </c>
+      <c r="C24" s="1">
+        <v>8</v>
+      </c>
+      <c r="D24" t="s">
+        <v>44</v>
+      </c>
+      <c r="E24" s="12">
+        <v>1</v>
+      </c>
+      <c r="F24" t="s">
+        <v>50</v>
+      </c>
+      <c r="G24" s="12">
+        <v>2</v>
+      </c>
+      <c r="H24" t="s">
+        <v>53</v>
+      </c>
+      <c r="I24" s="12" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B25" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>080103</v>
+      </c>
+      <c r="C25" s="1">
+        <v>8</v>
+      </c>
+      <c r="D25" t="s">
+        <v>44</v>
+      </c>
+      <c r="E25" s="12">
+        <v>1</v>
+      </c>
+      <c r="F25" t="s">
+        <v>50</v>
+      </c>
+      <c r="G25" s="12">
+        <v>3</v>
+      </c>
+      <c r="H25" t="s">
+        <v>54</v>
+      </c>
+      <c r="I25" s="12" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B26" s="6" t="str">
+        <f>_xlfn.CONCAT(TEXT(C26,"00"),TEXT(E26,"00"),TEXT(G26,"00"))</f>
+        <v>080104</v>
+      </c>
+      <c r="C26" s="1">
+        <v>8</v>
+      </c>
+      <c r="D26" t="s">
+        <v>44</v>
+      </c>
+      <c r="E26" s="12">
+        <v>1</v>
+      </c>
+      <c r="F26" t="s">
+        <v>50</v>
+      </c>
+      <c r="G26" s="12">
+        <v>4</v>
+      </c>
+      <c r="H26" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B27" s="6" t="str">
+        <f>_xlfn.CONCAT(TEXT(C27,"00"),TEXT(E27,"00"),TEXT(G27,"00"))</f>
+        <v>080105</v>
+      </c>
+      <c r="C27" s="1">
+        <v>8</v>
+      </c>
+      <c r="D27" t="s">
+        <v>44</v>
+      </c>
+      <c r="E27" s="12">
+        <v>1</v>
+      </c>
+      <c r="F27" t="s">
+        <v>50</v>
+      </c>
+      <c r="G27" s="12">
+        <v>5</v>
+      </c>
+      <c r="H27" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B28" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>080200</v>
+      </c>
+      <c r="C28" s="1">
+        <v>8</v>
+      </c>
+      <c r="D28" t="s">
+        <v>44</v>
+      </c>
+      <c r="E28" s="12">
+        <v>2</v>
+      </c>
+      <c r="F28" t="s">
+        <v>51</v>
+      </c>
+      <c r="G28" s="12">
+        <v>0</v>
+      </c>
+      <c r="H28" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B29" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>080300</v>
+      </c>
+      <c r="C29" s="1">
+        <v>8</v>
+      </c>
+      <c r="D29" t="s">
+        <v>44</v>
+      </c>
+      <c r="E29" s="12">
+        <v>3</v>
+      </c>
+      <c r="F29" t="s">
+        <v>52</v>
+      </c>
+      <c r="G29" s="12">
+        <v>0</v>
+      </c>
+      <c r="H29" t="s">
+        <v>52</v>
+      </c>
+      <c r="I29" s="12" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B30" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>080301</v>
+      </c>
+      <c r="C30" s="1">
+        <v>8</v>
+      </c>
+      <c r="D30" t="s">
+        <v>44</v>
+      </c>
+      <c r="E30" s="12">
+        <v>3</v>
+      </c>
+      <c r="F30" t="s">
+        <v>52</v>
+      </c>
+      <c r="G30" s="12">
+        <v>1</v>
+      </c>
+      <c r="H30" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B31" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>080401</v>
+      </c>
+      <c r="C31" s="1">
+        <v>8</v>
+      </c>
+      <c r="D31" t="s">
+        <v>44</v>
+      </c>
+      <c r="E31" s="1">
+        <v>4</v>
+      </c>
+      <c r="F31" t="s">
+        <v>45</v>
+      </c>
+      <c r="G31" s="12">
+        <v>1</v>
+      </c>
+      <c r="H31" t="s">
+        <v>60</v>
+      </c>
+      <c r="I31" s="12" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="32" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B32" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>080402</v>
+      </c>
+      <c r="C32" s="1">
+        <v>8</v>
+      </c>
+      <c r="D32" t="s">
+        <v>44</v>
+      </c>
+      <c r="E32" s="1">
+        <v>4</v>
+      </c>
+      <c r="F32" t="s">
+        <v>45</v>
+      </c>
+      <c r="G32" s="12">
+        <v>2</v>
+      </c>
+      <c r="H32" t="s">
+        <v>61</v>
+      </c>
+      <c r="I32" s="12" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B33" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>080403</v>
+      </c>
+      <c r="C33" s="1">
+        <v>8</v>
+      </c>
+      <c r="D33" t="s">
+        <v>44</v>
+      </c>
+      <c r="E33" s="1">
+        <v>4</v>
+      </c>
+      <c r="F33" t="s">
+        <v>45</v>
+      </c>
+      <c r="G33" s="12">
+        <v>3</v>
+      </c>
+      <c r="H33" t="s">
+        <v>62</v>
+      </c>
+      <c r="I33" s="12" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B34" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>080404</v>
+      </c>
+      <c r="C34" s="1">
+        <v>8</v>
+      </c>
+      <c r="D34" t="s">
+        <v>44</v>
+      </c>
+      <c r="E34" s="1">
+        <v>4</v>
+      </c>
+      <c r="F34" t="s">
+        <v>45</v>
+      </c>
+      <c r="G34" s="12">
+        <v>4</v>
+      </c>
+      <c r="H34" t="s">
+        <v>63</v>
+      </c>
+      <c r="I34" s="12" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B35" s="6" t="str">
+        <f t="shared" ref="B35:B36" si="4">_xlfn.CONCAT(TEXT(C35,"00"),TEXT(E35,"00"),TEXT(G35,"00"))</f>
+        <v>080405</v>
+      </c>
+      <c r="C35" s="1">
+        <v>8</v>
+      </c>
+      <c r="D35" t="s">
+        <v>44</v>
+      </c>
+      <c r="E35" s="1">
+        <v>4</v>
+      </c>
+      <c r="F35" t="s">
+        <v>45</v>
+      </c>
+      <c r="G35" s="1">
+        <v>5</v>
+      </c>
+      <c r="H35" t="s">
+        <v>46</v>
+      </c>
+      <c r="I35" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B36" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>080406</v>
+      </c>
+      <c r="C36" s="1">
+        <v>8</v>
+      </c>
+      <c r="D36" t="s">
+        <v>44</v>
+      </c>
+      <c r="E36" s="1">
+        <v>4</v>
+      </c>
+      <c r="F36" t="s">
+        <v>45</v>
+      </c>
+      <c r="G36" s="1">
+        <v>6</v>
+      </c>
+      <c r="H36" t="s">
+        <v>48</v>
+      </c>
+      <c r="I36" s="1" t="s">
+        <v>49</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
Complete Ch 08 05 Understanding semi-additive calculations
</commit_message>
<xml_diff>
--- a/Definitive Guide to DAX/DAX Functions Covered.xlsx
+++ b/Definitive Guide to DAX/DAX Functions Covered.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github.com\open-word\DAX\Definitive Guide to DAX\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FA58050-DE88-4BB4-A0B8-D675600DD63F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01E7C850-5238-4262-887F-FEAE5DB7745F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="18240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="1680" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="71">
   <si>
     <t>CALCULATE</t>
   </si>
@@ -237,6 +237,18 @@
   </si>
   <si>
     <t>SAMEPERIODLASTYEAR, DATESYTD</t>
+  </si>
+  <si>
+    <t>Understanding semi-additive calculations</t>
+  </si>
+  <si>
+    <t>Using LASTDATE and LASTNONBLANK</t>
+  </si>
+  <si>
+    <t>LASTDATE, LASTNONBLANK</t>
+  </si>
+  <si>
+    <t>Working with opening and closing balances</t>
   </si>
 </sst>
 </file>
@@ -361,7 +373,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -374,7 +386,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -655,10 +666,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:K36"/>
+  <dimension ref="B1:K38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I40" sqref="I40"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1168,13 +1179,13 @@
       <c r="D23" t="s">
         <v>44</v>
       </c>
-      <c r="E23" s="12">
+      <c r="E23" s="1">
         <v>1</v>
       </c>
       <c r="F23" t="s">
         <v>50</v>
       </c>
-      <c r="G23" s="12">
+      <c r="G23" s="1">
         <v>1</v>
       </c>
       <c r="H23" t="s">
@@ -1192,19 +1203,19 @@
       <c r="D24" t="s">
         <v>44</v>
       </c>
-      <c r="E24" s="12">
+      <c r="E24" s="1">
         <v>1</v>
       </c>
       <c r="F24" t="s">
         <v>50</v>
       </c>
-      <c r="G24" s="12">
+      <c r="G24" s="1">
         <v>2</v>
       </c>
       <c r="H24" t="s">
         <v>53</v>
       </c>
-      <c r="I24" s="12" t="s">
+      <c r="I24" s="1" t="s">
         <v>58</v>
       </c>
     </row>
@@ -1219,19 +1230,19 @@
       <c r="D25" t="s">
         <v>44</v>
       </c>
-      <c r="E25" s="12">
+      <c r="E25" s="1">
         <v>1</v>
       </c>
       <c r="F25" t="s">
         <v>50</v>
       </c>
-      <c r="G25" s="12">
+      <c r="G25" s="1">
         <v>3</v>
       </c>
       <c r="H25" t="s">
         <v>54</v>
       </c>
-      <c r="I25" s="12" t="s">
+      <c r="I25" s="1" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1246,13 +1257,13 @@
       <c r="D26" t="s">
         <v>44</v>
       </c>
-      <c r="E26" s="12">
+      <c r="E26" s="1">
         <v>1</v>
       </c>
       <c r="F26" t="s">
         <v>50</v>
       </c>
-      <c r="G26" s="12">
+      <c r="G26" s="1">
         <v>4</v>
       </c>
       <c r="H26" t="s">
@@ -1270,13 +1281,13 @@
       <c r="D27" t="s">
         <v>44</v>
       </c>
-      <c r="E27" s="12">
+      <c r="E27" s="1">
         <v>1</v>
       </c>
       <c r="F27" t="s">
         <v>50</v>
       </c>
-      <c r="G27" s="12">
+      <c r="G27" s="1">
         <v>5</v>
       </c>
       <c r="H27" t="s">
@@ -1294,13 +1305,13 @@
       <c r="D28" t="s">
         <v>44</v>
       </c>
-      <c r="E28" s="12">
+      <c r="E28" s="1">
         <v>2</v>
       </c>
       <c r="F28" t="s">
         <v>51</v>
       </c>
-      <c r="G28" s="12">
+      <c r="G28" s="1">
         <v>0</v>
       </c>
       <c r="H28" t="s">
@@ -1318,19 +1329,19 @@
       <c r="D29" t="s">
         <v>44</v>
       </c>
-      <c r="E29" s="12">
+      <c r="E29" s="1">
         <v>3</v>
       </c>
       <c r="F29" t="s">
         <v>52</v>
       </c>
-      <c r="G29" s="12">
+      <c r="G29" s="1">
         <v>0</v>
       </c>
       <c r="H29" t="s">
         <v>52</v>
       </c>
-      <c r="I29" s="12" t="s">
+      <c r="I29" s="1" t="s">
         <v>59</v>
       </c>
     </row>
@@ -1345,13 +1356,13 @@
       <c r="D30" t="s">
         <v>44</v>
       </c>
-      <c r="E30" s="12">
+      <c r="E30" s="1">
         <v>3</v>
       </c>
       <c r="F30" t="s">
         <v>52</v>
       </c>
-      <c r="G30" s="12">
+      <c r="G30" s="1">
         <v>1</v>
       </c>
       <c r="H30" t="s">
@@ -1375,13 +1386,13 @@
       <c r="F31" t="s">
         <v>45</v>
       </c>
-      <c r="G31" s="12">
+      <c r="G31" s="1">
         <v>1</v>
       </c>
       <c r="H31" t="s">
         <v>60</v>
       </c>
-      <c r="I31" s="12" t="s">
+      <c r="I31" s="1" t="s">
         <v>64</v>
       </c>
     </row>
@@ -1402,13 +1413,13 @@
       <c r="F32" t="s">
         <v>45</v>
       </c>
-      <c r="G32" s="12">
+      <c r="G32" s="1">
         <v>2</v>
       </c>
       <c r="H32" t="s">
         <v>61</v>
       </c>
-      <c r="I32" s="12" t="s">
+      <c r="I32" s="1" t="s">
         <v>65</v>
       </c>
     </row>
@@ -1429,13 +1440,13 @@
       <c r="F33" t="s">
         <v>45</v>
       </c>
-      <c r="G33" s="12">
+      <c r="G33" s="1">
         <v>3</v>
       </c>
       <c r="H33" t="s">
         <v>62</v>
       </c>
-      <c r="I33" s="12" t="s">
+      <c r="I33" s="1" t="s">
         <v>66</v>
       </c>
     </row>
@@ -1456,13 +1467,13 @@
       <c r="F34" t="s">
         <v>45</v>
       </c>
-      <c r="G34" s="12">
+      <c r="G34" s="1">
         <v>4</v>
       </c>
       <c r="H34" t="s">
         <v>63</v>
       </c>
-      <c r="I34" s="12" t="s">
+      <c r="I34" s="1" t="s">
         <v>66</v>
       </c>
     </row>
@@ -1518,6 +1529,37 @@
       </c>
       <c r="I36" s="1" t="s">
         <v>49</v>
+      </c>
+    </row>
+    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="E37" s="1">
+        <v>5</v>
+      </c>
+      <c r="F37" t="s">
+        <v>67</v>
+      </c>
+      <c r="G37" s="1">
+        <v>1</v>
+      </c>
+      <c r="H37" t="s">
+        <v>68</v>
+      </c>
+      <c r="I37" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="E38" s="1">
+        <v>5</v>
+      </c>
+      <c r="F38" t="s">
+        <v>67</v>
+      </c>
+      <c r="G38" s="1">
+        <v>2</v>
+      </c>
+      <c r="H38" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Complete Ch 08 06 Understanding advanced time intelligence calculations
</commit_message>
<xml_diff>
--- a/Definitive Guide to DAX/DAX Functions Covered.xlsx
+++ b/Definitive Guide to DAX/DAX Functions Covered.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github.com\open-word\DAX\Definitive Guide to DAX\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01E7C850-5238-4262-887F-FEAE5DB7745F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E6FE09D-A07E-489A-98A5-7B7FBB435124}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="1680" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="79">
   <si>
     <t>CALCULATE</t>
   </si>
@@ -249,6 +249,30 @@
   </si>
   <si>
     <t>Working with opening and closing balances</t>
+  </si>
+  <si>
+    <t>LASTNONBLANK, FIRSTNONBLANK, PARALLELPERIOD</t>
+  </si>
+  <si>
+    <t>Understanding advanced time intelligence calculations</t>
+  </si>
+  <si>
+    <t>Understanding periods to date</t>
+  </si>
+  <si>
+    <t>DATESYTD</t>
+  </si>
+  <si>
+    <t>Understanding DATEADD</t>
+  </si>
+  <si>
+    <t>Understanding FIRSTDATE, LASTDATE, FIRSTNONBLANK, LASTNONBLANK</t>
+  </si>
+  <si>
+    <t>FIRSTDATE, LASTDATE, FIRSTNONBLANK, LASTNONBLANK</t>
+  </si>
+  <si>
+    <t>Using drillthrough with time intelligence</t>
   </si>
 </sst>
 </file>
@@ -666,10 +690,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:K38"/>
+  <dimension ref="B1:K42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F39" sqref="F39"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H49" sqref="H49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -677,9 +701,9 @@
     <col min="2" max="2" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="44.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="46.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="50.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="58" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="66.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="63.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="31.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="51.7109375" bestFit="1" customWidth="1"/>
@@ -1532,6 +1556,16 @@
       </c>
     </row>
     <row r="37" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B37" s="6" t="str">
+        <f t="shared" ref="B37:B38" si="5">_xlfn.CONCAT(TEXT(C37,"00"),TEXT(E37,"00"),TEXT(G37,"00"))</f>
+        <v>080501</v>
+      </c>
+      <c r="C37" s="1">
+        <v>8</v>
+      </c>
+      <c r="D37" t="s">
+        <v>44</v>
+      </c>
       <c r="E37" s="1">
         <v>5</v>
       </c>
@@ -1549,6 +1583,16 @@
       </c>
     </row>
     <row r="38" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B38" s="6" t="str">
+        <f t="shared" si="5"/>
+        <v>080502</v>
+      </c>
+      <c r="C38" s="1">
+        <v>8</v>
+      </c>
+      <c r="D38" t="s">
+        <v>44</v>
+      </c>
       <c r="E38" s="1">
         <v>5</v>
       </c>
@@ -1560,6 +1604,111 @@
       </c>
       <c r="H38" t="s">
         <v>70</v>
+      </c>
+      <c r="I38" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B39" s="6" t="str">
+        <f t="shared" ref="B39:B41" si="6">_xlfn.CONCAT(TEXT(C39,"00"),TEXT(E39,"00"),TEXT(G39,"00"))</f>
+        <v>080601</v>
+      </c>
+      <c r="C39" s="1">
+        <v>8</v>
+      </c>
+      <c r="D39" t="s">
+        <v>44</v>
+      </c>
+      <c r="E39" s="1">
+        <v>6</v>
+      </c>
+      <c r="F39" t="s">
+        <v>72</v>
+      </c>
+      <c r="G39" s="1">
+        <v>1</v>
+      </c>
+      <c r="H39" t="s">
+        <v>73</v>
+      </c>
+      <c r="I39" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B40" s="6" t="str">
+        <f t="shared" si="6"/>
+        <v>080602</v>
+      </c>
+      <c r="C40" s="1">
+        <v>8</v>
+      </c>
+      <c r="D40" t="s">
+        <v>44</v>
+      </c>
+      <c r="E40" s="1">
+        <v>6</v>
+      </c>
+      <c r="F40" t="s">
+        <v>72</v>
+      </c>
+      <c r="G40" s="1">
+        <v>2</v>
+      </c>
+      <c r="H40" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B41" s="6" t="str">
+        <f t="shared" si="6"/>
+        <v>080603</v>
+      </c>
+      <c r="C41" s="1">
+        <v>8</v>
+      </c>
+      <c r="D41" t="s">
+        <v>44</v>
+      </c>
+      <c r="E41" s="1">
+        <v>6</v>
+      </c>
+      <c r="F41" t="s">
+        <v>72</v>
+      </c>
+      <c r="G41" s="1">
+        <v>3</v>
+      </c>
+      <c r="H41" t="s">
+        <v>76</v>
+      </c>
+      <c r="I41" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="42" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B42" s="6" t="str">
+        <f t="shared" ref="B42" si="7">_xlfn.CONCAT(TEXT(C42,"00"),TEXT(E42,"00"),TEXT(G42,"00"))</f>
+        <v>080604</v>
+      </c>
+      <c r="C42" s="1">
+        <v>8</v>
+      </c>
+      <c r="D42" t="s">
+        <v>44</v>
+      </c>
+      <c r="E42" s="1">
+        <v>6</v>
+      </c>
+      <c r="F42" t="s">
+        <v>72</v>
+      </c>
+      <c r="G42" s="1">
+        <v>4</v>
+      </c>
+      <c r="H42" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Complete Ch 08  Time intelligence calculations
</commit_message>
<xml_diff>
--- a/Definitive Guide to DAX/DAX Functions Covered.xlsx
+++ b/Definitive Guide to DAX/DAX Functions Covered.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github.com\open-word\DAX\Definitive Guide to DAX\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E6FE09D-A07E-489A-98A5-7B7FBB435124}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA4CA341-971A-49B9-869D-6A6BA96D47A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="1680" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="82">
   <si>
     <t>CALCULATE</t>
   </si>
@@ -273,6 +273,15 @@
   </si>
   <si>
     <t>Using drillthrough with time intelligence</t>
+  </si>
+  <si>
+    <t>Working with custom calendars</t>
+  </si>
+  <si>
+    <t>Working with weeks</t>
+  </si>
+  <si>
+    <t>Custom year-to-date, quarter-to-date, and month-to-date</t>
   </si>
 </sst>
 </file>
@@ -397,7 +406,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -410,6 +419,11 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -690,10 +704,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:K42"/>
+  <dimension ref="B1:K43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H49" sqref="H49"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E51" sqref="E51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1192,524 +1206,629 @@
       <c r="J21" s="10"/>
       <c r="K21" s="11"/>
     </row>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B22" s="2" t="str">
+        <f t="shared" ref="B22:B33" si="3">_xlfn.CONCAT(TEXT(C22,"00"),TEXT(E22,"00"),TEXT(G22,"00"))</f>
+        <v>080101</v>
+      </c>
+      <c r="C22" s="3">
+        <v>8</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E22" s="3">
+        <v>1</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G22" s="3">
+        <v>1</v>
+      </c>
+      <c r="H22" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="I22" s="4"/>
+      <c r="J22" s="4"/>
+      <c r="K22" s="5"/>
+    </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B23" s="6" t="str">
-        <f t="shared" ref="B23:B34" si="3">_xlfn.CONCAT(TEXT(C23,"00"),TEXT(E23,"00"),TEXT(G23,"00"))</f>
-        <v>080101</v>
-      </c>
-      <c r="C23" s="1">
-        <v>8</v>
-      </c>
-      <c r="D23" t="s">
-        <v>44</v>
-      </c>
-      <c r="E23" s="1">
-        <v>1</v>
-      </c>
-      <c r="F23" t="s">
+        <f t="shared" si="3"/>
+        <v>080102</v>
+      </c>
+      <c r="C23" s="12">
+        <v>8</v>
+      </c>
+      <c r="D23" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="E23" s="12">
+        <v>1</v>
+      </c>
+      <c r="F23" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="G23" s="1">
-        <v>1</v>
-      </c>
-      <c r="H23" t="s">
-        <v>51</v>
-      </c>
+      <c r="G23" s="12">
+        <v>2</v>
+      </c>
+      <c r="H23" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="I23" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="J23" s="13"/>
+      <c r="K23" s="7"/>
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B24" s="6" t="str">
         <f t="shared" si="3"/>
-        <v>080102</v>
-      </c>
-      <c r="C24" s="1">
-        <v>8</v>
-      </c>
-      <c r="D24" t="s">
-        <v>44</v>
-      </c>
-      <c r="E24" s="1">
-        <v>1</v>
-      </c>
-      <c r="F24" t="s">
+        <v>080103</v>
+      </c>
+      <c r="C24" s="12">
+        <v>8</v>
+      </c>
+      <c r="D24" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="E24" s="12">
+        <v>1</v>
+      </c>
+      <c r="F24" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="G24" s="1">
-        <v>2</v>
-      </c>
-      <c r="H24" t="s">
-        <v>53</v>
-      </c>
-      <c r="I24" s="1" t="s">
-        <v>58</v>
-      </c>
+      <c r="G24" s="12">
+        <v>3</v>
+      </c>
+      <c r="H24" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="I24" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="J24" s="13"/>
+      <c r="K24" s="7"/>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B25" s="6" t="str">
-        <f t="shared" si="3"/>
-        <v>080103</v>
-      </c>
-      <c r="C25" s="1">
-        <v>8</v>
-      </c>
-      <c r="D25" t="s">
-        <v>44</v>
-      </c>
-      <c r="E25" s="1">
-        <v>1</v>
-      </c>
-      <c r="F25" t="s">
+        <f>_xlfn.CONCAT(TEXT(C25,"00"),TEXT(E25,"00"),TEXT(G25,"00"))</f>
+        <v>080104</v>
+      </c>
+      <c r="C25" s="12">
+        <v>8</v>
+      </c>
+      <c r="D25" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="E25" s="12">
+        <v>1</v>
+      </c>
+      <c r="F25" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="G25" s="1">
-        <v>3</v>
-      </c>
-      <c r="H25" t="s">
-        <v>54</v>
-      </c>
-      <c r="I25" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="G25" s="12">
+        <v>4</v>
+      </c>
+      <c r="H25" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="I25" s="13"/>
+      <c r="J25" s="13"/>
+      <c r="K25" s="7"/>
     </row>
     <row r="26" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B26" s="6" t="str">
         <f>_xlfn.CONCAT(TEXT(C26,"00"),TEXT(E26,"00"),TEXT(G26,"00"))</f>
-        <v>080104</v>
-      </c>
-      <c r="C26" s="1">
-        <v>8</v>
-      </c>
-      <c r="D26" t="s">
-        <v>44</v>
-      </c>
-      <c r="E26" s="1">
-        <v>1</v>
-      </c>
-      <c r="F26" t="s">
+        <v>080105</v>
+      </c>
+      <c r="C26" s="12">
+        <v>8</v>
+      </c>
+      <c r="D26" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="E26" s="12">
+        <v>1</v>
+      </c>
+      <c r="F26" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="G26" s="1">
-        <v>4</v>
-      </c>
-      <c r="H26" t="s">
-        <v>55</v>
-      </c>
+      <c r="G26" s="12">
+        <v>5</v>
+      </c>
+      <c r="H26" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="I26" s="13"/>
+      <c r="J26" s="13"/>
+      <c r="K26" s="7"/>
     </row>
     <row r="27" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B27" s="6" t="str">
-        <f>_xlfn.CONCAT(TEXT(C27,"00"),TEXT(E27,"00"),TEXT(G27,"00"))</f>
-        <v>080105</v>
-      </c>
-      <c r="C27" s="1">
-        <v>8</v>
-      </c>
-      <c r="D27" t="s">
-        <v>44</v>
-      </c>
-      <c r="E27" s="1">
-        <v>1</v>
-      </c>
-      <c r="F27" t="s">
-        <v>50</v>
-      </c>
-      <c r="G27" s="1">
-        <v>5</v>
-      </c>
-      <c r="H27" t="s">
-        <v>57</v>
-      </c>
+        <f t="shared" si="3"/>
+        <v>080200</v>
+      </c>
+      <c r="C27" s="12">
+        <v>8</v>
+      </c>
+      <c r="D27" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="E27" s="12">
+        <v>2</v>
+      </c>
+      <c r="F27" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="G27" s="12">
+        <v>0</v>
+      </c>
+      <c r="H27" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="I27" s="13"/>
+      <c r="J27" s="13"/>
+      <c r="K27" s="7"/>
     </row>
     <row r="28" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B28" s="6" t="str">
         <f t="shared" si="3"/>
-        <v>080200</v>
-      </c>
-      <c r="C28" s="1">
-        <v>8</v>
-      </c>
-      <c r="D28" t="s">
-        <v>44</v>
-      </c>
-      <c r="E28" s="1">
-        <v>2</v>
-      </c>
-      <c r="F28" t="s">
-        <v>51</v>
-      </c>
-      <c r="G28" s="1">
+        <v>080300</v>
+      </c>
+      <c r="C28" s="12">
+        <v>8</v>
+      </c>
+      <c r="D28" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="E28" s="12">
+        <v>3</v>
+      </c>
+      <c r="F28" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="G28" s="12">
         <v>0</v>
       </c>
-      <c r="H28" t="s">
-        <v>51</v>
-      </c>
+      <c r="H28" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="I28" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="J28" s="13"/>
+      <c r="K28" s="7"/>
     </row>
     <row r="29" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B29" s="6" t="str">
         <f t="shared" si="3"/>
-        <v>080300</v>
-      </c>
-      <c r="C29" s="1">
-        <v>8</v>
-      </c>
-      <c r="D29" t="s">
-        <v>44</v>
-      </c>
-      <c r="E29" s="1">
+        <v>080301</v>
+      </c>
+      <c r="C29" s="12">
+        <v>8</v>
+      </c>
+      <c r="D29" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="E29" s="12">
         <v>3</v>
       </c>
-      <c r="F29" t="s">
+      <c r="F29" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="G29" s="1">
-        <v>0</v>
-      </c>
-      <c r="H29" t="s">
-        <v>52</v>
-      </c>
-      <c r="I29" s="1" t="s">
-        <v>59</v>
-      </c>
+      <c r="G29" s="12">
+        <v>1</v>
+      </c>
+      <c r="H29" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="I29" s="13"/>
+      <c r="J29" s="13"/>
+      <c r="K29" s="7"/>
     </row>
     <row r="30" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B30" s="6" t="str">
         <f t="shared" si="3"/>
-        <v>080301</v>
-      </c>
-      <c r="C30" s="1">
-        <v>8</v>
-      </c>
-      <c r="D30" t="s">
-        <v>44</v>
-      </c>
-      <c r="E30" s="1">
-        <v>3</v>
-      </c>
-      <c r="F30" t="s">
-        <v>52</v>
-      </c>
-      <c r="G30" s="1">
-        <v>1</v>
-      </c>
-      <c r="H30" t="s">
-        <v>56</v>
-      </c>
+        <v>080401</v>
+      </c>
+      <c r="C30" s="12">
+        <v>8</v>
+      </c>
+      <c r="D30" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="E30" s="12">
+        <v>4</v>
+      </c>
+      <c r="F30" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="G30" s="12">
+        <v>1</v>
+      </c>
+      <c r="H30" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="I30" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="J30" s="13"/>
+      <c r="K30" s="7"/>
     </row>
     <row r="31" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B31" s="6" t="str">
         <f t="shared" si="3"/>
-        <v>080401</v>
-      </c>
-      <c r="C31" s="1">
-        <v>8</v>
-      </c>
-      <c r="D31" t="s">
-        <v>44</v>
-      </c>
-      <c r="E31" s="1">
+        <v>080402</v>
+      </c>
+      <c r="C31" s="12">
+        <v>8</v>
+      </c>
+      <c r="D31" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="E31" s="12">
         <v>4</v>
       </c>
-      <c r="F31" t="s">
+      <c r="F31" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="G31" s="1">
-        <v>1</v>
-      </c>
-      <c r="H31" t="s">
-        <v>60</v>
-      </c>
-      <c r="I31" s="1" t="s">
-        <v>64</v>
-      </c>
+      <c r="G31" s="12">
+        <v>2</v>
+      </c>
+      <c r="H31" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="I31" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="J31" s="13"/>
+      <c r="K31" s="7"/>
     </row>
     <row r="32" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B32" s="6" t="str">
         <f t="shared" si="3"/>
-        <v>080402</v>
-      </c>
-      <c r="C32" s="1">
-        <v>8</v>
-      </c>
-      <c r="D32" t="s">
-        <v>44</v>
-      </c>
-      <c r="E32" s="1">
+        <v>080403</v>
+      </c>
+      <c r="C32" s="12">
+        <v>8</v>
+      </c>
+      <c r="D32" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="E32" s="12">
         <v>4</v>
       </c>
-      <c r="F32" t="s">
+      <c r="F32" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="G32" s="1">
-        <v>2</v>
-      </c>
-      <c r="H32" t="s">
-        <v>61</v>
-      </c>
-      <c r="I32" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="G32" s="12">
+        <v>3</v>
+      </c>
+      <c r="H32" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="I32" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="J32" s="13"/>
+      <c r="K32" s="7"/>
+    </row>
+    <row r="33" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B33" s="6" t="str">
         <f t="shared" si="3"/>
-        <v>080403</v>
-      </c>
-      <c r="C33" s="1">
-        <v>8</v>
-      </c>
-      <c r="D33" t="s">
-        <v>44</v>
-      </c>
-      <c r="E33" s="1">
+        <v>080404</v>
+      </c>
+      <c r="C33" s="12">
+        <v>8</v>
+      </c>
+      <c r="D33" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="E33" s="12">
         <v>4</v>
       </c>
-      <c r="F33" t="s">
+      <c r="F33" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="G33" s="1">
-        <v>3</v>
-      </c>
-      <c r="H33" t="s">
-        <v>62</v>
-      </c>
-      <c r="I33" s="1" t="s">
+      <c r="G33" s="12">
+        <v>4</v>
+      </c>
+      <c r="H33" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="I33" s="12" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J33" s="13"/>
+      <c r="K33" s="7"/>
+    </row>
+    <row r="34" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B34" s="6" t="str">
-        <f t="shared" si="3"/>
-        <v>080404</v>
-      </c>
-      <c r="C34" s="1">
-        <v>8</v>
-      </c>
-      <c r="D34" t="s">
-        <v>44</v>
-      </c>
-      <c r="E34" s="1">
+        <f t="shared" ref="B34:B35" si="4">_xlfn.CONCAT(TEXT(C34,"00"),TEXT(E34,"00"),TEXT(G34,"00"))</f>
+        <v>080405</v>
+      </c>
+      <c r="C34" s="12">
+        <v>8</v>
+      </c>
+      <c r="D34" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="E34" s="12">
         <v>4</v>
       </c>
-      <c r="F34" t="s">
+      <c r="F34" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="G34" s="1">
-        <v>4</v>
-      </c>
-      <c r="H34" t="s">
-        <v>63</v>
-      </c>
-      <c r="I34" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="G34" s="12">
+        <v>5</v>
+      </c>
+      <c r="H34" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="I34" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="J34" s="13"/>
+      <c r="K34" s="7"/>
+    </row>
+    <row r="35" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B35" s="6" t="str">
-        <f t="shared" ref="B35:B36" si="4">_xlfn.CONCAT(TEXT(C35,"00"),TEXT(E35,"00"),TEXT(G35,"00"))</f>
-        <v>080405</v>
-      </c>
-      <c r="C35" s="1">
-        <v>8</v>
-      </c>
-      <c r="D35" t="s">
-        <v>44</v>
-      </c>
-      <c r="E35" s="1">
-        <v>4</v>
-      </c>
-      <c r="F35" t="s">
-        <v>45</v>
-      </c>
-      <c r="G35" s="1">
-        <v>5</v>
-      </c>
-      <c r="H35" t="s">
-        <v>46</v>
-      </c>
-      <c r="I35" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B36" s="6" t="str">
         <f t="shared" si="4"/>
         <v>080406</v>
       </c>
-      <c r="C36" s="1">
-        <v>8</v>
-      </c>
-      <c r="D36" t="s">
-        <v>44</v>
-      </c>
-      <c r="E36" s="1">
+      <c r="C35" s="12">
+        <v>8</v>
+      </c>
+      <c r="D35" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="E35" s="12">
         <v>4</v>
       </c>
-      <c r="F36" t="s">
+      <c r="F35" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="G36" s="1">
+      <c r="G35" s="12">
         <v>6</v>
       </c>
-      <c r="H36" t="s">
+      <c r="H35" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="I36" s="1" t="s">
+      <c r="I35" s="12" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J35" s="13"/>
+      <c r="K35" s="7"/>
+    </row>
+    <row r="36" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B36" s="6" t="str">
+        <f t="shared" ref="B36:B37" si="5">_xlfn.CONCAT(TEXT(C36,"00"),TEXT(E36,"00"),TEXT(G36,"00"))</f>
+        <v>080501</v>
+      </c>
+      <c r="C36" s="12">
+        <v>8</v>
+      </c>
+      <c r="D36" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="E36" s="12">
+        <v>5</v>
+      </c>
+      <c r="F36" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="G36" s="12">
+        <v>1</v>
+      </c>
+      <c r="H36" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="I36" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="J36" s="13"/>
+      <c r="K36" s="7"/>
+    </row>
+    <row r="37" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B37" s="6" t="str">
-        <f t="shared" ref="B37:B38" si="5">_xlfn.CONCAT(TEXT(C37,"00"),TEXT(E37,"00"),TEXT(G37,"00"))</f>
-        <v>080501</v>
-      </c>
-      <c r="C37" s="1">
-        <v>8</v>
-      </c>
-      <c r="D37" t="s">
-        <v>44</v>
-      </c>
-      <c r="E37" s="1">
-        <v>5</v>
-      </c>
-      <c r="F37" t="s">
-        <v>67</v>
-      </c>
-      <c r="G37" s="1">
-        <v>1</v>
-      </c>
-      <c r="H37" t="s">
-        <v>68</v>
-      </c>
-      <c r="I37" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B38" s="6" t="str">
         <f t="shared" si="5"/>
         <v>080502</v>
       </c>
-      <c r="C38" s="1">
-        <v>8</v>
-      </c>
-      <c r="D38" t="s">
-        <v>44</v>
-      </c>
-      <c r="E38" s="1">
-        <v>5</v>
-      </c>
-      <c r="F38" t="s">
+      <c r="C37" s="12">
+        <v>8</v>
+      </c>
+      <c r="D37" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="E37" s="12">
+        <v>5</v>
+      </c>
+      <c r="F37" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="G38" s="1">
+      <c r="G37" s="12">
         <v>2</v>
       </c>
-      <c r="H38" t="s">
+      <c r="H37" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="I38" s="1" t="s">
+      <c r="I37" s="12" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J37" s="13"/>
+      <c r="K37" s="7"/>
+    </row>
+    <row r="38" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B38" s="6" t="str">
+        <f t="shared" ref="B38:B40" si="6">_xlfn.CONCAT(TEXT(C38,"00"),TEXT(E38,"00"),TEXT(G38,"00"))</f>
+        <v>080601</v>
+      </c>
+      <c r="C38" s="12">
+        <v>8</v>
+      </c>
+      <c r="D38" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="E38" s="12">
+        <v>6</v>
+      </c>
+      <c r="F38" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="G38" s="12">
+        <v>1</v>
+      </c>
+      <c r="H38" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="I38" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="J38" s="13"/>
+      <c r="K38" s="7"/>
+    </row>
+    <row r="39" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B39" s="6" t="str">
-        <f t="shared" ref="B39:B41" si="6">_xlfn.CONCAT(TEXT(C39,"00"),TEXT(E39,"00"),TEXT(G39,"00"))</f>
-        <v>080601</v>
-      </c>
-      <c r="C39" s="1">
-        <v>8</v>
-      </c>
-      <c r="D39" t="s">
-        <v>44</v>
-      </c>
-      <c r="E39" s="1">
+        <f t="shared" si="6"/>
+        <v>080602</v>
+      </c>
+      <c r="C39" s="12">
+        <v>8</v>
+      </c>
+      <c r="D39" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="E39" s="12">
         <v>6</v>
       </c>
-      <c r="F39" t="s">
+      <c r="F39" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="G39" s="1">
-        <v>1</v>
-      </c>
-      <c r="H39" t="s">
-        <v>73</v>
-      </c>
-      <c r="I39" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="G39" s="12">
+        <v>2</v>
+      </c>
+      <c r="H39" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="I39" s="13"/>
+      <c r="J39" s="13"/>
+      <c r="K39" s="7"/>
+    </row>
+    <row r="40" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B40" s="6" t="str">
         <f t="shared" si="6"/>
-        <v>080602</v>
-      </c>
-      <c r="C40" s="1">
-        <v>8</v>
-      </c>
-      <c r="D40" t="s">
-        <v>44</v>
-      </c>
-      <c r="E40" s="1">
+        <v>080603</v>
+      </c>
+      <c r="C40" s="12">
+        <v>8</v>
+      </c>
+      <c r="D40" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="E40" s="12">
         <v>6</v>
       </c>
-      <c r="F40" t="s">
+      <c r="F40" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="G40" s="1">
+      <c r="G40" s="12">
+        <v>3</v>
+      </c>
+      <c r="H40" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="I40" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="J40" s="13"/>
+      <c r="K40" s="7"/>
+    </row>
+    <row r="41" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B41" s="6" t="str">
+        <f t="shared" ref="B41" si="7">_xlfn.CONCAT(TEXT(C41,"00"),TEXT(E41,"00"),TEXT(G41,"00"))</f>
+        <v>080604</v>
+      </c>
+      <c r="C41" s="12">
+        <v>8</v>
+      </c>
+      <c r="D41" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="E41" s="12">
+        <v>6</v>
+      </c>
+      <c r="F41" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="G41" s="12">
+        <v>4</v>
+      </c>
+      <c r="H41" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="I41" s="13"/>
+      <c r="J41" s="13"/>
+      <c r="K41" s="7"/>
+    </row>
+    <row r="42" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B42" s="6" t="str">
+        <f t="shared" ref="B42:B43" si="8">_xlfn.CONCAT(TEXT(C42,"00"),TEXT(E42,"00"),TEXT(G42,"00"))</f>
+        <v>080701</v>
+      </c>
+      <c r="C42" s="12">
+        <v>8</v>
+      </c>
+      <c r="D42" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="E42" s="12">
+        <v>7</v>
+      </c>
+      <c r="F42" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="G42" s="12">
+        <v>1</v>
+      </c>
+      <c r="H42" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="I42" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="J42" s="13"/>
+      <c r="K42" s="7"/>
+    </row>
+    <row r="43" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B43" s="8" t="str">
+        <f t="shared" si="8"/>
+        <v>080702</v>
+      </c>
+      <c r="C43" s="9">
+        <v>8</v>
+      </c>
+      <c r="D43" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="E43" s="9">
+        <v>7</v>
+      </c>
+      <c r="F43" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="G43" s="9">
         <v>2</v>
       </c>
-      <c r="H40" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B41" s="6" t="str">
-        <f t="shared" si="6"/>
-        <v>080603</v>
-      </c>
-      <c r="C41" s="1">
-        <v>8</v>
-      </c>
-      <c r="D41" t="s">
-        <v>44</v>
-      </c>
-      <c r="E41" s="1">
-        <v>6</v>
-      </c>
-      <c r="F41" t="s">
-        <v>72</v>
-      </c>
-      <c r="G41" s="1">
-        <v>3</v>
-      </c>
-      <c r="H41" t="s">
-        <v>76</v>
-      </c>
-      <c r="I41" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="42" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B42" s="6" t="str">
-        <f t="shared" ref="B42" si="7">_xlfn.CONCAT(TEXT(C42,"00"),TEXT(E42,"00"),TEXT(G42,"00"))</f>
-        <v>080604</v>
-      </c>
-      <c r="C42" s="1">
-        <v>8</v>
-      </c>
-      <c r="D42" t="s">
-        <v>44</v>
-      </c>
-      <c r="E42" s="1">
-        <v>6</v>
-      </c>
-      <c r="F42" t="s">
-        <v>72</v>
-      </c>
-      <c r="G42" s="1">
-        <v>4</v>
-      </c>
-      <c r="H42" t="s">
-        <v>78</v>
-      </c>
+      <c r="H43" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="I43" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="J43" s="10"/>
+      <c r="K43" s="11"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
Complete Ch 09 Calculation groups
</commit_message>
<xml_diff>
--- a/Definitive Guide to DAX/DAX Functions Covered.xlsx
+++ b/Definitive Guide to DAX/DAX Functions Covered.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github.com\open-word\DAX\Definitive Guide to DAX\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA4CA341-971A-49B9-869D-6A6BA96D47A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E1D9302-C810-4A64-B579-CE71A65C5958}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="1680" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="92">
   <si>
     <t>CALCULATE</t>
   </si>
@@ -282,6 +282,36 @@
   </si>
   <si>
     <t>Custom year-to-date, quarter-to-date, and month-to-date</t>
+  </si>
+  <si>
+    <t>Calculation groups</t>
+  </si>
+  <si>
+    <t>Introducing calculation groups</t>
+  </si>
+  <si>
+    <t>Creating calculation groups</t>
+  </si>
+  <si>
+    <t>Understanding calculation groups</t>
+  </si>
+  <si>
+    <t>Understanding calculation item application</t>
+  </si>
+  <si>
+    <t>Understanding calculation group precedence</t>
+  </si>
+  <si>
+    <t>Including and excluding measures from calculation items</t>
+  </si>
+  <si>
+    <t>Understanding sideways recursion</t>
+  </si>
+  <si>
+    <t>Using the best practices</t>
+  </si>
+  <si>
+    <t>ISSELECTEDMEASURE</t>
   </si>
 </sst>
 </file>
@@ -406,7 +436,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -419,11 +449,17 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -704,10 +740,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:K43"/>
+  <dimension ref="B1:K51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E51" sqref="E51"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I50" sqref="I50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1238,28 +1274,27 @@
         <f t="shared" si="3"/>
         <v>080102</v>
       </c>
-      <c r="C23" s="12">
-        <v>8</v>
-      </c>
-      <c r="D23" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="E23" s="12">
-        <v>1</v>
-      </c>
-      <c r="F23" s="13" t="s">
+      <c r="C23" s="1">
+        <v>8</v>
+      </c>
+      <c r="D23" t="s">
+        <v>44</v>
+      </c>
+      <c r="E23" s="1">
+        <v>1</v>
+      </c>
+      <c r="F23" t="s">
         <v>50</v>
       </c>
-      <c r="G23" s="12">
+      <c r="G23" s="1">
         <v>2</v>
       </c>
-      <c r="H23" s="13" t="s">
+      <c r="H23" t="s">
         <v>53</v>
       </c>
-      <c r="I23" s="12" t="s">
+      <c r="I23" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="J23" s="13"/>
       <c r="K23" s="7"/>
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.25">
@@ -1267,28 +1302,27 @@
         <f t="shared" si="3"/>
         <v>080103</v>
       </c>
-      <c r="C24" s="12">
-        <v>8</v>
-      </c>
-      <c r="D24" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="E24" s="12">
-        <v>1</v>
-      </c>
-      <c r="F24" s="13" t="s">
+      <c r="C24" s="1">
+        <v>8</v>
+      </c>
+      <c r="D24" t="s">
+        <v>44</v>
+      </c>
+      <c r="E24" s="1">
+        <v>1</v>
+      </c>
+      <c r="F24" t="s">
         <v>50</v>
       </c>
-      <c r="G24" s="12">
+      <c r="G24" s="1">
         <v>3</v>
       </c>
-      <c r="H24" s="13" t="s">
+      <c r="H24" t="s">
         <v>54</v>
       </c>
-      <c r="I24" s="12" t="s">
+      <c r="I24" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="J24" s="13"/>
       <c r="K24" s="7"/>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.25">
@@ -1296,26 +1330,24 @@
         <f>_xlfn.CONCAT(TEXT(C25,"00"),TEXT(E25,"00"),TEXT(G25,"00"))</f>
         <v>080104</v>
       </c>
-      <c r="C25" s="12">
-        <v>8</v>
-      </c>
-      <c r="D25" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="E25" s="12">
-        <v>1</v>
-      </c>
-      <c r="F25" s="13" t="s">
+      <c r="C25" s="1">
+        <v>8</v>
+      </c>
+      <c r="D25" t="s">
+        <v>44</v>
+      </c>
+      <c r="E25" s="1">
+        <v>1</v>
+      </c>
+      <c r="F25" t="s">
         <v>50</v>
       </c>
-      <c r="G25" s="12">
+      <c r="G25" s="1">
         <v>4</v>
       </c>
-      <c r="H25" s="13" t="s">
+      <c r="H25" t="s">
         <v>55</v>
       </c>
-      <c r="I25" s="13"/>
-      <c r="J25" s="13"/>
       <c r="K25" s="7"/>
     </row>
     <row r="26" spans="2:11" x14ac:dyDescent="0.25">
@@ -1323,26 +1355,24 @@
         <f>_xlfn.CONCAT(TEXT(C26,"00"),TEXT(E26,"00"),TEXT(G26,"00"))</f>
         <v>080105</v>
       </c>
-      <c r="C26" s="12">
-        <v>8</v>
-      </c>
-      <c r="D26" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="E26" s="12">
-        <v>1</v>
-      </c>
-      <c r="F26" s="13" t="s">
+      <c r="C26" s="1">
+        <v>8</v>
+      </c>
+      <c r="D26" t="s">
+        <v>44</v>
+      </c>
+      <c r="E26" s="1">
+        <v>1</v>
+      </c>
+      <c r="F26" t="s">
         <v>50</v>
       </c>
-      <c r="G26" s="12">
-        <v>5</v>
-      </c>
-      <c r="H26" s="13" t="s">
+      <c r="G26" s="1">
+        <v>5</v>
+      </c>
+      <c r="H26" t="s">
         <v>57</v>
       </c>
-      <c r="I26" s="13"/>
-      <c r="J26" s="13"/>
       <c r="K26" s="7"/>
     </row>
     <row r="27" spans="2:11" x14ac:dyDescent="0.25">
@@ -1350,26 +1380,24 @@
         <f t="shared" si="3"/>
         <v>080200</v>
       </c>
-      <c r="C27" s="12">
-        <v>8</v>
-      </c>
-      <c r="D27" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="E27" s="12">
+      <c r="C27" s="1">
+        <v>8</v>
+      </c>
+      <c r="D27" t="s">
+        <v>44</v>
+      </c>
+      <c r="E27" s="1">
         <v>2</v>
       </c>
-      <c r="F27" s="13" t="s">
+      <c r="F27" t="s">
         <v>51</v>
       </c>
-      <c r="G27" s="12">
+      <c r="G27" s="1">
         <v>0</v>
       </c>
-      <c r="H27" s="13" t="s">
+      <c r="H27" t="s">
         <v>51</v>
       </c>
-      <c r="I27" s="13"/>
-      <c r="J27" s="13"/>
       <c r="K27" s="7"/>
     </row>
     <row r="28" spans="2:11" x14ac:dyDescent="0.25">
@@ -1377,28 +1405,27 @@
         <f t="shared" si="3"/>
         <v>080300</v>
       </c>
-      <c r="C28" s="12">
-        <v>8</v>
-      </c>
-      <c r="D28" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="E28" s="12">
+      <c r="C28" s="1">
+        <v>8</v>
+      </c>
+      <c r="D28" t="s">
+        <v>44</v>
+      </c>
+      <c r="E28" s="1">
         <v>3</v>
       </c>
-      <c r="F28" s="13" t="s">
+      <c r="F28" t="s">
         <v>52</v>
       </c>
-      <c r="G28" s="12">
+      <c r="G28" s="1">
         <v>0</v>
       </c>
-      <c r="H28" s="13" t="s">
+      <c r="H28" t="s">
         <v>52</v>
       </c>
-      <c r="I28" s="12" t="s">
+      <c r="I28" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="J28" s="13"/>
       <c r="K28" s="7"/>
     </row>
     <row r="29" spans="2:11" x14ac:dyDescent="0.25">
@@ -1406,26 +1433,24 @@
         <f t="shared" si="3"/>
         <v>080301</v>
       </c>
-      <c r="C29" s="12">
-        <v>8</v>
-      </c>
-      <c r="D29" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="E29" s="12">
+      <c r="C29" s="1">
+        <v>8</v>
+      </c>
+      <c r="D29" t="s">
+        <v>44</v>
+      </c>
+      <c r="E29" s="1">
         <v>3</v>
       </c>
-      <c r="F29" s="13" t="s">
+      <c r="F29" t="s">
         <v>52</v>
       </c>
-      <c r="G29" s="12">
-        <v>1</v>
-      </c>
-      <c r="H29" s="13" t="s">
+      <c r="G29" s="1">
+        <v>1</v>
+      </c>
+      <c r="H29" t="s">
         <v>56</v>
       </c>
-      <c r="I29" s="13"/>
-      <c r="J29" s="13"/>
       <c r="K29" s="7"/>
     </row>
     <row r="30" spans="2:11" x14ac:dyDescent="0.25">
@@ -1433,28 +1458,27 @@
         <f t="shared" si="3"/>
         <v>080401</v>
       </c>
-      <c r="C30" s="12">
-        <v>8</v>
-      </c>
-      <c r="D30" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="E30" s="12">
+      <c r="C30" s="1">
+        <v>8</v>
+      </c>
+      <c r="D30" t="s">
+        <v>44</v>
+      </c>
+      <c r="E30" s="1">
         <v>4</v>
       </c>
-      <c r="F30" s="13" t="s">
+      <c r="F30" t="s">
         <v>45</v>
       </c>
-      <c r="G30" s="12">
-        <v>1</v>
-      </c>
-      <c r="H30" s="13" t="s">
+      <c r="G30" s="1">
+        <v>1</v>
+      </c>
+      <c r="H30" t="s">
         <v>60</v>
       </c>
-      <c r="I30" s="12" t="s">
+      <c r="I30" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="J30" s="13"/>
       <c r="K30" s="7"/>
     </row>
     <row r="31" spans="2:11" x14ac:dyDescent="0.25">
@@ -1462,28 +1486,27 @@
         <f t="shared" si="3"/>
         <v>080402</v>
       </c>
-      <c r="C31" s="12">
-        <v>8</v>
-      </c>
-      <c r="D31" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="E31" s="12">
+      <c r="C31" s="1">
+        <v>8</v>
+      </c>
+      <c r="D31" t="s">
+        <v>44</v>
+      </c>
+      <c r="E31" s="1">
         <v>4</v>
       </c>
-      <c r="F31" s="13" t="s">
+      <c r="F31" t="s">
         <v>45</v>
       </c>
-      <c r="G31" s="12">
+      <c r="G31" s="1">
         <v>2</v>
       </c>
-      <c r="H31" s="13" t="s">
+      <c r="H31" t="s">
         <v>61</v>
       </c>
-      <c r="I31" s="12" t="s">
+      <c r="I31" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="J31" s="13"/>
       <c r="K31" s="7"/>
     </row>
     <row r="32" spans="2:11" x14ac:dyDescent="0.25">
@@ -1491,28 +1514,27 @@
         <f t="shared" si="3"/>
         <v>080403</v>
       </c>
-      <c r="C32" s="12">
-        <v>8</v>
-      </c>
-      <c r="D32" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="E32" s="12">
+      <c r="C32" s="1">
+        <v>8</v>
+      </c>
+      <c r="D32" t="s">
+        <v>44</v>
+      </c>
+      <c r="E32" s="1">
         <v>4</v>
       </c>
-      <c r="F32" s="13" t="s">
+      <c r="F32" t="s">
         <v>45</v>
       </c>
-      <c r="G32" s="12">
+      <c r="G32" s="1">
         <v>3</v>
       </c>
-      <c r="H32" s="13" t="s">
+      <c r="H32" t="s">
         <v>62</v>
       </c>
-      <c r="I32" s="12" t="s">
+      <c r="I32" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="J32" s="13"/>
       <c r="K32" s="7"/>
     </row>
     <row r="33" spans="2:11" x14ac:dyDescent="0.25">
@@ -1520,28 +1542,27 @@
         <f t="shared" si="3"/>
         <v>080404</v>
       </c>
-      <c r="C33" s="12">
-        <v>8</v>
-      </c>
-      <c r="D33" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="E33" s="12">
+      <c r="C33" s="1">
+        <v>8</v>
+      </c>
+      <c r="D33" t="s">
+        <v>44</v>
+      </c>
+      <c r="E33" s="1">
         <v>4</v>
       </c>
-      <c r="F33" s="13" t="s">
+      <c r="F33" t="s">
         <v>45</v>
       </c>
-      <c r="G33" s="12">
+      <c r="G33" s="1">
         <v>4</v>
       </c>
-      <c r="H33" s="13" t="s">
+      <c r="H33" t="s">
         <v>63</v>
       </c>
-      <c r="I33" s="12" t="s">
+      <c r="I33" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="J33" s="13"/>
       <c r="K33" s="7"/>
     </row>
     <row r="34" spans="2:11" x14ac:dyDescent="0.25">
@@ -1549,28 +1570,27 @@
         <f t="shared" ref="B34:B35" si="4">_xlfn.CONCAT(TEXT(C34,"00"),TEXT(E34,"00"),TEXT(G34,"00"))</f>
         <v>080405</v>
       </c>
-      <c r="C34" s="12">
-        <v>8</v>
-      </c>
-      <c r="D34" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="E34" s="12">
+      <c r="C34" s="1">
+        <v>8</v>
+      </c>
+      <c r="D34" t="s">
+        <v>44</v>
+      </c>
+      <c r="E34" s="1">
         <v>4</v>
       </c>
-      <c r="F34" s="13" t="s">
+      <c r="F34" t="s">
         <v>45</v>
       </c>
-      <c r="G34" s="12">
-        <v>5</v>
-      </c>
-      <c r="H34" s="13" t="s">
+      <c r="G34" s="1">
+        <v>5</v>
+      </c>
+      <c r="H34" t="s">
         <v>46</v>
       </c>
-      <c r="I34" s="12" t="s">
+      <c r="I34" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="J34" s="13"/>
       <c r="K34" s="7"/>
     </row>
     <row r="35" spans="2:11" x14ac:dyDescent="0.25">
@@ -1578,28 +1598,27 @@
         <f t="shared" si="4"/>
         <v>080406</v>
       </c>
-      <c r="C35" s="12">
-        <v>8</v>
-      </c>
-      <c r="D35" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="E35" s="12">
+      <c r="C35" s="1">
+        <v>8</v>
+      </c>
+      <c r="D35" t="s">
+        <v>44</v>
+      </c>
+      <c r="E35" s="1">
         <v>4</v>
       </c>
-      <c r="F35" s="13" t="s">
+      <c r="F35" t="s">
         <v>45</v>
       </c>
-      <c r="G35" s="12">
+      <c r="G35" s="1">
         <v>6</v>
       </c>
-      <c r="H35" s="13" t="s">
+      <c r="H35" t="s">
         <v>48</v>
       </c>
-      <c r="I35" s="12" t="s">
+      <c r="I35" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="J35" s="13"/>
       <c r="K35" s="7"/>
     </row>
     <row r="36" spans="2:11" x14ac:dyDescent="0.25">
@@ -1607,28 +1626,27 @@
         <f t="shared" ref="B36:B37" si="5">_xlfn.CONCAT(TEXT(C36,"00"),TEXT(E36,"00"),TEXT(G36,"00"))</f>
         <v>080501</v>
       </c>
-      <c r="C36" s="12">
-        <v>8</v>
-      </c>
-      <c r="D36" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="E36" s="12">
-        <v>5</v>
-      </c>
-      <c r="F36" s="13" t="s">
+      <c r="C36" s="1">
+        <v>8</v>
+      </c>
+      <c r="D36" t="s">
+        <v>44</v>
+      </c>
+      <c r="E36" s="1">
+        <v>5</v>
+      </c>
+      <c r="F36" t="s">
         <v>67</v>
       </c>
-      <c r="G36" s="12">
-        <v>1</v>
-      </c>
-      <c r="H36" s="13" t="s">
+      <c r="G36" s="1">
+        <v>1</v>
+      </c>
+      <c r="H36" t="s">
         <v>68</v>
       </c>
-      <c r="I36" s="12" t="s">
+      <c r="I36" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="J36" s="13"/>
       <c r="K36" s="7"/>
     </row>
     <row r="37" spans="2:11" x14ac:dyDescent="0.25">
@@ -1636,28 +1654,27 @@
         <f t="shared" si="5"/>
         <v>080502</v>
       </c>
-      <c r="C37" s="12">
-        <v>8</v>
-      </c>
-      <c r="D37" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="E37" s="12">
-        <v>5</v>
-      </c>
-      <c r="F37" s="13" t="s">
+      <c r="C37" s="1">
+        <v>8</v>
+      </c>
+      <c r="D37" t="s">
+        <v>44</v>
+      </c>
+      <c r="E37" s="1">
+        <v>5</v>
+      </c>
+      <c r="F37" t="s">
         <v>67</v>
       </c>
-      <c r="G37" s="12">
+      <c r="G37" s="1">
         <v>2</v>
       </c>
-      <c r="H37" s="13" t="s">
+      <c r="H37" t="s">
         <v>70</v>
       </c>
-      <c r="I37" s="12" t="s">
+      <c r="I37" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="J37" s="13"/>
       <c r="K37" s="7"/>
     </row>
     <row r="38" spans="2:11" x14ac:dyDescent="0.25">
@@ -1665,28 +1682,27 @@
         <f t="shared" ref="B38:B40" si="6">_xlfn.CONCAT(TEXT(C38,"00"),TEXT(E38,"00"),TEXT(G38,"00"))</f>
         <v>080601</v>
       </c>
-      <c r="C38" s="12">
-        <v>8</v>
-      </c>
-      <c r="D38" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="E38" s="12">
+      <c r="C38" s="1">
+        <v>8</v>
+      </c>
+      <c r="D38" t="s">
+        <v>44</v>
+      </c>
+      <c r="E38" s="1">
         <v>6</v>
       </c>
-      <c r="F38" s="13" t="s">
+      <c r="F38" t="s">
         <v>72</v>
       </c>
-      <c r="G38" s="12">
-        <v>1</v>
-      </c>
-      <c r="H38" s="13" t="s">
+      <c r="G38" s="1">
+        <v>1</v>
+      </c>
+      <c r="H38" t="s">
         <v>73</v>
       </c>
-      <c r="I38" s="12" t="s">
+      <c r="I38" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="J38" s="13"/>
       <c r="K38" s="7"/>
     </row>
     <row r="39" spans="2:11" x14ac:dyDescent="0.25">
@@ -1694,26 +1710,24 @@
         <f t="shared" si="6"/>
         <v>080602</v>
       </c>
-      <c r="C39" s="12">
-        <v>8</v>
-      </c>
-      <c r="D39" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="E39" s="12">
+      <c r="C39" s="1">
+        <v>8</v>
+      </c>
+      <c r="D39" t="s">
+        <v>44</v>
+      </c>
+      <c r="E39" s="1">
         <v>6</v>
       </c>
-      <c r="F39" s="13" t="s">
+      <c r="F39" t="s">
         <v>72</v>
       </c>
-      <c r="G39" s="12">
+      <c r="G39" s="1">
         <v>2</v>
       </c>
-      <c r="H39" s="13" t="s">
+      <c r="H39" t="s">
         <v>75</v>
       </c>
-      <c r="I39" s="13"/>
-      <c r="J39" s="13"/>
       <c r="K39" s="7"/>
     </row>
     <row r="40" spans="2:11" x14ac:dyDescent="0.25">
@@ -1721,28 +1735,27 @@
         <f t="shared" si="6"/>
         <v>080603</v>
       </c>
-      <c r="C40" s="12">
-        <v>8</v>
-      </c>
-      <c r="D40" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="E40" s="12">
+      <c r="C40" s="1">
+        <v>8</v>
+      </c>
+      <c r="D40" t="s">
+        <v>44</v>
+      </c>
+      <c r="E40" s="1">
         <v>6</v>
       </c>
-      <c r="F40" s="13" t="s">
+      <c r="F40" t="s">
         <v>72</v>
       </c>
-      <c r="G40" s="12">
+      <c r="G40" s="1">
         <v>3</v>
       </c>
-      <c r="H40" s="13" t="s">
+      <c r="H40" t="s">
         <v>76</v>
       </c>
-      <c r="I40" s="12" t="s">
+      <c r="I40" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="J40" s="13"/>
       <c r="K40" s="7"/>
     </row>
     <row r="41" spans="2:11" x14ac:dyDescent="0.25">
@@ -1750,55 +1763,52 @@
         <f t="shared" ref="B41" si="7">_xlfn.CONCAT(TEXT(C41,"00"),TEXT(E41,"00"),TEXT(G41,"00"))</f>
         <v>080604</v>
       </c>
-      <c r="C41" s="12">
-        <v>8</v>
-      </c>
-      <c r="D41" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="E41" s="12">
+      <c r="C41" s="1">
+        <v>8</v>
+      </c>
+      <c r="D41" t="s">
+        <v>44</v>
+      </c>
+      <c r="E41" s="1">
         <v>6</v>
       </c>
-      <c r="F41" s="13" t="s">
+      <c r="F41" t="s">
         <v>72</v>
       </c>
-      <c r="G41" s="12">
+      <c r="G41" s="1">
         <v>4</v>
       </c>
-      <c r="H41" s="13" t="s">
+      <c r="H41" t="s">
         <v>78</v>
       </c>
-      <c r="I41" s="13"/>
-      <c r="J41" s="13"/>
       <c r="K41" s="7"/>
     </row>
     <row r="42" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B42" s="6" t="str">
-        <f t="shared" ref="B42:B43" si="8">_xlfn.CONCAT(TEXT(C42,"00"),TEXT(E42,"00"),TEXT(G42,"00"))</f>
+        <f t="shared" ref="B42:B51" si="8">_xlfn.CONCAT(TEXT(C42,"00"),TEXT(E42,"00"),TEXT(G42,"00"))</f>
         <v>080701</v>
       </c>
-      <c r="C42" s="12">
-        <v>8</v>
-      </c>
-      <c r="D42" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="E42" s="12">
+      <c r="C42" s="1">
+        <v>8</v>
+      </c>
+      <c r="D42" t="s">
+        <v>44</v>
+      </c>
+      <c r="E42" s="1">
         <v>7</v>
       </c>
-      <c r="F42" s="13" t="s">
+      <c r="F42" t="s">
         <v>79</v>
       </c>
-      <c r="G42" s="12">
-        <v>1</v>
-      </c>
-      <c r="H42" s="13" t="s">
+      <c r="G42" s="1">
+        <v>1</v>
+      </c>
+      <c r="H42" t="s">
         <v>80</v>
       </c>
-      <c r="I42" s="12" t="s">
+      <c r="I42" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="J42" s="13"/>
       <c r="K42" s="7"/>
     </row>
     <row r="43" spans="2:11" x14ac:dyDescent="0.25">
@@ -1821,7 +1831,7 @@
       <c r="G43" s="9">
         <v>2</v>
       </c>
-      <c r="H43" s="14" t="s">
+      <c r="H43" s="12" t="s">
         <v>81</v>
       </c>
       <c r="I43" s="10" t="s">
@@ -1829,6 +1839,224 @@
       </c>
       <c r="J43" s="10"/>
       <c r="K43" s="11"/>
+    </row>
+    <row r="44" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B44" s="15" t="str">
+        <f t="shared" si="8"/>
+        <v>090101</v>
+      </c>
+      <c r="C44" s="16">
+        <v>9</v>
+      </c>
+      <c r="D44" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="E44" s="16">
+        <v>1</v>
+      </c>
+      <c r="F44" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="G44" s="16">
+        <v>1</v>
+      </c>
+      <c r="H44" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="I44" s="4"/>
+      <c r="J44" s="4"/>
+      <c r="K44" s="5"/>
+    </row>
+    <row r="45" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B45" s="6" t="str">
+        <f t="shared" si="8"/>
+        <v>090201</v>
+      </c>
+      <c r="C45" s="14">
+        <v>9</v>
+      </c>
+      <c r="D45" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="E45" s="14">
+        <v>2</v>
+      </c>
+      <c r="F45" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="G45" s="14">
+        <v>1</v>
+      </c>
+      <c r="H45" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="I45" s="18"/>
+      <c r="J45" s="18"/>
+      <c r="K45" s="7"/>
+    </row>
+    <row r="46" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B46" s="6" t="str">
+        <f t="shared" si="8"/>
+        <v>090301</v>
+      </c>
+      <c r="C46" s="14">
+        <v>9</v>
+      </c>
+      <c r="D46" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="E46" s="14">
+        <v>3</v>
+      </c>
+      <c r="F46" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="G46" s="14">
+        <v>1</v>
+      </c>
+      <c r="H46" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="I46" s="18"/>
+      <c r="J46" s="18"/>
+      <c r="K46" s="7"/>
+    </row>
+    <row r="47" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B47" s="6" t="str">
+        <f t="shared" si="8"/>
+        <v>090302</v>
+      </c>
+      <c r="C47" s="14">
+        <v>9</v>
+      </c>
+      <c r="D47" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="E47" s="14">
+        <v>3</v>
+      </c>
+      <c r="F47" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="G47" s="14">
+        <v>2</v>
+      </c>
+      <c r="H47" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="I47" s="18"/>
+      <c r="J47" s="18"/>
+      <c r="K47" s="7"/>
+    </row>
+    <row r="48" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B48" s="6" t="str">
+        <f t="shared" si="8"/>
+        <v>090303</v>
+      </c>
+      <c r="C48" s="14">
+        <v>9</v>
+      </c>
+      <c r="D48" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="E48" s="14">
+        <v>3</v>
+      </c>
+      <c r="F48" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="G48" s="14">
+        <v>3</v>
+      </c>
+      <c r="H48" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="I48" s="18"/>
+      <c r="J48" s="18"/>
+      <c r="K48" s="7"/>
+    </row>
+    <row r="49" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B49" s="6" t="str">
+        <f t="shared" si="8"/>
+        <v>090304</v>
+      </c>
+      <c r="C49" s="14">
+        <v>9</v>
+      </c>
+      <c r="D49" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="E49" s="14">
+        <v>3</v>
+      </c>
+      <c r="F49" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="G49" s="14">
+        <v>4</v>
+      </c>
+      <c r="H49" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="I49" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="J49" s="18"/>
+      <c r="K49" s="7"/>
+    </row>
+    <row r="50" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B50" s="6" t="str">
+        <f t="shared" si="8"/>
+        <v>090305</v>
+      </c>
+      <c r="C50" s="14">
+        <v>9</v>
+      </c>
+      <c r="D50" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="E50" s="14">
+        <v>3</v>
+      </c>
+      <c r="F50" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="G50" s="14">
+        <v>5</v>
+      </c>
+      <c r="H50" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="I50" s="18"/>
+      <c r="J50" s="18"/>
+      <c r="K50" s="7"/>
+    </row>
+    <row r="51" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B51" s="8" t="str">
+        <f t="shared" si="8"/>
+        <v>090401</v>
+      </c>
+      <c r="C51" s="19">
+        <v>9</v>
+      </c>
+      <c r="D51" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="E51" s="19">
+        <v>4</v>
+      </c>
+      <c r="F51" s="20" t="s">
+        <v>90</v>
+      </c>
+      <c r="G51" s="19">
+        <v>1</v>
+      </c>
+      <c r="H51" s="20" t="s">
+        <v>90</v>
+      </c>
+      <c r="I51" s="10"/>
+      <c r="J51" s="10"/>
+      <c r="K51" s="11"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
Complete CH 10 01 Introducing HASONEVALUE and SELECTEDVALUE
</commit_message>
<xml_diff>
--- a/Definitive Guide to DAX/DAX Functions Covered.xlsx
+++ b/Definitive Guide to DAX/DAX Functions Covered.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github.com\open-word\DAX\Definitive Guide to DAX\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E1D9302-C810-4A64-B579-CE71A65C5958}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{618951DF-9CF9-4577-8220-AF753E3EFAD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="1680" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="95">
   <si>
     <t>CALCULATE</t>
   </si>
@@ -312,6 +312,15 @@
   </si>
   <si>
     <t>ISSELECTEDMEASURE</t>
+  </si>
+  <si>
+    <t>Working with the filter context</t>
+  </si>
+  <si>
+    <t>Using HASONEVALUE and SELECTEDVALUE</t>
+  </si>
+  <si>
+    <t>HASONEVALUE, SELECTEDVALUE</t>
   </si>
 </sst>
 </file>
@@ -436,7 +445,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -454,12 +463,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -740,10 +743,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:K51"/>
+  <dimension ref="B1:K52"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I50" sqref="I50"/>
+      <selection activeCell="H58" sqref="H58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1841,23 +1844,23 @@
       <c r="K43" s="11"/>
     </row>
     <row r="44" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B44" s="15" t="str">
+      <c r="B44" s="2" t="str">
         <f t="shared" si="8"/>
         <v>090101</v>
       </c>
-      <c r="C44" s="16">
+      <c r="C44" s="3">
         <v>9</v>
       </c>
-      <c r="D44" s="17" t="s">
+      <c r="D44" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="E44" s="16">
-        <v>1</v>
-      </c>
-      <c r="F44" s="17" t="s">
+      <c r="E44" s="3">
+        <v>1</v>
+      </c>
+      <c r="F44" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="G44" s="16">
+      <c r="G44" s="3">
         <v>1</v>
       </c>
       <c r="H44" s="4" t="s">
@@ -1872,26 +1875,24 @@
         <f t="shared" si="8"/>
         <v>090201</v>
       </c>
-      <c r="C45" s="14">
+      <c r="C45" s="1">
         <v>9</v>
       </c>
-      <c r="D45" s="18" t="s">
+      <c r="D45" t="s">
         <v>82</v>
       </c>
-      <c r="E45" s="14">
+      <c r="E45" s="1">
         <v>2</v>
       </c>
-      <c r="F45" s="13" t="s">
+      <c r="F45" t="s">
         <v>84</v>
       </c>
-      <c r="G45" s="14">
-        <v>1</v>
-      </c>
-      <c r="H45" s="18" t="s">
+      <c r="G45" s="1">
+        <v>1</v>
+      </c>
+      <c r="H45" t="s">
         <v>84</v>
       </c>
-      <c r="I45" s="18"/>
-      <c r="J45" s="18"/>
       <c r="K45" s="7"/>
     </row>
     <row r="46" spans="2:11" x14ac:dyDescent="0.25">
@@ -1899,26 +1900,24 @@
         <f t="shared" si="8"/>
         <v>090301</v>
       </c>
-      <c r="C46" s="14">
+      <c r="C46" s="1">
         <v>9</v>
       </c>
-      <c r="D46" s="18" t="s">
+      <c r="D46" t="s">
         <v>82</v>
       </c>
-      <c r="E46" s="14">
+      <c r="E46" s="1">
         <v>3</v>
       </c>
-      <c r="F46" s="13" t="s">
+      <c r="F46" t="s">
         <v>85</v>
       </c>
-      <c r="G46" s="14">
-        <v>1</v>
-      </c>
-      <c r="H46" s="18" t="s">
+      <c r="G46" s="1">
+        <v>1</v>
+      </c>
+      <c r="H46" t="s">
         <v>85</v>
       </c>
-      <c r="I46" s="18"/>
-      <c r="J46" s="18"/>
       <c r="K46" s="7"/>
     </row>
     <row r="47" spans="2:11" x14ac:dyDescent="0.25">
@@ -1926,26 +1925,24 @@
         <f t="shared" si="8"/>
         <v>090302</v>
       </c>
-      <c r="C47" s="14">
+      <c r="C47" s="1">
         <v>9</v>
       </c>
-      <c r="D47" s="18" t="s">
+      <c r="D47" t="s">
         <v>82</v>
       </c>
-      <c r="E47" s="14">
+      <c r="E47" s="1">
         <v>3</v>
       </c>
-      <c r="F47" s="13" t="s">
+      <c r="F47" t="s">
         <v>85</v>
       </c>
-      <c r="G47" s="14">
+      <c r="G47" s="1">
         <v>2</v>
       </c>
-      <c r="H47" s="18" t="s">
+      <c r="H47" t="s">
         <v>86</v>
       </c>
-      <c r="I47" s="18"/>
-      <c r="J47" s="18"/>
       <c r="K47" s="7"/>
     </row>
     <row r="48" spans="2:11" x14ac:dyDescent="0.25">
@@ -1953,26 +1950,24 @@
         <f t="shared" si="8"/>
         <v>090303</v>
       </c>
-      <c r="C48" s="14">
+      <c r="C48" s="1">
         <v>9</v>
       </c>
-      <c r="D48" s="18" t="s">
+      <c r="D48" t="s">
         <v>82</v>
       </c>
-      <c r="E48" s="14">
+      <c r="E48" s="1">
         <v>3</v>
       </c>
-      <c r="F48" s="13" t="s">
+      <c r="F48" t="s">
         <v>85</v>
       </c>
-      <c r="G48" s="14">
+      <c r="G48" s="1">
         <v>3</v>
       </c>
-      <c r="H48" s="18" t="s">
+      <c r="H48" t="s">
         <v>87</v>
       </c>
-      <c r="I48" s="18"/>
-      <c r="J48" s="18"/>
       <c r="K48" s="7"/>
     </row>
     <row r="49" spans="2:11" x14ac:dyDescent="0.25">
@@ -1980,28 +1975,27 @@
         <f t="shared" si="8"/>
         <v>090304</v>
       </c>
-      <c r="C49" s="14">
+      <c r="C49" s="1">
         <v>9</v>
       </c>
-      <c r="D49" s="18" t="s">
+      <c r="D49" t="s">
         <v>82</v>
       </c>
-      <c r="E49" s="14">
+      <c r="E49" s="1">
         <v>3</v>
       </c>
-      <c r="F49" s="13" t="s">
+      <c r="F49" t="s">
         <v>85</v>
       </c>
-      <c r="G49" s="14">
+      <c r="G49" s="1">
         <v>4</v>
       </c>
-      <c r="H49" s="18" t="s">
+      <c r="H49" t="s">
         <v>88</v>
       </c>
-      <c r="I49" s="14" t="s">
+      <c r="I49" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="J49" s="18"/>
       <c r="K49" s="7"/>
     </row>
     <row r="50" spans="2:11" x14ac:dyDescent="0.25">
@@ -2009,26 +2003,24 @@
         <f t="shared" si="8"/>
         <v>090305</v>
       </c>
-      <c r="C50" s="14">
+      <c r="C50" s="1">
         <v>9</v>
       </c>
-      <c r="D50" s="18" t="s">
+      <c r="D50" t="s">
         <v>82</v>
       </c>
-      <c r="E50" s="14">
+      <c r="E50" s="1">
         <v>3</v>
       </c>
-      <c r="F50" s="13" t="s">
+      <c r="F50" t="s">
         <v>85</v>
       </c>
-      <c r="G50" s="14">
-        <v>5</v>
-      </c>
-      <c r="H50" s="13" t="s">
+      <c r="G50" s="1">
+        <v>5</v>
+      </c>
+      <c r="H50" t="s">
         <v>89</v>
       </c>
-      <c r="I50" s="18"/>
-      <c r="J50" s="18"/>
       <c r="K50" s="7"/>
     </row>
     <row r="51" spans="2:11" x14ac:dyDescent="0.25">
@@ -2036,27 +2028,54 @@
         <f t="shared" si="8"/>
         <v>090401</v>
       </c>
-      <c r="C51" s="19">
+      <c r="C51" s="9">
         <v>9</v>
       </c>
       <c r="D51" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="E51" s="19">
+      <c r="E51" s="9">
         <v>4</v>
       </c>
-      <c r="F51" s="20" t="s">
+      <c r="F51" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="G51" s="19">
-        <v>1</v>
-      </c>
-      <c r="H51" s="20" t="s">
+      <c r="G51" s="9">
+        <v>1</v>
+      </c>
+      <c r="H51" s="10" t="s">
         <v>90</v>
       </c>
       <c r="I51" s="10"/>
       <c r="J51" s="10"/>
       <c r="K51" s="11"/>
+    </row>
+    <row r="52" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B52" t="str">
+        <f t="shared" ref="B52" si="9">_xlfn.CONCAT(TEXT(C52,"00"),TEXT(E52,"00"),TEXT(G52,"00"))</f>
+        <v>100101</v>
+      </c>
+      <c r="C52" s="1">
+        <v>10</v>
+      </c>
+      <c r="D52" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="E52" s="14">
+        <v>1</v>
+      </c>
+      <c r="F52" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="G52" s="14">
+        <v>1</v>
+      </c>
+      <c r="H52" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="I52" s="14" t="s">
+        <v>94</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
Complete Ch 10 03 Understanding differences between VALUES and FILTERS
</commit_message>
<xml_diff>
--- a/Definitive Guide to DAX/DAX Functions Covered.xlsx
+++ b/Definitive Guide to DAX/DAX Functions Covered.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github.com\open-word\DAX\Definitive Guide to DAX\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{618951DF-9CF9-4577-8220-AF753E3EFAD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08481F71-B796-475E-B002-6198756AFFA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="1680" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="99">
   <si>
     <t>CALCULATE</t>
   </si>
@@ -321,6 +321,18 @@
   </si>
   <si>
     <t>HASONEVALUE, SELECTEDVALUE</t>
+  </si>
+  <si>
+    <t>ISFILTERED, ISCROSSFILTERED</t>
+  </si>
+  <si>
+    <t>Introducing ISFILTERED and ISCROSSFILTERED</t>
+  </si>
+  <si>
+    <t>Understanding differences between VALUES and FILTERS</t>
+  </si>
+  <si>
+    <t>VALUES, FILTERS</t>
   </si>
 </sst>
 </file>
@@ -743,10 +755,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:K52"/>
+  <dimension ref="B1:K58"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H58" sqref="H58"/>
+      <selection activeCell="H57" sqref="H57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2077,6 +2089,108 @@
         <v>94</v>
       </c>
     </row>
+    <row r="53" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B53" t="str">
+        <f t="shared" ref="B53:B58" si="10">_xlfn.CONCAT(TEXT(C53,"00"),TEXT(E53,"00"),TEXT(G53,"00"))</f>
+        <v>100201</v>
+      </c>
+      <c r="C53" s="1">
+        <v>10</v>
+      </c>
+      <c r="D53" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="E53" s="14">
+        <v>2</v>
+      </c>
+      <c r="F53" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="G53" s="14">
+        <v>1</v>
+      </c>
+      <c r="H53" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="I53" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="54" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B54" t="str">
+        <f t="shared" si="10"/>
+        <v>100301</v>
+      </c>
+      <c r="C54" s="1">
+        <v>10</v>
+      </c>
+      <c r="D54" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="E54" s="14">
+        <v>3</v>
+      </c>
+      <c r="F54" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="G54" s="14">
+        <v>1</v>
+      </c>
+      <c r="H54" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="I54" s="14" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="55" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B55" t="str">
+        <f t="shared" si="10"/>
+        <v>100000</v>
+      </c>
+      <c r="C55" s="1">
+        <v>10</v>
+      </c>
+      <c r="D55" s="13" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="56" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B56" t="str">
+        <f t="shared" si="10"/>
+        <v>100000</v>
+      </c>
+      <c r="C56" s="1">
+        <v>10</v>
+      </c>
+      <c r="D56" s="13" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="57" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B57" t="str">
+        <f t="shared" si="10"/>
+        <v>100000</v>
+      </c>
+      <c r="C57" s="1">
+        <v>10</v>
+      </c>
+      <c r="D57" s="13" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="58" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B58" t="str">
+        <f t="shared" si="10"/>
+        <v>100000</v>
+      </c>
+      <c r="C58" s="1">
+        <v>10</v>
+      </c>
+      <c r="D58" s="13" t="s">
+        <v>92</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Complete Ch 10 04 Understanding the difference between ALLEXCEPT and ALL, VALUES
</commit_message>
<xml_diff>
--- a/Definitive Guide to DAX/DAX Functions Covered.xlsx
+++ b/Definitive Guide to DAX/DAX Functions Covered.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github.com\open-word\DAX\Definitive Guide to DAX\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08481F71-B796-475E-B002-6198756AFFA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8478C3B2-6D1F-4EC5-B1C9-D1C6CFABD8A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="1680" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="101">
   <si>
     <t>CALCULATE</t>
   </si>
@@ -333,6 +333,12 @@
   </si>
   <si>
     <t>VALUES, FILTERS</t>
+  </si>
+  <si>
+    <t>ALLEXCEPT, ALL, VALUES</t>
+  </si>
+  <si>
+    <t>Understanding the difference between ALLEXCEPT and ALL, VALUES</t>
   </si>
 </sst>
 </file>
@@ -758,7 +764,7 @@
   <dimension ref="B1:K58"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H57" sqref="H57"/>
+      <selection activeCell="H56" sqref="H56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -766,7 +772,7 @@
     <col min="2" max="2" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="44.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="50.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="60.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="3" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="66.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="63.28515625" bestFit="1" customWidth="1"/>
@@ -2146,13 +2152,28 @@
     <row r="55" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B55" t="str">
         <f t="shared" si="10"/>
-        <v>100000</v>
+        <v>100401</v>
       </c>
       <c r="C55" s="1">
         <v>10</v>
       </c>
       <c r="D55" s="13" t="s">
         <v>92</v>
+      </c>
+      <c r="E55" s="14">
+        <v>4</v>
+      </c>
+      <c r="F55" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="G55" s="14">
+        <v>1</v>
+      </c>
+      <c r="H55" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="I55" s="14" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="56" spans="2:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Complete Ch 10 05 Using ALL to avoind context transition
</commit_message>
<xml_diff>
--- a/Definitive Guide to DAX/DAX Functions Covered.xlsx
+++ b/Definitive Guide to DAX/DAX Functions Covered.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github.com\open-word\DAX\Definitive Guide to DAX\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8478C3B2-6D1F-4EC5-B1C9-D1C6CFABD8A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91646FCA-EF5A-47DC-8CB6-BEB1F8F2BBFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="1680" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="105">
   <si>
     <t>CALCULATE</t>
   </si>
@@ -339,6 +339,18 @@
   </si>
   <si>
     <t>Understanding the difference between ALLEXCEPT and ALL, VALUES</t>
+  </si>
+  <si>
+    <t>Using ALL to avoid context transition</t>
+  </si>
+  <si>
+    <t>ALL, ALLEXCEPT</t>
+  </si>
+  <si>
+    <t>Using ISEMPTY</t>
+  </si>
+  <si>
+    <t>ISEMPTY</t>
   </si>
 </sst>
 </file>
@@ -763,8 +775,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:K58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H56" sqref="H56"/>
+    <sheetView tabSelected="1" topLeftCell="B28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I57" sqref="I57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -772,7 +784,7 @@
     <col min="2" max="2" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="44.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="60.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="62" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="3" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="66.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="63.28515625" bestFit="1" customWidth="1"/>
@@ -2179,25 +2191,55 @@
     <row r="56" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B56" t="str">
         <f t="shared" si="10"/>
-        <v>100000</v>
+        <v>100501</v>
       </c>
       <c r="C56" s="1">
         <v>10</v>
       </c>
       <c r="D56" s="13" t="s">
         <v>92</v>
+      </c>
+      <c r="E56" s="14">
+        <v>5</v>
+      </c>
+      <c r="F56" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="G56" s="14">
+        <v>1</v>
+      </c>
+      <c r="H56" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="I56" s="14" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="57" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B57" t="str">
         <f t="shared" si="10"/>
-        <v>100000</v>
+        <v>100601</v>
       </c>
       <c r="C57" s="1">
         <v>10</v>
       </c>
       <c r="D57" s="13" t="s">
         <v>92</v>
+      </c>
+      <c r="E57" s="14">
+        <v>6</v>
+      </c>
+      <c r="F57" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="G57" s="14">
+        <v>1</v>
+      </c>
+      <c r="H57" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="I57" s="14" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="58" spans="2:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Complete Ch 10 07 Introducing data lineage and TREATAS
</commit_message>
<xml_diff>
--- a/Definitive Guide to DAX/DAX Functions Covered.xlsx
+++ b/Definitive Guide to DAX/DAX Functions Covered.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github.com\open-word\DAX\Definitive Guide to DAX\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91646FCA-EF5A-47DC-8CB6-BEB1F8F2BBFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77F22C47-2EDF-467B-9947-85214961B814}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="1680" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="107">
   <si>
     <t>CALCULATE</t>
   </si>
@@ -351,6 +351,12 @@
   </si>
   <si>
     <t>ISEMPTY</t>
+  </si>
+  <si>
+    <t>Introducing data lineage and TREATAS</t>
+  </si>
+  <si>
+    <t>TREATAS</t>
   </si>
 </sst>
 </file>
@@ -475,7 +481,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -491,8 +497,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -776,7 +780,7 @@
   <dimension ref="B1:K58"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I57" sqref="I57"/>
+      <selection activeCell="I59" sqref="I59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2088,22 +2092,22 @@
       <c r="C52" s="1">
         <v>10</v>
       </c>
-      <c r="D52" s="13" t="s">
+      <c r="D52" t="s">
         <v>92</v>
       </c>
-      <c r="E52" s="14">
-        <v>1</v>
-      </c>
-      <c r="F52" s="13" t="s">
+      <c r="E52" s="1">
+        <v>1</v>
+      </c>
+      <c r="F52" t="s">
         <v>93</v>
       </c>
-      <c r="G52" s="14">
-        <v>1</v>
-      </c>
-      <c r="H52" s="13" t="s">
+      <c r="G52" s="1">
+        <v>1</v>
+      </c>
+      <c r="H52" t="s">
         <v>93</v>
       </c>
-      <c r="I52" s="14" t="s">
+      <c r="I52" s="1" t="s">
         <v>94</v>
       </c>
     </row>
@@ -2115,19 +2119,19 @@
       <c r="C53" s="1">
         <v>10</v>
       </c>
-      <c r="D53" s="13" t="s">
+      <c r="D53" t="s">
         <v>92</v>
       </c>
-      <c r="E53" s="14">
+      <c r="E53" s="1">
         <v>2</v>
       </c>
-      <c r="F53" s="13" t="s">
+      <c r="F53" t="s">
         <v>96</v>
       </c>
-      <c r="G53" s="14">
-        <v>1</v>
-      </c>
-      <c r="H53" s="13" t="s">
+      <c r="G53" s="1">
+        <v>1</v>
+      </c>
+      <c r="H53" t="s">
         <v>96</v>
       </c>
       <c r="I53" t="s">
@@ -2142,22 +2146,22 @@
       <c r="C54" s="1">
         <v>10</v>
       </c>
-      <c r="D54" s="13" t="s">
+      <c r="D54" t="s">
         <v>92</v>
       </c>
-      <c r="E54" s="14">
+      <c r="E54" s="1">
         <v>3</v>
       </c>
-      <c r="F54" s="13" t="s">
+      <c r="F54" t="s">
         <v>97</v>
       </c>
-      <c r="G54" s="14">
-        <v>1</v>
-      </c>
-      <c r="H54" s="13" t="s">
+      <c r="G54" s="1">
+        <v>1</v>
+      </c>
+      <c r="H54" t="s">
         <v>97</v>
       </c>
-      <c r="I54" s="14" t="s">
+      <c r="I54" s="1" t="s">
         <v>98</v>
       </c>
     </row>
@@ -2169,22 +2173,22 @@
       <c r="C55" s="1">
         <v>10</v>
       </c>
-      <c r="D55" s="13" t="s">
+      <c r="D55" t="s">
         <v>92</v>
       </c>
-      <c r="E55" s="14">
+      <c r="E55" s="1">
         <v>4</v>
       </c>
-      <c r="F55" s="13" t="s">
+      <c r="F55" t="s">
         <v>100</v>
       </c>
-      <c r="G55" s="14">
-        <v>1</v>
-      </c>
-      <c r="H55" s="13" t="s">
+      <c r="G55" s="1">
+        <v>1</v>
+      </c>
+      <c r="H55" t="s">
         <v>100</v>
       </c>
-      <c r="I55" s="14" t="s">
+      <c r="I55" s="1" t="s">
         <v>99</v>
       </c>
     </row>
@@ -2196,22 +2200,22 @@
       <c r="C56" s="1">
         <v>10</v>
       </c>
-      <c r="D56" s="13" t="s">
+      <c r="D56" t="s">
         <v>92</v>
       </c>
-      <c r="E56" s="14">
-        <v>5</v>
-      </c>
-      <c r="F56" s="13" t="s">
+      <c r="E56" s="1">
+        <v>5</v>
+      </c>
+      <c r="F56" t="s">
         <v>101</v>
       </c>
-      <c r="G56" s="14">
-        <v>1</v>
-      </c>
-      <c r="H56" s="13" t="s">
+      <c r="G56" s="1">
+        <v>1</v>
+      </c>
+      <c r="H56" t="s">
         <v>101</v>
       </c>
-      <c r="I56" s="14" t="s">
+      <c r="I56" s="1" t="s">
         <v>102</v>
       </c>
     </row>
@@ -2223,35 +2227,50 @@
       <c r="C57" s="1">
         <v>10</v>
       </c>
-      <c r="D57" s="13" t="s">
+      <c r="D57" t="s">
         <v>92</v>
       </c>
-      <c r="E57" s="14">
+      <c r="E57" s="1">
         <v>6</v>
       </c>
-      <c r="F57" s="13" t="s">
+      <c r="F57" t="s">
         <v>103</v>
       </c>
-      <c r="G57" s="14">
-        <v>1</v>
-      </c>
-      <c r="H57" s="13" t="s">
+      <c r="G57" s="1">
+        <v>1</v>
+      </c>
+      <c r="H57" t="s">
         <v>103</v>
       </c>
-      <c r="I57" s="14" t="s">
+      <c r="I57" s="1" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="58" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B58" t="str">
         <f t="shared" si="10"/>
-        <v>100000</v>
+        <v>100701</v>
       </c>
       <c r="C58" s="1">
         <v>10</v>
       </c>
-      <c r="D58" s="13" t="s">
+      <c r="D58" t="s">
         <v>92</v>
+      </c>
+      <c r="E58" s="1">
+        <v>7</v>
+      </c>
+      <c r="F58" t="s">
+        <v>105</v>
+      </c>
+      <c r="G58" s="1">
+        <v>1</v>
+      </c>
+      <c r="H58" t="s">
+        <v>105</v>
+      </c>
+      <c r="I58" s="1" t="s">
+        <v>106</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Complete Ch 10 Working with the filter context
</commit_message>
<xml_diff>
--- a/Definitive Guide to DAX/DAX Functions Covered.xlsx
+++ b/Definitive Guide to DAX/DAX Functions Covered.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github.com\open-word\DAX\Definitive Guide to DAX\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77F22C47-2EDF-467B-9947-85214961B814}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29821E06-CFA8-4375-8DDD-B263B2484389}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="1680" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="108">
   <si>
     <t>CALCULATE</t>
   </si>
@@ -357,6 +357,9 @@
   </si>
   <si>
     <t>TREATAS</t>
+  </si>
+  <si>
+    <t>Understanding arbitrarily shaped filters</t>
   </si>
 </sst>
 </file>
@@ -777,10 +780,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:K58"/>
+  <dimension ref="B1:K59"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I59" sqref="I59"/>
+      <selection activeCell="H60" sqref="H60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2273,6 +2276,30 @@
         <v>106</v>
       </c>
     </row>
+    <row r="59" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B59" t="str">
+        <f t="shared" ref="B59" si="11">_xlfn.CONCAT(TEXT(C59,"00"),TEXT(E59,"00"),TEXT(G59,"00"))</f>
+        <v>100801</v>
+      </c>
+      <c r="C59" s="1">
+        <v>10</v>
+      </c>
+      <c r="D59" t="s">
+        <v>92</v>
+      </c>
+      <c r="E59" s="1">
+        <v>8</v>
+      </c>
+      <c r="F59" t="s">
+        <v>107</v>
+      </c>
+      <c r="G59" s="1">
+        <v>1</v>
+      </c>
+      <c r="H59" t="s">
+        <v>107</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Complete Ch 11 01 Computing percentages over hierarchies
</commit_message>
<xml_diff>
--- a/Definitive Guide to DAX/DAX Functions Covered.xlsx
+++ b/Definitive Guide to DAX/DAX Functions Covered.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github.com\open-word\DAX\Definitive Guide to DAX\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29821E06-CFA8-4375-8DDD-B263B2484389}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95CA6F14-3F7A-4050-8A51-E6926FFB12D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="1680" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="111">
   <si>
     <t>CALCULATE</t>
   </si>
@@ -360,6 +360,15 @@
   </si>
   <si>
     <t>Understanding arbitrarily shaped filters</t>
+  </si>
+  <si>
+    <t>Handling hierarchies</t>
+  </si>
+  <si>
+    <t>Computing percentages over hierarchies</t>
+  </si>
+  <si>
+    <t>ALLSELECTED, ISINSCOPE</t>
   </si>
 </sst>
 </file>
@@ -484,7 +493,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -500,6 +509,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -780,10 +791,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:K59"/>
+  <dimension ref="B1:K60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H60" sqref="H60"/>
+    <sheetView tabSelected="1" topLeftCell="B31" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I61" sqref="I61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2088,217 +2099,263 @@
       <c r="K51" s="11"/>
     </row>
     <row r="52" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B52" t="str">
+      <c r="B52" s="2" t="str">
         <f t="shared" ref="B52" si="9">_xlfn.CONCAT(TEXT(C52,"00"),TEXT(E52,"00"),TEXT(G52,"00"))</f>
         <v>100101</v>
       </c>
-      <c r="C52" s="1">
+      <c r="C52" s="3">
         <v>10</v>
       </c>
-      <c r="D52" t="s">
+      <c r="D52" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="E52" s="1">
-        <v>1</v>
-      </c>
-      <c r="F52" t="s">
+      <c r="E52" s="3">
+        <v>1</v>
+      </c>
+      <c r="F52" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="G52" s="1">
-        <v>1</v>
-      </c>
-      <c r="H52" t="s">
+      <c r="G52" s="3">
+        <v>1</v>
+      </c>
+      <c r="H52" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="I52" s="1" t="s">
+      <c r="I52" s="3" t="s">
         <v>94</v>
       </c>
+      <c r="J52" s="4"/>
+      <c r="K52" s="5"/>
     </row>
     <row r="53" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B53" t="str">
+      <c r="B53" s="6" t="str">
         <f t="shared" ref="B53:B58" si="10">_xlfn.CONCAT(TEXT(C53,"00"),TEXT(E53,"00"),TEXT(G53,"00"))</f>
         <v>100201</v>
       </c>
-      <c r="C53" s="1">
+      <c r="C53" s="13">
         <v>10</v>
       </c>
-      <c r="D53" t="s">
+      <c r="D53" s="14" t="s">
         <v>92</v>
       </c>
-      <c r="E53" s="1">
+      <c r="E53" s="13">
         <v>2</v>
       </c>
-      <c r="F53" t="s">
+      <c r="F53" s="14" t="s">
         <v>96</v>
       </c>
-      <c r="G53" s="1">
-        <v>1</v>
-      </c>
-      <c r="H53" t="s">
+      <c r="G53" s="13">
+        <v>1</v>
+      </c>
+      <c r="H53" s="14" t="s">
         <v>96</v>
       </c>
-      <c r="I53" t="s">
+      <c r="I53" s="14" t="s">
         <v>95</v>
       </c>
+      <c r="J53" s="14"/>
+      <c r="K53" s="7"/>
     </row>
     <row r="54" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B54" t="str">
+      <c r="B54" s="6" t="str">
         <f t="shared" si="10"/>
         <v>100301</v>
       </c>
-      <c r="C54" s="1">
+      <c r="C54" s="13">
         <v>10</v>
       </c>
-      <c r="D54" t="s">
+      <c r="D54" s="14" t="s">
         <v>92</v>
       </c>
-      <c r="E54" s="1">
+      <c r="E54" s="13">
         <v>3</v>
       </c>
-      <c r="F54" t="s">
+      <c r="F54" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="G54" s="1">
-        <v>1</v>
-      </c>
-      <c r="H54" t="s">
+      <c r="G54" s="13">
+        <v>1</v>
+      </c>
+      <c r="H54" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="I54" s="1" t="s">
+      <c r="I54" s="13" t="s">
         <v>98</v>
       </c>
+      <c r="J54" s="14"/>
+      <c r="K54" s="7"/>
     </row>
     <row r="55" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B55" t="str">
+      <c r="B55" s="6" t="str">
         <f t="shared" si="10"/>
         <v>100401</v>
       </c>
-      <c r="C55" s="1">
+      <c r="C55" s="13">
         <v>10</v>
       </c>
-      <c r="D55" t="s">
+      <c r="D55" s="14" t="s">
         <v>92</v>
       </c>
-      <c r="E55" s="1">
+      <c r="E55" s="13">
         <v>4</v>
       </c>
-      <c r="F55" t="s">
+      <c r="F55" s="14" t="s">
         <v>100</v>
       </c>
-      <c r="G55" s="1">
-        <v>1</v>
-      </c>
-      <c r="H55" t="s">
+      <c r="G55" s="13">
+        <v>1</v>
+      </c>
+      <c r="H55" s="14" t="s">
         <v>100</v>
       </c>
-      <c r="I55" s="1" t="s">
+      <c r="I55" s="13" t="s">
         <v>99</v>
       </c>
+      <c r="J55" s="14"/>
+      <c r="K55" s="7"/>
     </row>
     <row r="56" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B56" t="str">
+      <c r="B56" s="6" t="str">
         <f t="shared" si="10"/>
         <v>100501</v>
       </c>
-      <c r="C56" s="1">
+      <c r="C56" s="13">
         <v>10</v>
       </c>
-      <c r="D56" t="s">
+      <c r="D56" s="14" t="s">
         <v>92</v>
       </c>
-      <c r="E56" s="1">
-        <v>5</v>
-      </c>
-      <c r="F56" t="s">
+      <c r="E56" s="13">
+        <v>5</v>
+      </c>
+      <c r="F56" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="G56" s="1">
-        <v>1</v>
-      </c>
-      <c r="H56" t="s">
+      <c r="G56" s="13">
+        <v>1</v>
+      </c>
+      <c r="H56" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="I56" s="1" t="s">
+      <c r="I56" s="13" t="s">
         <v>102</v>
       </c>
+      <c r="J56" s="14"/>
+      <c r="K56" s="7"/>
     </row>
     <row r="57" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B57" t="str">
+      <c r="B57" s="6" t="str">
         <f t="shared" si="10"/>
         <v>100601</v>
       </c>
-      <c r="C57" s="1">
+      <c r="C57" s="13">
         <v>10</v>
       </c>
-      <c r="D57" t="s">
+      <c r="D57" s="14" t="s">
         <v>92</v>
       </c>
-      <c r="E57" s="1">
+      <c r="E57" s="13">
         <v>6</v>
       </c>
-      <c r="F57" t="s">
+      <c r="F57" s="14" t="s">
         <v>103</v>
       </c>
-      <c r="G57" s="1">
-        <v>1</v>
-      </c>
-      <c r="H57" t="s">
+      <c r="G57" s="13">
+        <v>1</v>
+      </c>
+      <c r="H57" s="14" t="s">
         <v>103</v>
       </c>
-      <c r="I57" s="1" t="s">
+      <c r="I57" s="13" t="s">
         <v>104</v>
       </c>
+      <c r="J57" s="14"/>
+      <c r="K57" s="7"/>
     </row>
     <row r="58" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B58" t="str">
+      <c r="B58" s="6" t="str">
         <f t="shared" si="10"/>
         <v>100701</v>
       </c>
-      <c r="C58" s="1">
+      <c r="C58" s="13">
         <v>10</v>
       </c>
-      <c r="D58" t="s">
+      <c r="D58" s="14" t="s">
         <v>92</v>
       </c>
-      <c r="E58" s="1">
+      <c r="E58" s="13">
         <v>7</v>
       </c>
-      <c r="F58" t="s">
+      <c r="F58" s="14" t="s">
         <v>105</v>
       </c>
-      <c r="G58" s="1">
-        <v>1</v>
-      </c>
-      <c r="H58" t="s">
+      <c r="G58" s="13">
+        <v>1</v>
+      </c>
+      <c r="H58" s="14" t="s">
         <v>105</v>
       </c>
-      <c r="I58" s="1" t="s">
+      <c r="I58" s="13" t="s">
         <v>106</v>
       </c>
+      <c r="J58" s="14"/>
+      <c r="K58" s="7"/>
     </row>
     <row r="59" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B59" t="str">
+      <c r="B59" s="8" t="str">
         <f t="shared" ref="B59" si="11">_xlfn.CONCAT(TEXT(C59,"00"),TEXT(E59,"00"),TEXT(G59,"00"))</f>
         <v>100801</v>
       </c>
-      <c r="C59" s="1">
+      <c r="C59" s="9">
         <v>10</v>
       </c>
-      <c r="D59" t="s">
+      <c r="D59" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="E59" s="1">
+      <c r="E59" s="9">
         <v>8</v>
       </c>
-      <c r="F59" t="s">
+      <c r="F59" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="G59" s="1">
-        <v>1</v>
-      </c>
-      <c r="H59" t="s">
+      <c r="G59" s="9">
+        <v>1</v>
+      </c>
+      <c r="H59" s="10" t="s">
         <v>107</v>
       </c>
+      <c r="I59" s="10"/>
+      <c r="J59" s="10"/>
+      <c r="K59" s="11"/>
+    </row>
+    <row r="60" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B60" s="2" t="str">
+        <f t="shared" ref="B60" si="12">_xlfn.CONCAT(TEXT(C60,"00"),TEXT(E60,"00"),TEXT(G60,"00"))</f>
+        <v>110101</v>
+      </c>
+      <c r="C60" s="3">
+        <v>11</v>
+      </c>
+      <c r="D60" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="E60" s="3">
+        <v>1</v>
+      </c>
+      <c r="F60" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="G60" s="3">
+        <v>1</v>
+      </c>
+      <c r="H60" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="I60" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="J60" s="4"/>
+      <c r="K60" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
Complete Ch 11 Handling hierarchies
</commit_message>
<xml_diff>
--- a/Definitive Guide to DAX/DAX Functions Covered.xlsx
+++ b/Definitive Guide to DAX/DAX Functions Covered.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github.com\open-word\DAX\Definitive Guide to DAX\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95CA6F14-3F7A-4050-8A51-E6926FFB12D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C620F47-53DD-41A7-A40C-BCC2AA8E4120}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="1680" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="18240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="113">
   <si>
     <t>CALCULATE</t>
   </si>
@@ -369,6 +369,12 @@
   </si>
   <si>
     <t>ALLSELECTED, ISINSCOPE</t>
+  </si>
+  <si>
+    <t>Handling parent-child hierarchies</t>
+  </si>
+  <si>
+    <t>PATH, PATHITEM, PATHLENGTH, LOOKUPVALUE, ISINSCOPE</t>
   </si>
 </sst>
 </file>
@@ -509,8 +515,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -791,10 +797,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:K60"/>
+  <dimension ref="B1:K61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B31" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I61" sqref="I61"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I53" sqref="I53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2132,28 +2138,27 @@
         <f t="shared" ref="B53:B58" si="10">_xlfn.CONCAT(TEXT(C53,"00"),TEXT(E53,"00"),TEXT(G53,"00"))</f>
         <v>100201</v>
       </c>
-      <c r="C53" s="13">
+      <c r="C53" s="1">
         <v>10</v>
       </c>
-      <c r="D53" s="14" t="s">
+      <c r="D53" t="s">
         <v>92</v>
       </c>
-      <c r="E53" s="13">
+      <c r="E53" s="1">
         <v>2</v>
       </c>
-      <c r="F53" s="14" t="s">
+      <c r="F53" t="s">
         <v>96</v>
       </c>
-      <c r="G53" s="13">
-        <v>1</v>
-      </c>
-      <c r="H53" s="14" t="s">
+      <c r="G53" s="1">
+        <v>1</v>
+      </c>
+      <c r="H53" t="s">
         <v>96</v>
       </c>
-      <c r="I53" s="14" t="s">
+      <c r="I53" t="s">
         <v>95</v>
       </c>
-      <c r="J53" s="14"/>
       <c r="K53" s="7"/>
     </row>
     <row r="54" spans="2:11" x14ac:dyDescent="0.25">
@@ -2161,28 +2166,27 @@
         <f t="shared" si="10"/>
         <v>100301</v>
       </c>
-      <c r="C54" s="13">
+      <c r="C54" s="1">
         <v>10</v>
       </c>
-      <c r="D54" s="14" t="s">
+      <c r="D54" t="s">
         <v>92</v>
       </c>
-      <c r="E54" s="13">
+      <c r="E54" s="1">
         <v>3</v>
       </c>
-      <c r="F54" s="14" t="s">
+      <c r="F54" t="s">
         <v>97</v>
       </c>
-      <c r="G54" s="13">
-        <v>1</v>
-      </c>
-      <c r="H54" s="14" t="s">
+      <c r="G54" s="1">
+        <v>1</v>
+      </c>
+      <c r="H54" t="s">
         <v>97</v>
       </c>
-      <c r="I54" s="13" t="s">
+      <c r="I54" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="J54" s="14"/>
       <c r="K54" s="7"/>
     </row>
     <row r="55" spans="2:11" x14ac:dyDescent="0.25">
@@ -2190,28 +2194,27 @@
         <f t="shared" si="10"/>
         <v>100401</v>
       </c>
-      <c r="C55" s="13">
+      <c r="C55" s="1">
         <v>10</v>
       </c>
-      <c r="D55" s="14" t="s">
+      <c r="D55" t="s">
         <v>92</v>
       </c>
-      <c r="E55" s="13">
+      <c r="E55" s="1">
         <v>4</v>
       </c>
-      <c r="F55" s="14" t="s">
+      <c r="F55" t="s">
         <v>100</v>
       </c>
-      <c r="G55" s="13">
-        <v>1</v>
-      </c>
-      <c r="H55" s="14" t="s">
+      <c r="G55" s="1">
+        <v>1</v>
+      </c>
+      <c r="H55" t="s">
         <v>100</v>
       </c>
-      <c r="I55" s="13" t="s">
+      <c r="I55" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="J55" s="14"/>
       <c r="K55" s="7"/>
     </row>
     <row r="56" spans="2:11" x14ac:dyDescent="0.25">
@@ -2219,28 +2222,27 @@
         <f t="shared" si="10"/>
         <v>100501</v>
       </c>
-      <c r="C56" s="13">
+      <c r="C56" s="1">
         <v>10</v>
       </c>
-      <c r="D56" s="14" t="s">
+      <c r="D56" t="s">
         <v>92</v>
       </c>
-      <c r="E56" s="13">
-        <v>5</v>
-      </c>
-      <c r="F56" s="14" t="s">
+      <c r="E56" s="1">
+        <v>5</v>
+      </c>
+      <c r="F56" t="s">
         <v>101</v>
       </c>
-      <c r="G56" s="13">
-        <v>1</v>
-      </c>
-      <c r="H56" s="14" t="s">
+      <c r="G56" s="1">
+        <v>1</v>
+      </c>
+      <c r="H56" t="s">
         <v>101</v>
       </c>
-      <c r="I56" s="13" t="s">
+      <c r="I56" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="J56" s="14"/>
       <c r="K56" s="7"/>
     </row>
     <row r="57" spans="2:11" x14ac:dyDescent="0.25">
@@ -2248,28 +2250,27 @@
         <f t="shared" si="10"/>
         <v>100601</v>
       </c>
-      <c r="C57" s="13">
+      <c r="C57" s="1">
         <v>10</v>
       </c>
-      <c r="D57" s="14" t="s">
+      <c r="D57" t="s">
         <v>92</v>
       </c>
-      <c r="E57" s="13">
+      <c r="E57" s="1">
         <v>6</v>
       </c>
-      <c r="F57" s="14" t="s">
+      <c r="F57" t="s">
         <v>103</v>
       </c>
-      <c r="G57" s="13">
-        <v>1</v>
-      </c>
-      <c r="H57" s="14" t="s">
+      <c r="G57" s="1">
+        <v>1</v>
+      </c>
+      <c r="H57" t="s">
         <v>103</v>
       </c>
-      <c r="I57" s="13" t="s">
+      <c r="I57" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="J57" s="14"/>
       <c r="K57" s="7"/>
     </row>
     <row r="58" spans="2:11" x14ac:dyDescent="0.25">
@@ -2277,28 +2278,27 @@
         <f t="shared" si="10"/>
         <v>100701</v>
       </c>
-      <c r="C58" s="13">
+      <c r="C58" s="1">
         <v>10</v>
       </c>
-      <c r="D58" s="14" t="s">
+      <c r="D58" t="s">
         <v>92</v>
       </c>
-      <c r="E58" s="13">
+      <c r="E58" s="1">
         <v>7</v>
       </c>
-      <c r="F58" s="14" t="s">
+      <c r="F58" t="s">
         <v>105</v>
       </c>
-      <c r="G58" s="13">
-        <v>1</v>
-      </c>
-      <c r="H58" s="14" t="s">
+      <c r="G58" s="1">
+        <v>1</v>
+      </c>
+      <c r="H58" t="s">
         <v>105</v>
       </c>
-      <c r="I58" s="13" t="s">
+      <c r="I58" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="J58" s="14"/>
       <c r="K58" s="7"/>
     </row>
     <row r="59" spans="2:11" x14ac:dyDescent="0.25">
@@ -2330,7 +2330,7 @@
     </row>
     <row r="60" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B60" s="2" t="str">
-        <f t="shared" ref="B60" si="12">_xlfn.CONCAT(TEXT(C60,"00"),TEXT(E60,"00"),TEXT(G60,"00"))</f>
+        <f t="shared" ref="B60:B61" si="12">_xlfn.CONCAT(TEXT(C60,"00"),TEXT(E60,"00"),TEXT(G60,"00"))</f>
         <v>110101</v>
       </c>
       <c r="C60" s="3">
@@ -2356,6 +2356,35 @@
       </c>
       <c r="J60" s="4"/>
       <c r="K60" s="5"/>
+    </row>
+    <row r="61" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B61" s="8" t="str">
+        <f t="shared" si="12"/>
+        <v>110201</v>
+      </c>
+      <c r="C61" s="13">
+        <v>11</v>
+      </c>
+      <c r="D61" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="E61" s="13">
+        <v>2</v>
+      </c>
+      <c r="F61" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="G61" s="13">
+        <v>1</v>
+      </c>
+      <c r="H61" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="I61" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="J61" s="10"/>
+      <c r="K61" s="11"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
Complete Ch 12 01 Using CALCULATETABLE
</commit_message>
<xml_diff>
--- a/Definitive Guide to DAX/DAX Functions Covered.xlsx
+++ b/Definitive Guide to DAX/DAX Functions Covered.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github.com\open-word\DAX\Definitive Guide to DAX\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C620F47-53DD-41A7-A40C-BCC2AA8E4120}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E2CB163-14D1-4F70-8C35-658332904781}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="18240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="1680" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="116">
   <si>
     <t>CALCULATE</t>
   </si>
@@ -375,6 +375,15 @@
   </si>
   <si>
     <t>PATH, PATHITEM, PATHLENGTH, LOOKUPVALUE, ISINSCOPE</t>
+  </si>
+  <si>
+    <t>Working with tables</t>
+  </si>
+  <si>
+    <t>Using CALCULATETABLE</t>
+  </si>
+  <si>
+    <t>CALCULATETABLE</t>
   </si>
 </sst>
 </file>
@@ -515,8 +524,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -797,10 +806,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:K61"/>
+  <dimension ref="B1:K62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I53" sqref="I53"/>
+    <sheetView tabSelected="1" topLeftCell="B37" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I62" sqref="I62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2330,7 +2339,7 @@
     </row>
     <row r="60" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B60" s="2" t="str">
-        <f t="shared" ref="B60:B61" si="12">_xlfn.CONCAT(TEXT(C60,"00"),TEXT(E60,"00"),TEXT(G60,"00"))</f>
+        <f t="shared" ref="B60:B62" si="12">_xlfn.CONCAT(TEXT(C60,"00"),TEXT(E60,"00"),TEXT(G60,"00"))</f>
         <v>110101</v>
       </c>
       <c r="C60" s="3">
@@ -2362,22 +2371,22 @@
         <f t="shared" si="12"/>
         <v>110201</v>
       </c>
-      <c r="C61" s="13">
+      <c r="C61" s="9">
         <v>11</v>
       </c>
-      <c r="D61" s="14" t="s">
+      <c r="D61" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="E61" s="13">
+      <c r="E61" s="9">
         <v>2</v>
       </c>
-      <c r="F61" s="14" t="s">
+      <c r="F61" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="G61" s="13">
-        <v>1</v>
-      </c>
-      <c r="H61" s="14" t="s">
+      <c r="G61" s="9">
+        <v>1</v>
+      </c>
+      <c r="H61" s="10" t="s">
         <v>111</v>
       </c>
       <c r="I61" s="9" t="s">
@@ -2385,6 +2394,33 @@
       </c>
       <c r="J61" s="10"/>
       <c r="K61" s="11"/>
+    </row>
+    <row r="62" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B62" t="str">
+        <f t="shared" si="12"/>
+        <v>120101</v>
+      </c>
+      <c r="C62" s="13">
+        <v>12</v>
+      </c>
+      <c r="D62" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="E62" s="13">
+        <v>1</v>
+      </c>
+      <c r="F62" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="G62" s="13">
+        <v>1</v>
+      </c>
+      <c r="H62" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="I62" s="13" t="s">
+        <v>115</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
Complete Ch 12 02 Manipulating tables
</commit_message>
<xml_diff>
--- a/Definitive Guide to DAX/DAX Functions Covered.xlsx
+++ b/Definitive Guide to DAX/DAX Functions Covered.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github.com\open-word\DAX\Definitive Guide to DAX\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E2CB163-14D1-4F70-8C35-658332904781}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2A9FEAB-4868-4823-91C6-0D074AD3824F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="1680" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="129">
   <si>
     <t>CALCULATE</t>
   </si>
@@ -384,6 +384,45 @@
   </si>
   <si>
     <t>CALCULATETABLE</t>
+  </si>
+  <si>
+    <t>Manipulating tables</t>
+  </si>
+  <si>
+    <t>Using ADDCOLUMNS</t>
+  </si>
+  <si>
+    <t>ADDCOLUMNS</t>
+  </si>
+  <si>
+    <t>Using SUMMARIZE</t>
+  </si>
+  <si>
+    <t>SUMMARIZE, ADDCOLUMNS</t>
+  </si>
+  <si>
+    <t>Using CROSSJOIN</t>
+  </si>
+  <si>
+    <t>CROSSJOIN</t>
+  </si>
+  <si>
+    <t>Using UNION</t>
+  </si>
+  <si>
+    <t>UNION</t>
+  </si>
+  <si>
+    <t>Using INTERCEPT</t>
+  </si>
+  <si>
+    <t>Using EXCEPT</t>
+  </si>
+  <si>
+    <t>INTERSECT</t>
+  </si>
+  <si>
+    <t>EXCEPT</t>
   </si>
 </sst>
 </file>
@@ -806,10 +845,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:K62"/>
+  <dimension ref="B1:K68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B37" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I62" sqref="I62"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F72" sqref="F72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2339,7 +2378,7 @@
     </row>
     <row r="60" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B60" s="2" t="str">
-        <f t="shared" ref="B60:B62" si="12">_xlfn.CONCAT(TEXT(C60,"00"),TEXT(E60,"00"),TEXT(G60,"00"))</f>
+        <f t="shared" ref="B60:B66" si="12">_xlfn.CONCAT(TEXT(C60,"00"),TEXT(E60,"00"),TEXT(G60,"00"))</f>
         <v>110101</v>
       </c>
       <c r="C60" s="3">
@@ -2420,6 +2459,168 @@
       </c>
       <c r="I62" s="13" t="s">
         <v>115</v>
+      </c>
+    </row>
+    <row r="63" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B63" t="str">
+        <f t="shared" si="12"/>
+        <v>120201</v>
+      </c>
+      <c r="C63" s="13">
+        <v>12</v>
+      </c>
+      <c r="D63" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="E63" s="13">
+        <v>2</v>
+      </c>
+      <c r="F63" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="G63" s="13">
+        <v>1</v>
+      </c>
+      <c r="H63" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="I63" s="13" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="64" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B64" t="str">
+        <f t="shared" si="12"/>
+        <v>120202</v>
+      </c>
+      <c r="C64" s="13">
+        <v>12</v>
+      </c>
+      <c r="D64" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="E64" s="13">
+        <v>2</v>
+      </c>
+      <c r="F64" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="G64" s="13">
+        <v>2</v>
+      </c>
+      <c r="H64" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="I64" s="13" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="65" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B65" t="str">
+        <f t="shared" si="12"/>
+        <v>120203</v>
+      </c>
+      <c r="C65" s="13">
+        <v>12</v>
+      </c>
+      <c r="D65" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="E65" s="13">
+        <v>2</v>
+      </c>
+      <c r="F65" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="G65" s="13">
+        <v>3</v>
+      </c>
+      <c r="H65" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="I65" s="13" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="66" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B66" t="str">
+        <f t="shared" si="12"/>
+        <v>120204</v>
+      </c>
+      <c r="C66" s="13">
+        <v>12</v>
+      </c>
+      <c r="D66" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="E66" s="13">
+        <v>2</v>
+      </c>
+      <c r="F66" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="G66" s="13">
+        <v>4</v>
+      </c>
+      <c r="H66" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="I66" s="13" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="67" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B67" t="str">
+        <f t="shared" ref="B67:B68" si="13">_xlfn.CONCAT(TEXT(C67,"00"),TEXT(E67,"00"),TEXT(G67,"00"))</f>
+        <v>120205</v>
+      </c>
+      <c r="C67" s="13">
+        <v>12</v>
+      </c>
+      <c r="D67" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="E67" s="13">
+        <v>2</v>
+      </c>
+      <c r="F67" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="G67" s="13">
+        <v>5</v>
+      </c>
+      <c r="H67" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="I67" s="13" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="68" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B68" t="str">
+        <f t="shared" si="13"/>
+        <v>120206</v>
+      </c>
+      <c r="C68" s="13">
+        <v>12</v>
+      </c>
+      <c r="D68" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="E68" s="13">
+        <v>2</v>
+      </c>
+      <c r="F68" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="G68" s="13">
+        <v>6</v>
+      </c>
+      <c r="H68" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="I68" s="13" t="s">
+        <v>128</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Complete Ch 12 03 Using tables as filters
</commit_message>
<xml_diff>
--- a/Definitive Guide to DAX/DAX Functions Covered.xlsx
+++ b/Definitive Guide to DAX/DAX Functions Covered.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github.com\open-word\DAX\Definitive Guide to DAX\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2A9FEAB-4868-4823-91C6-0D074AD3824F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D64DDC85-A7E6-41C7-B1EA-C653F0B18561}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="1680" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="137">
   <si>
     <t>CALCULATE</t>
   </si>
@@ -423,6 +423,30 @@
   </si>
   <si>
     <t>EXCEPT</t>
+  </si>
+  <si>
+    <t>SUMMARIZE, CROSSJOIN, CALCULATE</t>
+  </si>
+  <si>
+    <t>Using tables as filters</t>
+  </si>
+  <si>
+    <t>Implementing OR conditions</t>
+  </si>
+  <si>
+    <t>Narrowing sales computation to the first years customers</t>
+  </si>
+  <si>
+    <t>CALCULATETABLE, ALLSELECTED, FIRSTNONBLANK, KEEPFILTERS</t>
+  </si>
+  <si>
+    <t>Computing new customers</t>
+  </si>
+  <si>
+    <t>CALCULATETABLE, ADDCOLUMNS, VALUES, FILTER, COUNTROWS</t>
+  </si>
+  <si>
+    <t>Reusing table expressions with DETAILROWS</t>
   </si>
 </sst>
 </file>
@@ -547,7 +571,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -563,8 +587,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -845,10 +867,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:K68"/>
+  <dimension ref="B1:K73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F72" sqref="F72"/>
+    <sheetView tabSelected="1" topLeftCell="B37" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I72" sqref="I72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2439,25 +2461,25 @@
         <f t="shared" si="12"/>
         <v>120101</v>
       </c>
-      <c r="C62" s="13">
+      <c r="C62" s="1">
         <v>12</v>
       </c>
-      <c r="D62" s="14" t="s">
+      <c r="D62" t="s">
         <v>113</v>
       </c>
-      <c r="E62" s="13">
-        <v>1</v>
-      </c>
-      <c r="F62" s="14" t="s">
+      <c r="E62" s="1">
+        <v>1</v>
+      </c>
+      <c r="F62" t="s">
         <v>114</v>
       </c>
-      <c r="G62" s="13">
-        <v>1</v>
-      </c>
-      <c r="H62" s="14" t="s">
+      <c r="G62" s="1">
+        <v>1</v>
+      </c>
+      <c r="H62" t="s">
         <v>114</v>
       </c>
-      <c r="I62" s="13" t="s">
+      <c r="I62" s="1" t="s">
         <v>115</v>
       </c>
     </row>
@@ -2466,25 +2488,25 @@
         <f t="shared" si="12"/>
         <v>120201</v>
       </c>
-      <c r="C63" s="13">
+      <c r="C63" s="1">
         <v>12</v>
       </c>
-      <c r="D63" s="14" t="s">
+      <c r="D63" t="s">
         <v>113</v>
       </c>
-      <c r="E63" s="13">
+      <c r="E63" s="1">
         <v>2</v>
       </c>
-      <c r="F63" s="14" t="s">
+      <c r="F63" t="s">
         <v>116</v>
       </c>
-      <c r="G63" s="13">
-        <v>1</v>
-      </c>
-      <c r="H63" s="14" t="s">
+      <c r="G63" s="1">
+        <v>1</v>
+      </c>
+      <c r="H63" t="s">
         <v>117</v>
       </c>
-      <c r="I63" s="13" t="s">
+      <c r="I63" s="1" t="s">
         <v>118</v>
       </c>
     </row>
@@ -2493,25 +2515,25 @@
         <f t="shared" si="12"/>
         <v>120202</v>
       </c>
-      <c r="C64" s="13">
+      <c r="C64" s="1">
         <v>12</v>
       </c>
-      <c r="D64" s="14" t="s">
+      <c r="D64" t="s">
         <v>113</v>
       </c>
-      <c r="E64" s="13">
+      <c r="E64" s="1">
         <v>2</v>
       </c>
-      <c r="F64" s="14" t="s">
+      <c r="F64" t="s">
         <v>116</v>
       </c>
-      <c r="G64" s="13">
+      <c r="G64" s="1">
         <v>2</v>
       </c>
-      <c r="H64" s="14" t="s">
+      <c r="H64" t="s">
         <v>119</v>
       </c>
-      <c r="I64" s="13" t="s">
+      <c r="I64" s="1" t="s">
         <v>120</v>
       </c>
     </row>
@@ -2520,25 +2542,25 @@
         <f t="shared" si="12"/>
         <v>120203</v>
       </c>
-      <c r="C65" s="13">
+      <c r="C65" s="1">
         <v>12</v>
       </c>
-      <c r="D65" s="14" t="s">
+      <c r="D65" t="s">
         <v>113</v>
       </c>
-      <c r="E65" s="13">
+      <c r="E65" s="1">
         <v>2</v>
       </c>
-      <c r="F65" s="14" t="s">
+      <c r="F65" t="s">
         <v>116</v>
       </c>
-      <c r="G65" s="13">
+      <c r="G65" s="1">
         <v>3</v>
       </c>
-      <c r="H65" s="14" t="s">
+      <c r="H65" t="s">
         <v>121</v>
       </c>
-      <c r="I65" s="13" t="s">
+      <c r="I65" s="1" t="s">
         <v>122</v>
       </c>
     </row>
@@ -2547,52 +2569,52 @@
         <f t="shared" si="12"/>
         <v>120204</v>
       </c>
-      <c r="C66" s="13">
+      <c r="C66" s="1">
         <v>12</v>
       </c>
-      <c r="D66" s="14" t="s">
+      <c r="D66" t="s">
         <v>113</v>
       </c>
-      <c r="E66" s="13">
+      <c r="E66" s="1">
         <v>2</v>
       </c>
-      <c r="F66" s="14" t="s">
+      <c r="F66" t="s">
         <v>116</v>
       </c>
-      <c r="G66" s="13">
+      <c r="G66" s="1">
         <v>4</v>
       </c>
-      <c r="H66" s="14" t="s">
+      <c r="H66" t="s">
         <v>123</v>
       </c>
-      <c r="I66" s="13" t="s">
+      <c r="I66" s="1" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="67" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B67" t="str">
-        <f t="shared" ref="B67:B68" si="13">_xlfn.CONCAT(TEXT(C67,"00"),TEXT(E67,"00"),TEXT(G67,"00"))</f>
+        <f t="shared" ref="B67:B73" si="13">_xlfn.CONCAT(TEXT(C67,"00"),TEXT(E67,"00"),TEXT(G67,"00"))</f>
         <v>120205</v>
       </c>
-      <c r="C67" s="13">
+      <c r="C67" s="1">
         <v>12</v>
       </c>
-      <c r="D67" s="14" t="s">
+      <c r="D67" t="s">
         <v>113</v>
       </c>
-      <c r="E67" s="13">
+      <c r="E67" s="1">
         <v>2</v>
       </c>
-      <c r="F67" s="14" t="s">
+      <c r="F67" t="s">
         <v>116</v>
       </c>
-      <c r="G67" s="13">
+      <c r="G67" s="1">
         <v>5</v>
       </c>
-      <c r="H67" s="14" t="s">
+      <c r="H67" t="s">
         <v>125</v>
       </c>
-      <c r="I67" s="13" t="s">
+      <c r="I67" s="1" t="s">
         <v>127</v>
       </c>
     </row>
@@ -2601,26 +2623,143 @@
         <f t="shared" si="13"/>
         <v>120206</v>
       </c>
-      <c r="C68" s="13">
+      <c r="C68" s="1">
         <v>12</v>
       </c>
-      <c r="D68" s="14" t="s">
+      <c r="D68" t="s">
         <v>113</v>
       </c>
-      <c r="E68" s="13">
+      <c r="E68" s="1">
         <v>2</v>
       </c>
-      <c r="F68" s="14" t="s">
+      <c r="F68" t="s">
         <v>116</v>
       </c>
-      <c r="G68" s="13">
+      <c r="G68" s="1">
         <v>6</v>
       </c>
-      <c r="H68" s="14" t="s">
+      <c r="H68" t="s">
         <v>126</v>
       </c>
-      <c r="I68" s="13" t="s">
+      <c r="I68" s="1" t="s">
         <v>128</v>
+      </c>
+    </row>
+    <row r="69" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B69" t="str">
+        <f t="shared" si="13"/>
+        <v>120301</v>
+      </c>
+      <c r="C69" s="1">
+        <v>12</v>
+      </c>
+      <c r="D69" t="s">
+        <v>113</v>
+      </c>
+      <c r="E69" s="1">
+        <v>3</v>
+      </c>
+      <c r="F69" t="s">
+        <v>130</v>
+      </c>
+      <c r="G69" s="1">
+        <v>1</v>
+      </c>
+      <c r="H69" t="s">
+        <v>131</v>
+      </c>
+      <c r="I69" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="70" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B70" t="str">
+        <f t="shared" si="13"/>
+        <v>120302</v>
+      </c>
+      <c r="C70" s="1">
+        <v>12</v>
+      </c>
+      <c r="D70" t="s">
+        <v>113</v>
+      </c>
+      <c r="E70" s="1">
+        <v>3</v>
+      </c>
+      <c r="F70" t="s">
+        <v>130</v>
+      </c>
+      <c r="G70" s="1">
+        <v>2</v>
+      </c>
+      <c r="H70" t="s">
+        <v>132</v>
+      </c>
+      <c r="I70" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="71" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B71" t="str">
+        <f t="shared" si="13"/>
+        <v>120303</v>
+      </c>
+      <c r="C71" s="1">
+        <v>12</v>
+      </c>
+      <c r="D71" t="s">
+        <v>113</v>
+      </c>
+      <c r="E71" s="1">
+        <v>3</v>
+      </c>
+      <c r="F71" t="s">
+        <v>130</v>
+      </c>
+      <c r="G71" s="1">
+        <v>3</v>
+      </c>
+      <c r="H71" t="s">
+        <v>134</v>
+      </c>
+      <c r="I71" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="72" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B72" t="str">
+        <f t="shared" si="13"/>
+        <v>120304</v>
+      </c>
+      <c r="C72" s="1">
+        <v>12</v>
+      </c>
+      <c r="D72" t="s">
+        <v>113</v>
+      </c>
+      <c r="E72" s="1">
+        <v>3</v>
+      </c>
+      <c r="F72" t="s">
+        <v>130</v>
+      </c>
+      <c r="G72" s="1">
+        <v>4</v>
+      </c>
+      <c r="H72" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="73" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B73" t="str">
+        <f t="shared" si="13"/>
+        <v>120000</v>
+      </c>
+      <c r="C73" s="1">
+        <v>12</v>
+      </c>
+      <c r="D73" t="s">
+        <v>113</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Complete Ch 12 Working with tables
</commit_message>
<xml_diff>
--- a/Definitive Guide to DAX/DAX Functions Covered.xlsx
+++ b/Definitive Guide to DAX/DAX Functions Covered.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github.com\open-word\DAX\Definitive Guide to DAX\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D64DDC85-A7E6-41C7-B1EA-C653F0B18561}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B21BEF42-6E19-46C1-A6EC-B53B266191D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="146">
   <si>
     <t>CALCULATE</t>
   </si>
@@ -447,6 +447,33 @@
   </si>
   <si>
     <t>Reusing table expressions with DETAILROWS</t>
+  </si>
+  <si>
+    <t>Creating calculated tables</t>
+  </si>
+  <si>
+    <t>Using SELECTCOLUMNS</t>
+  </si>
+  <si>
+    <t>SELECTCOLUMNS</t>
+  </si>
+  <si>
+    <t>Creating static tables with ROW</t>
+  </si>
+  <si>
+    <t>ROW</t>
+  </si>
+  <si>
+    <t>Creating static tables with DATATABLE</t>
+  </si>
+  <si>
+    <t>DATATABLE</t>
+  </si>
+  <si>
+    <t>Using GENERATESERIES</t>
+  </si>
+  <si>
+    <t>GENERATESERIES</t>
   </si>
 </sst>
 </file>
@@ -571,7 +598,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -587,6 +614,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -867,23 +896,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:K73"/>
+  <dimension ref="B1:K76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B37" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I72" sqref="I72"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="44.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="62" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="66.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="63.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="31.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="51.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="48" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="3.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="67.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="3.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="70.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="104.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="35.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="57.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:11" x14ac:dyDescent="0.25">
@@ -2457,310 +2487,437 @@
       <c r="K61" s="11"/>
     </row>
     <row r="62" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B62" t="str">
+      <c r="B62" s="2" t="str">
         <f t="shared" si="12"/>
         <v>120101</v>
       </c>
-      <c r="C62" s="1">
+      <c r="C62" s="3">
         <v>12</v>
       </c>
-      <c r="D62" t="s">
+      <c r="D62" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="E62" s="1">
-        <v>1</v>
-      </c>
-      <c r="F62" t="s">
+      <c r="E62" s="3">
+        <v>1</v>
+      </c>
+      <c r="F62" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="G62" s="1">
-        <v>1</v>
-      </c>
-      <c r="H62" t="s">
+      <c r="G62" s="3">
+        <v>1</v>
+      </c>
+      <c r="H62" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="I62" s="1" t="s">
+      <c r="I62" s="3" t="s">
         <v>115</v>
       </c>
+      <c r="J62" s="4"/>
+      <c r="K62" s="5"/>
     </row>
     <row r="63" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B63" t="str">
+      <c r="B63" s="6" t="str">
         <f t="shared" si="12"/>
         <v>120201</v>
       </c>
-      <c r="C63" s="1">
+      <c r="C63" s="13">
         <v>12</v>
       </c>
-      <c r="D63" t="s">
+      <c r="D63" s="14" t="s">
         <v>113</v>
       </c>
-      <c r="E63" s="1">
+      <c r="E63" s="13">
         <v>2</v>
       </c>
-      <c r="F63" t="s">
+      <c r="F63" s="14" t="s">
         <v>116</v>
       </c>
-      <c r="G63" s="1">
-        <v>1</v>
-      </c>
-      <c r="H63" t="s">
+      <c r="G63" s="13">
+        <v>1</v>
+      </c>
+      <c r="H63" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="I63" s="1" t="s">
+      <c r="I63" s="13" t="s">
         <v>118</v>
       </c>
+      <c r="J63" s="14"/>
+      <c r="K63" s="7"/>
     </row>
     <row r="64" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B64" t="str">
+      <c r="B64" s="6" t="str">
         <f t="shared" si="12"/>
         <v>120202</v>
       </c>
-      <c r="C64" s="1">
+      <c r="C64" s="13">
         <v>12</v>
       </c>
-      <c r="D64" t="s">
+      <c r="D64" s="14" t="s">
         <v>113</v>
       </c>
-      <c r="E64" s="1">
+      <c r="E64" s="13">
         <v>2</v>
       </c>
-      <c r="F64" t="s">
+      <c r="F64" s="14" t="s">
         <v>116</v>
       </c>
-      <c r="G64" s="1">
+      <c r="G64" s="13">
         <v>2</v>
       </c>
-      <c r="H64" t="s">
+      <c r="H64" s="14" t="s">
         <v>119</v>
       </c>
-      <c r="I64" s="1" t="s">
+      <c r="I64" s="13" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="65" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B65" t="str">
+      <c r="J64" s="14"/>
+      <c r="K64" s="7"/>
+    </row>
+    <row r="65" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B65" s="6" t="str">
         <f t="shared" si="12"/>
         <v>120203</v>
       </c>
-      <c r="C65" s="1">
+      <c r="C65" s="13">
         <v>12</v>
       </c>
-      <c r="D65" t="s">
+      <c r="D65" s="14" t="s">
         <v>113</v>
       </c>
-      <c r="E65" s="1">
+      <c r="E65" s="13">
         <v>2</v>
       </c>
-      <c r="F65" t="s">
+      <c r="F65" s="14" t="s">
         <v>116</v>
       </c>
-      <c r="G65" s="1">
+      <c r="G65" s="13">
         <v>3</v>
       </c>
-      <c r="H65" t="s">
+      <c r="H65" s="14" t="s">
         <v>121</v>
       </c>
-      <c r="I65" s="1" t="s">
+      <c r="I65" s="13" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="66" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B66" t="str">
+      <c r="J65" s="14"/>
+      <c r="K65" s="7"/>
+    </row>
+    <row r="66" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B66" s="6" t="str">
         <f t="shared" si="12"/>
         <v>120204</v>
       </c>
-      <c r="C66" s="1">
+      <c r="C66" s="13">
         <v>12</v>
       </c>
-      <c r="D66" t="s">
+      <c r="D66" s="14" t="s">
         <v>113</v>
       </c>
-      <c r="E66" s="1">
+      <c r="E66" s="13">
         <v>2</v>
       </c>
-      <c r="F66" t="s">
+      <c r="F66" s="14" t="s">
         <v>116</v>
       </c>
-      <c r="G66" s="1">
+      <c r="G66" s="13">
         <v>4</v>
       </c>
-      <c r="H66" t="s">
+      <c r="H66" s="14" t="s">
         <v>123</v>
       </c>
-      <c r="I66" s="1" t="s">
+      <c r="I66" s="13" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="67" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B67" t="str">
+      <c r="J66" s="14"/>
+      <c r="K66" s="7"/>
+    </row>
+    <row r="67" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B67" s="6" t="str">
         <f t="shared" ref="B67:B73" si="13">_xlfn.CONCAT(TEXT(C67,"00"),TEXT(E67,"00"),TEXT(G67,"00"))</f>
         <v>120205</v>
       </c>
-      <c r="C67" s="1">
+      <c r="C67" s="13">
         <v>12</v>
       </c>
-      <c r="D67" t="s">
+      <c r="D67" s="14" t="s">
         <v>113</v>
       </c>
-      <c r="E67" s="1">
+      <c r="E67" s="13">
         <v>2</v>
       </c>
-      <c r="F67" t="s">
+      <c r="F67" s="14" t="s">
         <v>116</v>
       </c>
-      <c r="G67" s="1">
+      <c r="G67" s="13">
         <v>5</v>
       </c>
-      <c r="H67" t="s">
+      <c r="H67" s="14" t="s">
         <v>125</v>
       </c>
-      <c r="I67" s="1" t="s">
+      <c r="I67" s="13" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="68" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B68" t="str">
+      <c r="J67" s="14"/>
+      <c r="K67" s="7"/>
+    </row>
+    <row r="68" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B68" s="6" t="str">
         <f t="shared" si="13"/>
         <v>120206</v>
       </c>
-      <c r="C68" s="1">
+      <c r="C68" s="13">
         <v>12</v>
       </c>
-      <c r="D68" t="s">
+      <c r="D68" s="14" t="s">
         <v>113</v>
       </c>
-      <c r="E68" s="1">
+      <c r="E68" s="13">
         <v>2</v>
       </c>
-      <c r="F68" t="s">
+      <c r="F68" s="14" t="s">
         <v>116</v>
       </c>
-      <c r="G68" s="1">
+      <c r="G68" s="13">
         <v>6</v>
       </c>
-      <c r="H68" t="s">
+      <c r="H68" s="14" t="s">
         <v>126</v>
       </c>
-      <c r="I68" s="1" t="s">
+      <c r="I68" s="13" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="69" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B69" t="str">
+      <c r="J68" s="14"/>
+      <c r="K68" s="7"/>
+    </row>
+    <row r="69" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B69" s="6" t="str">
         <f t="shared" si="13"/>
         <v>120301</v>
       </c>
-      <c r="C69" s="1">
+      <c r="C69" s="13">
         <v>12</v>
       </c>
-      <c r="D69" t="s">
+      <c r="D69" s="14" t="s">
         <v>113</v>
       </c>
-      <c r="E69" s="1">
+      <c r="E69" s="13">
         <v>3</v>
       </c>
-      <c r="F69" t="s">
+      <c r="F69" s="14" t="s">
         <v>130</v>
       </c>
-      <c r="G69" s="1">
-        <v>1</v>
-      </c>
-      <c r="H69" t="s">
+      <c r="G69" s="13">
+        <v>1</v>
+      </c>
+      <c r="H69" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="I69" s="1" t="s">
+      <c r="I69" s="13" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="70" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B70" t="str">
+      <c r="J69" s="14"/>
+      <c r="K69" s="7"/>
+    </row>
+    <row r="70" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B70" s="6" t="str">
         <f t="shared" si="13"/>
         <v>120302</v>
       </c>
-      <c r="C70" s="1">
+      <c r="C70" s="13">
         <v>12</v>
       </c>
-      <c r="D70" t="s">
+      <c r="D70" s="14" t="s">
         <v>113</v>
       </c>
-      <c r="E70" s="1">
+      <c r="E70" s="13">
         <v>3</v>
       </c>
-      <c r="F70" t="s">
+      <c r="F70" s="14" t="s">
         <v>130</v>
       </c>
-      <c r="G70" s="1">
+      <c r="G70" s="13">
         <v>2</v>
       </c>
-      <c r="H70" t="s">
+      <c r="H70" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="I70" s="1" t="s">
+      <c r="I70" s="13" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="71" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B71" t="str">
+      <c r="J70" s="14"/>
+      <c r="K70" s="7"/>
+    </row>
+    <row r="71" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B71" s="6" t="str">
         <f t="shared" si="13"/>
         <v>120303</v>
       </c>
-      <c r="C71" s="1">
+      <c r="C71" s="13">
         <v>12</v>
       </c>
-      <c r="D71" t="s">
+      <c r="D71" s="14" t="s">
         <v>113</v>
       </c>
-      <c r="E71" s="1">
+      <c r="E71" s="13">
         <v>3</v>
       </c>
-      <c r="F71" t="s">
+      <c r="F71" s="14" t="s">
         <v>130</v>
       </c>
-      <c r="G71" s="1">
+      <c r="G71" s="13">
         <v>3</v>
       </c>
-      <c r="H71" t="s">
+      <c r="H71" s="14" t="s">
         <v>134</v>
       </c>
-      <c r="I71" s="1" t="s">
+      <c r="I71" s="13" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="72" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B72" t="str">
+      <c r="J71" s="14"/>
+      <c r="K71" s="7"/>
+    </row>
+    <row r="72" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B72" s="6" t="str">
         <f t="shared" si="13"/>
         <v>120304</v>
       </c>
-      <c r="C72" s="1">
+      <c r="C72" s="13">
         <v>12</v>
       </c>
-      <c r="D72" t="s">
+      <c r="D72" s="14" t="s">
         <v>113</v>
       </c>
-      <c r="E72" s="1">
+      <c r="E72" s="13">
         <v>3</v>
       </c>
-      <c r="F72" t="s">
+      <c r="F72" s="14" t="s">
         <v>130</v>
       </c>
-      <c r="G72" s="1">
+      <c r="G72" s="13">
         <v>4</v>
       </c>
-      <c r="H72" t="s">
+      <c r="H72" s="14" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="73" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B73" t="str">
+      <c r="I72" s="14"/>
+      <c r="J72" s="14"/>
+      <c r="K72" s="7"/>
+    </row>
+    <row r="73" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B73" s="6" t="str">
         <f t="shared" si="13"/>
-        <v>120000</v>
-      </c>
-      <c r="C73" s="1">
+        <v>120401</v>
+      </c>
+      <c r="C73" s="13">
         <v>12</v>
       </c>
-      <c r="D73" t="s">
+      <c r="D73" s="14" t="s">
         <v>113</v>
       </c>
+      <c r="E73" s="13">
+        <v>4</v>
+      </c>
+      <c r="F73" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="G73" s="13">
+        <v>1</v>
+      </c>
+      <c r="H73" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="I73" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="J73" s="14"/>
+      <c r="K73" s="7"/>
+    </row>
+    <row r="74" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B74" s="6" t="str">
+        <f t="shared" ref="B74:B76" si="14">_xlfn.CONCAT(TEXT(C74,"00"),TEXT(E74,"00"),TEXT(G74,"00"))</f>
+        <v>120402</v>
+      </c>
+      <c r="C74" s="13">
+        <v>12</v>
+      </c>
+      <c r="D74" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="E74" s="13">
+        <v>4</v>
+      </c>
+      <c r="F74" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="G74" s="13">
+        <v>2</v>
+      </c>
+      <c r="H74" s="14" t="s">
+        <v>140</v>
+      </c>
+      <c r="I74" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="J74" s="14"/>
+      <c r="K74" s="7"/>
+    </row>
+    <row r="75" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B75" s="6" t="str">
+        <f t="shared" si="14"/>
+        <v>120403</v>
+      </c>
+      <c r="C75" s="13">
+        <v>12</v>
+      </c>
+      <c r="D75" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="E75" s="13">
+        <v>4</v>
+      </c>
+      <c r="F75" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="G75" s="13">
+        <v>3</v>
+      </c>
+      <c r="H75" s="14" t="s">
+        <v>142</v>
+      </c>
+      <c r="I75" s="13" t="s">
+        <v>143</v>
+      </c>
+      <c r="J75" s="14"/>
+      <c r="K75" s="7"/>
+    </row>
+    <row r="76" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B76" s="8" t="str">
+        <f t="shared" si="14"/>
+        <v>120404</v>
+      </c>
+      <c r="C76" s="9">
+        <v>12</v>
+      </c>
+      <c r="D76" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="E76" s="9">
+        <v>4</v>
+      </c>
+      <c r="F76" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="G76" s="9">
+        <v>4</v>
+      </c>
+      <c r="H76" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="I76" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="J76" s="10"/>
+      <c r="K76" s="11"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
Complete Ch 13 02 Understanding EVALUATE
</commit_message>
<xml_diff>
--- a/Definitive Guide to DAX/DAX Functions Covered.xlsx
+++ b/Definitive Guide to DAX/DAX Functions Covered.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github.com\open-word\DAX\Definitive Guide to DAX\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B21BEF42-6E19-46C1-A6EC-B53B266191D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F434ED8-2065-4FDD-8189-F098CE1F22A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="156">
   <si>
     <t>CALCULATE</t>
   </si>
@@ -443,9 +443,6 @@
     <t>Computing new customers</t>
   </si>
   <si>
-    <t>CALCULATETABLE, ADDCOLUMNS, VALUES, FILTER, COUNTROWS</t>
-  </si>
-  <si>
     <t>Reusing table expressions with DETAILROWS</t>
   </si>
   <si>
@@ -474,6 +471,39 @@
   </si>
   <si>
     <t>GENERATESERIES</t>
+  </si>
+  <si>
+    <t>Authoring queries</t>
+  </si>
+  <si>
+    <t>Introducing DAX Studio</t>
+  </si>
+  <si>
+    <t>Understanding EVALUATE</t>
+  </si>
+  <si>
+    <t>Introducing the EVALUATE syntax</t>
+  </si>
+  <si>
+    <t>CALCULATETABLE, ADDCOLUMNS, VALUES, FILTER, COUNTROWS, DISTINCTCOUNT</t>
+  </si>
+  <si>
+    <t>DEFINE, EVALUATE, ORDER BY, ADDCOLUMNS, SUMMARIZE</t>
+  </si>
+  <si>
+    <t>Using VAR in DEFINE</t>
+  </si>
+  <si>
+    <t>Using MEASURE in DEFINE</t>
+  </si>
+  <si>
+    <t>VAR</t>
+  </si>
+  <si>
+    <t>MEASURE</t>
+  </si>
+  <si>
+    <t>Implementing common DAX query patterns</t>
   </si>
 </sst>
 </file>
@@ -598,7 +628,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -616,6 +646,8 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -896,10 +928,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:K76"/>
+  <dimension ref="B1:K89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D91" sqref="D91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2520,28 +2552,27 @@
         <f t="shared" si="12"/>
         <v>120201</v>
       </c>
-      <c r="C63" s="13">
+      <c r="C63" s="1">
         <v>12</v>
       </c>
-      <c r="D63" s="14" t="s">
+      <c r="D63" t="s">
         <v>113</v>
       </c>
-      <c r="E63" s="13">
+      <c r="E63" s="1">
         <v>2</v>
       </c>
-      <c r="F63" s="14" t="s">
+      <c r="F63" t="s">
         <v>116</v>
       </c>
-      <c r="G63" s="13">
-        <v>1</v>
-      </c>
-      <c r="H63" s="14" t="s">
+      <c r="G63" s="1">
+        <v>1</v>
+      </c>
+      <c r="H63" t="s">
         <v>117</v>
       </c>
-      <c r="I63" s="13" t="s">
+      <c r="I63" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="J63" s="14"/>
       <c r="K63" s="7"/>
     </row>
     <row r="64" spans="2:11" x14ac:dyDescent="0.25">
@@ -2549,28 +2580,27 @@
         <f t="shared" si="12"/>
         <v>120202</v>
       </c>
-      <c r="C64" s="13">
+      <c r="C64" s="1">
         <v>12</v>
       </c>
-      <c r="D64" s="14" t="s">
+      <c r="D64" t="s">
         <v>113</v>
       </c>
-      <c r="E64" s="13">
+      <c r="E64" s="1">
         <v>2</v>
       </c>
-      <c r="F64" s="14" t="s">
+      <c r="F64" t="s">
         <v>116</v>
       </c>
-      <c r="G64" s="13">
+      <c r="G64" s="1">
         <v>2</v>
       </c>
-      <c r="H64" s="14" t="s">
+      <c r="H64" t="s">
         <v>119</v>
       </c>
-      <c r="I64" s="13" t="s">
+      <c r="I64" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="J64" s="14"/>
       <c r="K64" s="7"/>
     </row>
     <row r="65" spans="2:11" x14ac:dyDescent="0.25">
@@ -2578,28 +2608,27 @@
         <f t="shared" si="12"/>
         <v>120203</v>
       </c>
-      <c r="C65" s="13">
+      <c r="C65" s="1">
         <v>12</v>
       </c>
-      <c r="D65" s="14" t="s">
+      <c r="D65" t="s">
         <v>113</v>
       </c>
-      <c r="E65" s="13">
+      <c r="E65" s="1">
         <v>2</v>
       </c>
-      <c r="F65" s="14" t="s">
+      <c r="F65" t="s">
         <v>116</v>
       </c>
-      <c r="G65" s="13">
+      <c r="G65" s="1">
         <v>3</v>
       </c>
-      <c r="H65" s="14" t="s">
+      <c r="H65" t="s">
         <v>121</v>
       </c>
-      <c r="I65" s="13" t="s">
+      <c r="I65" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="J65" s="14"/>
       <c r="K65" s="7"/>
     </row>
     <row r="66" spans="2:11" x14ac:dyDescent="0.25">
@@ -2607,28 +2636,27 @@
         <f t="shared" si="12"/>
         <v>120204</v>
       </c>
-      <c r="C66" s="13">
+      <c r="C66" s="1">
         <v>12</v>
       </c>
-      <c r="D66" s="14" t="s">
+      <c r="D66" t="s">
         <v>113</v>
       </c>
-      <c r="E66" s="13">
+      <c r="E66" s="1">
         <v>2</v>
       </c>
-      <c r="F66" s="14" t="s">
+      <c r="F66" t="s">
         <v>116</v>
       </c>
-      <c r="G66" s="13">
+      <c r="G66" s="1">
         <v>4</v>
       </c>
-      <c r="H66" s="14" t="s">
+      <c r="H66" t="s">
         <v>123</v>
       </c>
-      <c r="I66" s="13" t="s">
+      <c r="I66" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="J66" s="14"/>
       <c r="K66" s="7"/>
     </row>
     <row r="67" spans="2:11" x14ac:dyDescent="0.25">
@@ -2636,28 +2664,27 @@
         <f t="shared" ref="B67:B73" si="13">_xlfn.CONCAT(TEXT(C67,"00"),TEXT(E67,"00"),TEXT(G67,"00"))</f>
         <v>120205</v>
       </c>
-      <c r="C67" s="13">
+      <c r="C67" s="1">
         <v>12</v>
       </c>
-      <c r="D67" s="14" t="s">
+      <c r="D67" t="s">
         <v>113</v>
       </c>
-      <c r="E67" s="13">
+      <c r="E67" s="1">
         <v>2</v>
       </c>
-      <c r="F67" s="14" t="s">
+      <c r="F67" t="s">
         <v>116</v>
       </c>
-      <c r="G67" s="13">
+      <c r="G67" s="1">
         <v>5</v>
       </c>
-      <c r="H67" s="14" t="s">
+      <c r="H67" t="s">
         <v>125</v>
       </c>
-      <c r="I67" s="13" t="s">
+      <c r="I67" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="J67" s="14"/>
       <c r="K67" s="7"/>
     </row>
     <row r="68" spans="2:11" x14ac:dyDescent="0.25">
@@ -2665,28 +2692,27 @@
         <f t="shared" si="13"/>
         <v>120206</v>
       </c>
-      <c r="C68" s="13">
+      <c r="C68" s="1">
         <v>12</v>
       </c>
-      <c r="D68" s="14" t="s">
+      <c r="D68" t="s">
         <v>113</v>
       </c>
-      <c r="E68" s="13">
+      <c r="E68" s="1">
         <v>2</v>
       </c>
-      <c r="F68" s="14" t="s">
+      <c r="F68" t="s">
         <v>116</v>
       </c>
-      <c r="G68" s="13">
+      <c r="G68" s="1">
         <v>6</v>
       </c>
-      <c r="H68" s="14" t="s">
+      <c r="H68" t="s">
         <v>126</v>
       </c>
-      <c r="I68" s="13" t="s">
+      <c r="I68" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="J68" s="14"/>
       <c r="K68" s="7"/>
     </row>
     <row r="69" spans="2:11" x14ac:dyDescent="0.25">
@@ -2694,28 +2720,27 @@
         <f t="shared" si="13"/>
         <v>120301</v>
       </c>
-      <c r="C69" s="13">
+      <c r="C69" s="1">
         <v>12</v>
       </c>
-      <c r="D69" s="14" t="s">
+      <c r="D69" t="s">
         <v>113</v>
       </c>
-      <c r="E69" s="13">
+      <c r="E69" s="1">
         <v>3</v>
       </c>
-      <c r="F69" s="14" t="s">
+      <c r="F69" t="s">
         <v>130</v>
       </c>
-      <c r="G69" s="13">
-        <v>1</v>
-      </c>
-      <c r="H69" s="14" t="s">
+      <c r="G69" s="1">
+        <v>1</v>
+      </c>
+      <c r="H69" t="s">
         <v>131</v>
       </c>
-      <c r="I69" s="13" t="s">
+      <c r="I69" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="J69" s="14"/>
       <c r="K69" s="7"/>
     </row>
     <row r="70" spans="2:11" x14ac:dyDescent="0.25">
@@ -2723,28 +2748,27 @@
         <f t="shared" si="13"/>
         <v>120302</v>
       </c>
-      <c r="C70" s="13">
+      <c r="C70" s="1">
         <v>12</v>
       </c>
-      <c r="D70" s="14" t="s">
+      <c r="D70" t="s">
         <v>113</v>
       </c>
-      <c r="E70" s="13">
+      <c r="E70" s="1">
         <v>3</v>
       </c>
-      <c r="F70" s="14" t="s">
+      <c r="F70" t="s">
         <v>130</v>
       </c>
-      <c r="G70" s="13">
+      <c r="G70" s="1">
         <v>2</v>
       </c>
-      <c r="H70" s="14" t="s">
+      <c r="H70" t="s">
         <v>132</v>
       </c>
-      <c r="I70" s="13" t="s">
+      <c r="I70" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="J70" s="14"/>
       <c r="K70" s="7"/>
     </row>
     <row r="71" spans="2:11" x14ac:dyDescent="0.25">
@@ -2752,28 +2776,27 @@
         <f t="shared" si="13"/>
         <v>120303</v>
       </c>
-      <c r="C71" s="13">
+      <c r="C71" s="1">
         <v>12</v>
       </c>
-      <c r="D71" s="14" t="s">
+      <c r="D71" t="s">
         <v>113</v>
       </c>
-      <c r="E71" s="13">
+      <c r="E71" s="1">
         <v>3</v>
       </c>
-      <c r="F71" s="14" t="s">
+      <c r="F71" t="s">
         <v>130</v>
       </c>
-      <c r="G71" s="13">
+      <c r="G71" s="1">
         <v>3</v>
       </c>
-      <c r="H71" s="14" t="s">
+      <c r="H71" t="s">
         <v>134</v>
       </c>
-      <c r="I71" s="13" t="s">
-        <v>135</v>
-      </c>
-      <c r="J71" s="14"/>
+      <c r="I71" s="1" t="s">
+        <v>149</v>
+      </c>
       <c r="K71" s="7"/>
     </row>
     <row r="72" spans="2:11" x14ac:dyDescent="0.25">
@@ -2781,26 +2804,24 @@
         <f t="shared" si="13"/>
         <v>120304</v>
       </c>
-      <c r="C72" s="13">
+      <c r="C72" s="1">
         <v>12</v>
       </c>
-      <c r="D72" s="14" t="s">
+      <c r="D72" t="s">
         <v>113</v>
       </c>
-      <c r="E72" s="13">
+      <c r="E72" s="1">
         <v>3</v>
       </c>
-      <c r="F72" s="14" t="s">
+      <c r="F72" t="s">
         <v>130</v>
       </c>
-      <c r="G72" s="13">
+      <c r="G72" s="1">
         <v>4</v>
       </c>
-      <c r="H72" s="14" t="s">
-        <v>136</v>
-      </c>
-      <c r="I72" s="14"/>
-      <c r="J72" s="14"/>
+      <c r="H72" t="s">
+        <v>135</v>
+      </c>
       <c r="K72" s="7"/>
     </row>
     <row r="73" spans="2:11" x14ac:dyDescent="0.25">
@@ -2808,28 +2829,27 @@
         <f t="shared" si="13"/>
         <v>120401</v>
       </c>
-      <c r="C73" s="13">
+      <c r="C73" s="1">
         <v>12</v>
       </c>
-      <c r="D73" s="14" t="s">
+      <c r="D73" t="s">
         <v>113</v>
       </c>
-      <c r="E73" s="13">
+      <c r="E73" s="1">
         <v>4</v>
       </c>
-      <c r="F73" s="14" t="s">
+      <c r="F73" t="s">
+        <v>136</v>
+      </c>
+      <c r="G73" s="1">
+        <v>1</v>
+      </c>
+      <c r="H73" t="s">
         <v>137</v>
       </c>
-      <c r="G73" s="13">
-        <v>1</v>
-      </c>
-      <c r="H73" s="14" t="s">
+      <c r="I73" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="I73" s="13" t="s">
-        <v>139</v>
-      </c>
-      <c r="J73" s="14"/>
       <c r="K73" s="7"/>
     </row>
     <row r="74" spans="2:11" x14ac:dyDescent="0.25">
@@ -2837,28 +2857,27 @@
         <f t="shared" ref="B74:B76" si="14">_xlfn.CONCAT(TEXT(C74,"00"),TEXT(E74,"00"),TEXT(G74,"00"))</f>
         <v>120402</v>
       </c>
-      <c r="C74" s="13">
+      <c r="C74" s="1">
         <v>12</v>
       </c>
-      <c r="D74" s="14" t="s">
+      <c r="D74" t="s">
         <v>113</v>
       </c>
-      <c r="E74" s="13">
+      <c r="E74" s="1">
         <v>4</v>
       </c>
-      <c r="F74" s="14" t="s">
-        <v>137</v>
-      </c>
-      <c r="G74" s="13">
+      <c r="F74" t="s">
+        <v>136</v>
+      </c>
+      <c r="G74" s="1">
         <v>2</v>
       </c>
-      <c r="H74" s="14" t="s">
+      <c r="H74" t="s">
+        <v>139</v>
+      </c>
+      <c r="I74" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="I74" s="13" t="s">
-        <v>141</v>
-      </c>
-      <c r="J74" s="14"/>
       <c r="K74" s="7"/>
     </row>
     <row r="75" spans="2:11" x14ac:dyDescent="0.25">
@@ -2866,28 +2885,27 @@
         <f t="shared" si="14"/>
         <v>120403</v>
       </c>
-      <c r="C75" s="13">
+      <c r="C75" s="1">
         <v>12</v>
       </c>
-      <c r="D75" s="14" t="s">
+      <c r="D75" t="s">
         <v>113</v>
       </c>
-      <c r="E75" s="13">
+      <c r="E75" s="1">
         <v>4</v>
       </c>
-      <c r="F75" s="14" t="s">
-        <v>137</v>
-      </c>
-      <c r="G75" s="13">
+      <c r="F75" t="s">
+        <v>136</v>
+      </c>
+      <c r="G75" s="1">
         <v>3</v>
       </c>
-      <c r="H75" s="14" t="s">
+      <c r="H75" t="s">
+        <v>141</v>
+      </c>
+      <c r="I75" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="I75" s="13" t="s">
-        <v>143</v>
-      </c>
-      <c r="J75" s="14"/>
       <c r="K75" s="7"/>
     </row>
     <row r="76" spans="2:11" x14ac:dyDescent="0.25">
@@ -2905,19 +2923,267 @@
         <v>4</v>
       </c>
       <c r="F76" s="10" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G76" s="9">
         <v>4</v>
       </c>
       <c r="H76" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="I76" s="9" t="s">
         <v>144</v>
-      </c>
-      <c r="I76" s="9" t="s">
-        <v>145</v>
       </c>
       <c r="J76" s="10"/>
       <c r="K76" s="11"/>
+    </row>
+    <row r="77" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B77" s="2" t="str">
+        <f t="shared" ref="B77:B88" si="15">_xlfn.CONCAT(TEXT(C77,"00"),TEXT(E77,"00"),TEXT(G77,"00"))</f>
+        <v>130101</v>
+      </c>
+      <c r="C77" s="3">
+        <v>13</v>
+      </c>
+      <c r="D77" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="E77" s="3">
+        <v>1</v>
+      </c>
+      <c r="F77" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="G77" s="3">
+        <v>1</v>
+      </c>
+      <c r="H77" s="4" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="78" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B78" s="6" t="str">
+        <f t="shared" si="15"/>
+        <v>130201</v>
+      </c>
+      <c r="C78" s="13">
+        <v>13</v>
+      </c>
+      <c r="D78" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="E78" s="13">
+        <v>2</v>
+      </c>
+      <c r="F78" s="15" t="s">
+        <v>147</v>
+      </c>
+      <c r="G78" s="13">
+        <v>1</v>
+      </c>
+      <c r="H78" s="15" t="s">
+        <v>148</v>
+      </c>
+      <c r="I78" s="16" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="79" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B79" s="6" t="str">
+        <f t="shared" si="15"/>
+        <v>130202</v>
+      </c>
+      <c r="C79" s="13">
+        <v>13</v>
+      </c>
+      <c r="D79" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="E79" s="13">
+        <v>2</v>
+      </c>
+      <c r="F79" s="15" t="s">
+        <v>147</v>
+      </c>
+      <c r="G79" s="13">
+        <v>2</v>
+      </c>
+      <c r="H79" s="15" t="s">
+        <v>151</v>
+      </c>
+      <c r="I79" s="16" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="80" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B80" s="6" t="str">
+        <f t="shared" si="15"/>
+        <v>130203</v>
+      </c>
+      <c r="C80" s="13">
+        <v>13</v>
+      </c>
+      <c r="D80" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="E80" s="13">
+        <v>2</v>
+      </c>
+      <c r="F80" s="15" t="s">
+        <v>147</v>
+      </c>
+      <c r="G80" s="13">
+        <v>3</v>
+      </c>
+      <c r="H80" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="I80" s="16" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="81" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B81" s="6" t="str">
+        <f t="shared" si="15"/>
+        <v>130301</v>
+      </c>
+      <c r="C81" s="13">
+        <v>13</v>
+      </c>
+      <c r="D81" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="E81" s="13">
+        <v>3</v>
+      </c>
+      <c r="F81" s="15" t="s">
+        <v>155</v>
+      </c>
+      <c r="G81" s="13">
+        <v>1</v>
+      </c>
+      <c r="H81" s="14"/>
+    </row>
+    <row r="82" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B82" s="6" t="str">
+        <f t="shared" si="15"/>
+        <v>130000</v>
+      </c>
+      <c r="C82" s="13">
+        <v>13</v>
+      </c>
+      <c r="D82" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="E82" s="13"/>
+      <c r="F82" s="14"/>
+      <c r="G82" s="13"/>
+      <c r="H82" s="14"/>
+    </row>
+    <row r="83" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B83" s="6" t="str">
+        <f t="shared" si="15"/>
+        <v>130000</v>
+      </c>
+      <c r="C83" s="13">
+        <v>13</v>
+      </c>
+      <c r="D83" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="E83" s="13"/>
+      <c r="F83" s="14"/>
+      <c r="G83" s="13"/>
+      <c r="H83" s="14"/>
+    </row>
+    <row r="84" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B84" s="6" t="str">
+        <f t="shared" si="15"/>
+        <v>130000</v>
+      </c>
+      <c r="C84" s="13">
+        <v>13</v>
+      </c>
+      <c r="D84" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="E84" s="13"/>
+      <c r="F84" s="14"/>
+      <c r="G84" s="13"/>
+      <c r="H84" s="14"/>
+    </row>
+    <row r="85" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B85" s="6" t="str">
+        <f t="shared" si="15"/>
+        <v>130000</v>
+      </c>
+      <c r="C85" s="13">
+        <v>13</v>
+      </c>
+      <c r="D85" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="E85" s="13"/>
+      <c r="F85" s="14"/>
+      <c r="G85" s="13"/>
+      <c r="H85" s="14"/>
+    </row>
+    <row r="86" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B86" s="6" t="str">
+        <f t="shared" si="15"/>
+        <v>130000</v>
+      </c>
+      <c r="C86" s="13">
+        <v>13</v>
+      </c>
+      <c r="D86" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="E86" s="13"/>
+      <c r="F86" s="14"/>
+      <c r="G86" s="13"/>
+      <c r="H86" s="14"/>
+    </row>
+    <row r="87" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B87" s="6" t="str">
+        <f t="shared" si="15"/>
+        <v>130000</v>
+      </c>
+      <c r="C87" s="13">
+        <v>13</v>
+      </c>
+      <c r="D87" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="E87" s="13"/>
+      <c r="F87" s="14"/>
+      <c r="G87" s="13"/>
+      <c r="H87" s="14"/>
+    </row>
+    <row r="88" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B88" s="6" t="str">
+        <f t="shared" si="15"/>
+        <v>130000</v>
+      </c>
+      <c r="C88" s="13">
+        <v>13</v>
+      </c>
+      <c r="D88" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="E88" s="13"/>
+      <c r="F88" s="14"/>
+      <c r="G88" s="13"/>
+      <c r="H88" s="14"/>
+    </row>
+    <row r="89" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B89" s="6"/>
+      <c r="C89" s="14"/>
+      <c r="D89" s="14"/>
+      <c r="E89" s="14"/>
+      <c r="F89" s="14"/>
+      <c r="G89" s="14"/>
+      <c r="H89" s="14"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
Complete Ch 13 03 Implementing common DAX query patterns
</commit_message>
<xml_diff>
--- a/Definitive Guide to DAX/DAX Functions Covered.xlsx
+++ b/Definitive Guide to DAX/DAX Functions Covered.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github.com\open-word\DAX\Definitive Guide to DAX\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F434ED8-2065-4FDD-8189-F098CE1F22A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCEBD6D8-812D-4311-A0AE-ECED968B2C24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28800" yWindow="0" windowWidth="17775" windowHeight="16200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="179">
   <si>
     <t>CALCULATE</t>
   </si>
@@ -504,6 +504,75 @@
   </si>
   <si>
     <t>Implementing common DAX query patterns</t>
+  </si>
+  <si>
+    <t>Using ROW to test measures</t>
+  </si>
+  <si>
+    <t>ROW, CALCULATETABLE</t>
+  </si>
+  <si>
+    <t>SUMMARIZE</t>
+  </si>
+  <si>
+    <t>SUMMARIZECOLUMNS, ROLLUPADDISSUBTOTAL, ROLLUPGROUP, FILTER</t>
+  </si>
+  <si>
+    <t>Using TOPN</t>
+  </si>
+  <si>
+    <t>Using SUMMARIZECOLUMNS</t>
+  </si>
+  <si>
+    <t>TOPN</t>
+  </si>
+  <si>
+    <t>Using GENERATE and GENERATEALL</t>
+  </si>
+  <si>
+    <t>Using ISONORAFTER</t>
+  </si>
+  <si>
+    <t>ISONORAFTER</t>
+  </si>
+  <si>
+    <t>GENERATE, GENERATEALL</t>
+  </si>
+  <si>
+    <t>Using ADDMISSINGITEMS</t>
+  </si>
+  <si>
+    <t>ADDMISSINGITEMS</t>
+  </si>
+  <si>
+    <t>Using TOPNSKIP</t>
+  </si>
+  <si>
+    <t>TOPNSKIP</t>
+  </si>
+  <si>
+    <t>GROUPBY</t>
+  </si>
+  <si>
+    <t>Using GROUBY</t>
+  </si>
+  <si>
+    <t>NATURALINNERJOIN, NATURALLEFTOUTERJOIN</t>
+  </si>
+  <si>
+    <t>Using SUBSTITUTEWITHINDEX</t>
+  </si>
+  <si>
+    <t>Using NATURALINNERJOIN and NATURALLEFTOUTERJOIN</t>
+  </si>
+  <si>
+    <t>SUBSTITUTEWITHINDEX</t>
+  </si>
+  <si>
+    <t>Using SAMPLE</t>
+  </si>
+  <si>
+    <t>SAMPLE</t>
   </si>
 </sst>
 </file>
@@ -928,10 +997,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:K89"/>
+  <dimension ref="B1:K92"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A46" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D91" sqref="D91"/>
+      <selection activeCell="I93" sqref="I93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3042,7 +3111,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="81" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B81" s="6" t="str">
         <f t="shared" si="15"/>
         <v>130301</v>
@@ -3062,12 +3131,17 @@
       <c r="G81" s="13">
         <v>1</v>
       </c>
-      <c r="H81" s="14"/>
-    </row>
-    <row r="82" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H81" s="15" t="s">
+        <v>156</v>
+      </c>
+      <c r="I81" s="16" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="82" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B82" s="6" t="str">
         <f t="shared" si="15"/>
-        <v>130000</v>
+        <v>130302</v>
       </c>
       <c r="C82" s="13">
         <v>13</v>
@@ -3075,15 +3149,26 @@
       <c r="D82" s="15" t="s">
         <v>145</v>
       </c>
-      <c r="E82" s="13"/>
-      <c r="F82" s="14"/>
-      <c r="G82" s="13"/>
-      <c r="H82" s="14"/>
-    </row>
-    <row r="83" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E82" s="13">
+        <v>3</v>
+      </c>
+      <c r="F82" s="15" t="s">
+        <v>155</v>
+      </c>
+      <c r="G82" s="13">
+        <v>2</v>
+      </c>
+      <c r="H82" s="15" t="s">
+        <v>119</v>
+      </c>
+      <c r="I82" s="16" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="83" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B83" s="6" t="str">
         <f t="shared" si="15"/>
-        <v>130000</v>
+        <v>130303</v>
       </c>
       <c r="C83" s="13">
         <v>13</v>
@@ -3091,15 +3176,26 @@
       <c r="D83" s="15" t="s">
         <v>145</v>
       </c>
-      <c r="E83" s="13"/>
-      <c r="F83" s="14"/>
-      <c r="G83" s="13"/>
-      <c r="H83" s="14"/>
-    </row>
-    <row r="84" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E83" s="13">
+        <v>3</v>
+      </c>
+      <c r="F83" s="15" t="s">
+        <v>155</v>
+      </c>
+      <c r="G83" s="13">
+        <v>3</v>
+      </c>
+      <c r="H83" s="15" t="s">
+        <v>161</v>
+      </c>
+      <c r="I83" s="16" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="84" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B84" s="6" t="str">
         <f t="shared" si="15"/>
-        <v>130000</v>
+        <v>130304</v>
       </c>
       <c r="C84" s="13">
         <v>13</v>
@@ -3107,15 +3203,26 @@
       <c r="D84" s="15" t="s">
         <v>145</v>
       </c>
-      <c r="E84" s="13"/>
-      <c r="F84" s="14"/>
-      <c r="G84" s="13"/>
-      <c r="H84" s="14"/>
-    </row>
-    <row r="85" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E84" s="13">
+        <v>3</v>
+      </c>
+      <c r="F84" s="15" t="s">
+        <v>155</v>
+      </c>
+      <c r="G84" s="13">
+        <v>4</v>
+      </c>
+      <c r="H84" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="I84" s="16" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="85" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B85" s="6" t="str">
         <f t="shared" si="15"/>
-        <v>130000</v>
+        <v>130005</v>
       </c>
       <c r="C85" s="13">
         <v>13</v>
@@ -3125,13 +3232,20 @@
       </c>
       <c r="E85" s="13"/>
       <c r="F85" s="14"/>
-      <c r="G85" s="13"/>
-      <c r="H85" s="14"/>
-    </row>
-    <row r="86" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="G85" s="13">
+        <v>5</v>
+      </c>
+      <c r="H85" s="15" t="s">
+        <v>163</v>
+      </c>
+      <c r="I85" s="16" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="86" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B86" s="6" t="str">
         <f t="shared" si="15"/>
-        <v>130000</v>
+        <v>130006</v>
       </c>
       <c r="C86" s="13">
         <v>13</v>
@@ -3141,13 +3255,20 @@
       </c>
       <c r="E86" s="13"/>
       <c r="F86" s="14"/>
-      <c r="G86" s="13"/>
-      <c r="H86" s="14"/>
-    </row>
-    <row r="87" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="G86" s="13">
+        <v>6</v>
+      </c>
+      <c r="H86" s="15" t="s">
+        <v>164</v>
+      </c>
+      <c r="I86" s="16" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="87" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B87" s="6" t="str">
         <f t="shared" si="15"/>
-        <v>130000</v>
+        <v>130007</v>
       </c>
       <c r="C87" s="13">
         <v>13</v>
@@ -3157,13 +3278,20 @@
       </c>
       <c r="E87" s="13"/>
       <c r="F87" s="14"/>
-      <c r="G87" s="13"/>
-      <c r="H87" s="14"/>
-    </row>
-    <row r="88" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="G87" s="13">
+        <v>7</v>
+      </c>
+      <c r="H87" s="15" t="s">
+        <v>167</v>
+      </c>
+      <c r="I87" s="16" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="88" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B88" s="6" t="str">
         <f t="shared" si="15"/>
-        <v>130000</v>
+        <v>130008</v>
       </c>
       <c r="C88" s="13">
         <v>13</v>
@@ -3173,17 +3301,64 @@
       </c>
       <c r="E88" s="13"/>
       <c r="F88" s="14"/>
-      <c r="G88" s="13"/>
-      <c r="H88" s="14"/>
-    </row>
-    <row r="89" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="G88" s="13">
+        <v>8</v>
+      </c>
+      <c r="H88" s="15" t="s">
+        <v>169</v>
+      </c>
+      <c r="I88" s="16" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="89" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B89" s="6"/>
       <c r="C89" s="14"/>
       <c r="D89" s="14"/>
       <c r="E89" s="14"/>
       <c r="F89" s="14"/>
-      <c r="G89" s="14"/>
-      <c r="H89" s="14"/>
+      <c r="G89" s="16">
+        <v>9</v>
+      </c>
+      <c r="H89" s="15" t="s">
+        <v>172</v>
+      </c>
+      <c r="I89" s="16" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="90" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="G90" s="16">
+        <v>10</v>
+      </c>
+      <c r="H90" t="s">
+        <v>175</v>
+      </c>
+      <c r="I90" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="91" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="G91" s="16">
+        <v>11</v>
+      </c>
+      <c r="H91" t="s">
+        <v>174</v>
+      </c>
+      <c r="I91" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="92" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="G92" s="16">
+        <v>12</v>
+      </c>
+      <c r="H92" t="s">
+        <v>177</v>
+      </c>
+      <c r="I92" s="16" t="s">
+        <v>178</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
Complete Ch 13 Authoring queries
</commit_message>
<xml_diff>
--- a/Definitive Guide to DAX/DAX Functions Covered.xlsx
+++ b/Definitive Guide to DAX/DAX Functions Covered.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github.com\open-word\DAX\Definitive Guide to DAX\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCEBD6D8-812D-4311-A0AE-ECED968B2C24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75AF152C-6F09-4985-9E49-8250645EEEFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="0" windowWidth="17775" windowHeight="16200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="180">
   <si>
     <t>CALCULATE</t>
   </si>
@@ -573,6 +573,9 @@
   </si>
   <si>
     <t>SAMPLE</t>
+  </si>
+  <si>
+    <t>Understanding the auto-exists behavior in DAX queries</t>
   </si>
 </sst>
 </file>
@@ -697,7 +700,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -717,6 +720,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -997,10 +1002,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:K92"/>
+  <dimension ref="B1:K93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I93" sqref="I93"/>
+    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D101" sqref="D101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3029,6 +3034,9 @@
       <c r="H77" s="4" t="s">
         <v>146</v>
       </c>
+      <c r="I77" s="4"/>
+      <c r="J77" s="4"/>
+      <c r="K77" s="5"/>
     </row>
     <row r="78" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B78" s="6" t="str">
@@ -3056,6 +3064,8 @@
       <c r="I78" s="16" t="s">
         <v>150</v>
       </c>
+      <c r="J78" s="14"/>
+      <c r="K78" s="7"/>
     </row>
     <row r="79" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B79" s="6" t="str">
@@ -3083,6 +3093,8 @@
       <c r="I79" s="16" t="s">
         <v>153</v>
       </c>
+      <c r="J79" s="14"/>
+      <c r="K79" s="7"/>
     </row>
     <row r="80" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B80" s="6" t="str">
@@ -3110,8 +3122,10 @@
       <c r="I80" s="16" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="81" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J80" s="14"/>
+      <c r="K80" s="7"/>
+    </row>
+    <row r="81" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B81" s="6" t="str">
         <f t="shared" si="15"/>
         <v>130301</v>
@@ -3137,8 +3151,10 @@
       <c r="I81" s="16" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="82" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J81" s="14"/>
+      <c r="K81" s="7"/>
+    </row>
+    <row r="82" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B82" s="6" t="str">
         <f t="shared" si="15"/>
         <v>130302</v>
@@ -3164,8 +3180,10 @@
       <c r="I82" s="16" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="83" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J82" s="14"/>
+      <c r="K82" s="7"/>
+    </row>
+    <row r="83" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B83" s="6" t="str">
         <f t="shared" si="15"/>
         <v>130303</v>
@@ -3191,8 +3209,10 @@
       <c r="I83" s="16" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="84" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J83" s="14"/>
+      <c r="K83" s="7"/>
+    </row>
+    <row r="84" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B84" s="6" t="str">
         <f t="shared" si="15"/>
         <v>130304</v>
@@ -3218,11 +3238,13 @@
       <c r="I84" s="16" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="85" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J84" s="14"/>
+      <c r="K84" s="7"/>
+    </row>
+    <row r="85" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B85" s="6" t="str">
         <f t="shared" si="15"/>
-        <v>130005</v>
+        <v>130305</v>
       </c>
       <c r="C85" s="13">
         <v>13</v>
@@ -3230,8 +3252,12 @@
       <c r="D85" s="15" t="s">
         <v>145</v>
       </c>
-      <c r="E85" s="13"/>
-      <c r="F85" s="14"/>
+      <c r="E85" s="13">
+        <v>3</v>
+      </c>
+      <c r="F85" s="15" t="s">
+        <v>155</v>
+      </c>
       <c r="G85" s="13">
         <v>5</v>
       </c>
@@ -3241,11 +3267,13 @@
       <c r="I85" s="16" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="86" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J85" s="14"/>
+      <c r="K85" s="7"/>
+    </row>
+    <row r="86" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B86" s="6" t="str">
         <f t="shared" si="15"/>
-        <v>130006</v>
+        <v>130306</v>
       </c>
       <c r="C86" s="13">
         <v>13</v>
@@ -3253,8 +3281,12 @@
       <c r="D86" s="15" t="s">
         <v>145</v>
       </c>
-      <c r="E86" s="13"/>
-      <c r="F86" s="14"/>
+      <c r="E86" s="13">
+        <v>3</v>
+      </c>
+      <c r="F86" s="15" t="s">
+        <v>155</v>
+      </c>
       <c r="G86" s="13">
         <v>6</v>
       </c>
@@ -3264,11 +3296,13 @@
       <c r="I86" s="16" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="87" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J86" s="14"/>
+      <c r="K86" s="7"/>
+    </row>
+    <row r="87" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B87" s="6" t="str">
         <f t="shared" si="15"/>
-        <v>130007</v>
+        <v>130307</v>
       </c>
       <c r="C87" s="13">
         <v>13</v>
@@ -3276,8 +3310,12 @@
       <c r="D87" s="15" t="s">
         <v>145</v>
       </c>
-      <c r="E87" s="13"/>
-      <c r="F87" s="14"/>
+      <c r="E87" s="13">
+        <v>3</v>
+      </c>
+      <c r="F87" s="15" t="s">
+        <v>155</v>
+      </c>
       <c r="G87" s="13">
         <v>7</v>
       </c>
@@ -3287,11 +3325,13 @@
       <c r="I87" s="16" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="88" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J87" s="14"/>
+      <c r="K87" s="7"/>
+    </row>
+    <row r="88" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B88" s="6" t="str">
         <f t="shared" si="15"/>
-        <v>130008</v>
+        <v>130308</v>
       </c>
       <c r="C88" s="13">
         <v>13</v>
@@ -3299,8 +3339,12 @@
       <c r="D88" s="15" t="s">
         <v>145</v>
       </c>
-      <c r="E88" s="13"/>
-      <c r="F88" s="14"/>
+      <c r="E88" s="13">
+        <v>3</v>
+      </c>
+      <c r="F88" s="15" t="s">
+        <v>155</v>
+      </c>
       <c r="G88" s="13">
         <v>8</v>
       </c>
@@ -3310,13 +3354,26 @@
       <c r="I88" s="16" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="89" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B89" s="6"/>
-      <c r="C89" s="14"/>
-      <c r="D89" s="14"/>
-      <c r="E89" s="14"/>
-      <c r="F89" s="14"/>
+      <c r="J88" s="14"/>
+      <c r="K88" s="7"/>
+    </row>
+    <row r="89" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B89" s="6" t="str">
+        <f t="shared" ref="B89:B93" si="16">_xlfn.CONCAT(TEXT(C89,"00"),TEXT(E89,"00"),TEXT(G89,"00"))</f>
+        <v>130309</v>
+      </c>
+      <c r="C89" s="13">
+        <v>13</v>
+      </c>
+      <c r="D89" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="E89" s="13">
+        <v>3</v>
+      </c>
+      <c r="F89" s="15" t="s">
+        <v>155</v>
+      </c>
       <c r="G89" s="16">
         <v>9</v>
       </c>
@@ -3326,39 +3383,122 @@
       <c r="I89" s="16" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="90" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J89" s="14"/>
+      <c r="K89" s="7"/>
+    </row>
+    <row r="90" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B90" s="6" t="str">
+        <f t="shared" si="16"/>
+        <v>130310</v>
+      </c>
+      <c r="C90" s="13">
+        <v>13</v>
+      </c>
+      <c r="D90" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="E90" s="13">
+        <v>3</v>
+      </c>
+      <c r="F90" s="15" t="s">
+        <v>155</v>
+      </c>
       <c r="G90" s="16">
         <v>10</v>
       </c>
-      <c r="H90" t="s">
+      <c r="H90" s="14" t="s">
         <v>175</v>
       </c>
-      <c r="I90" t="s">
+      <c r="I90" s="14" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="91" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J90" s="14"/>
+      <c r="K90" s="7"/>
+    </row>
+    <row r="91" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B91" s="6" t="str">
+        <f t="shared" si="16"/>
+        <v>130311</v>
+      </c>
+      <c r="C91" s="13">
+        <v>13</v>
+      </c>
+      <c r="D91" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="E91" s="13">
+        <v>3</v>
+      </c>
+      <c r="F91" s="15" t="s">
+        <v>155</v>
+      </c>
       <c r="G91" s="16">
         <v>11</v>
       </c>
-      <c r="H91" t="s">
+      <c r="H91" s="14" t="s">
         <v>174</v>
       </c>
-      <c r="I91" t="s">
+      <c r="I91" s="14" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="92" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J91" s="14"/>
+      <c r="K91" s="7"/>
+    </row>
+    <row r="92" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B92" s="6" t="str">
+        <f t="shared" si="16"/>
+        <v>130312</v>
+      </c>
+      <c r="C92" s="13">
+        <v>13</v>
+      </c>
+      <c r="D92" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="E92" s="13">
+        <v>3</v>
+      </c>
+      <c r="F92" s="15" t="s">
+        <v>155</v>
+      </c>
       <c r="G92" s="16">
         <v>12</v>
       </c>
-      <c r="H92" t="s">
+      <c r="H92" s="14" t="s">
         <v>177</v>
       </c>
       <c r="I92" s="16" t="s">
         <v>178</v>
       </c>
+      <c r="J92" s="14"/>
+      <c r="K92" s="7"/>
+    </row>
+    <row r="93" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B93" s="8" t="str">
+        <f t="shared" si="16"/>
+        <v>130401</v>
+      </c>
+      <c r="C93" s="10">
+        <v>13</v>
+      </c>
+      <c r="D93" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="E93" s="17">
+        <v>4</v>
+      </c>
+      <c r="F93" s="18" t="s">
+        <v>179</v>
+      </c>
+      <c r="G93" s="17">
+        <v>1</v>
+      </c>
+      <c r="H93" s="18" t="s">
+        <v>179</v>
+      </c>
+      <c r="I93" s="10"/>
+      <c r="J93" s="10"/>
+      <c r="K93" s="11"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>